<commit_message>
atualiza planilha compras coronavirus
</commit_message>
<xml_diff>
--- a/data-raw/compras-coronavirus.xlsx
+++ b/data-raw/compras-coronavirus.xlsx
@@ -8,7 +8,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5799" uniqueCount="932">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5859" uniqueCount="937">
   <si>
     <t>Número Processo -  Formatado</t>
   </si>
@@ -2471,6 +2471,21 @@
   </si>
   <si>
     <t xml:space="preserve">ALFALAGOS LTDA </t>
+  </si>
+  <si>
+    <t>2121022 000037/2020</t>
+  </si>
+  <si>
+    <t>17.359.233/0001-88</t>
+  </si>
+  <si>
+    <t>TECIDOS E ARMARINHOS MIGUEL BARTOLOMEU S/A</t>
+  </si>
+  <si>
+    <t>18.625.083/0001-70</t>
+  </si>
+  <si>
+    <t>SUL MINAS INDUSTRIA E COMERCIO DE CONFECCOES LTDA</t>
   </si>
   <si>
     <t>2261032 000112/2020</t>
@@ -3002,7 +3017,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AF368"/>
+  <dimension ref="A1:AF372"/>
   <cols>
     <col min="1" max="1" width="27.8093" customWidth="1"/>
     <col min="2" max="2" width="23.8165" customWidth="1"/>
@@ -31967,25 +31982,25 @@
         <v>33</v>
       </c>
       <c r="C324" s="4">
-        <v>43920</v>
+        <v>44057</v>
       </c>
       <c r="D324" s="5" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
       <c r="E324" s="5" t="s">
         <v>33</v>
       </c>
       <c r="F324" s="6">
-        <v>2260</v>
+        <v>2120</v>
       </c>
       <c r="G324" s="3" t="s">
-        <v>822</v>
+        <v>784</v>
       </c>
       <c r="H324" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I324" s="3" t="s">
-        <v>37</v>
+        <v>806</v>
       </c>
       <c r="J324" s="7">
         <v>0</v>
@@ -31998,10 +32013,10 @@
       <c r="P324" s="9"/>
       <c r="Q324" s="8"/>
       <c r="R324" s="5" t="s">
-        <v>823</v>
+        <v>818</v>
       </c>
       <c r="S324" s="5" t="s">
-        <v>824</v>
+        <v>819</v>
       </c>
       <c r="T324" s="3" t="s">
         <v>33</v>
@@ -32010,37 +32025,37 @@
         <v>33</v>
       </c>
       <c r="V324" s="7">
-        <v>82414</v>
+        <v>1.672584e6</v>
       </c>
       <c r="W324" s="5" t="s">
-        <v>825</v>
+        <v>620</v>
       </c>
       <c r="X324" s="7">
-        <v>2261</v>
+        <v>2121</v>
       </c>
       <c r="Y324" s="5" t="s">
-        <v>822</v>
+        <v>786</v>
       </c>
       <c r="Z324" s="5" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="AA324" s="3" t="s">
-        <v>44</v>
+        <v>295</v>
       </c>
       <c r="AB324" s="10">
-        <v>10000</v>
+        <v>4</v>
       </c>
       <c r="AC324" s="11">
-        <v>676000e-6</v>
+        <v>36.99</v>
       </c>
       <c r="AD324" s="11">
-        <v>676000e-6</v>
+        <v>36.99</v>
       </c>
       <c r="AE324" s="12">
-        <v>6760</v>
+        <v>147.96</v>
       </c>
       <c r="AF324" s="12">
-        <v>6760</v>
+        <v>147.96</v>
       </c>
     </row>
     <row r="325" s="1" customFormat="1" ht="18.1322" customHeight="1">
@@ -32051,25 +32066,25 @@
         <v>33</v>
       </c>
       <c r="C325" s="14">
-        <v>43920</v>
+        <v>44057</v>
       </c>
       <c r="D325" s="15" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
       <c r="E325" s="15" t="s">
         <v>33</v>
       </c>
       <c r="F325" s="16">
-        <v>2260</v>
+        <v>2120</v>
       </c>
       <c r="G325" s="13" t="s">
-        <v>822</v>
+        <v>784</v>
       </c>
       <c r="H325" s="13" t="s">
         <v>36</v>
       </c>
       <c r="I325" s="13" t="s">
-        <v>37</v>
+        <v>806</v>
       </c>
       <c r="J325" s="17">
         <v>0</v>
@@ -32082,10 +32097,10 @@
       <c r="P325" s="19"/>
       <c r="Q325" s="18"/>
       <c r="R325" s="15" t="s">
-        <v>823</v>
+        <v>818</v>
       </c>
       <c r="S325" s="15" t="s">
-        <v>824</v>
+        <v>819</v>
       </c>
       <c r="T325" s="13" t="s">
         <v>33</v>
@@ -32094,37 +32109,37 @@
         <v>33</v>
       </c>
       <c r="V325" s="17">
-        <v>1.670891e6</v>
+        <v>1.672592e6</v>
       </c>
       <c r="W325" s="15" t="s">
-        <v>826</v>
+        <v>621</v>
       </c>
       <c r="X325" s="17">
-        <v>2261</v>
+        <v>2121</v>
       </c>
       <c r="Y325" s="15" t="s">
-        <v>822</v>
+        <v>786</v>
       </c>
       <c r="Z325" s="15" t="s">
-        <v>129</v>
+        <v>373</v>
       </c>
       <c r="AA325" s="13" t="s">
-        <v>44</v>
+        <v>295</v>
       </c>
       <c r="AB325" s="21">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="AC325" s="22">
-        <v>34.9</v>
+        <v>36.99</v>
       </c>
       <c r="AD325" s="22">
-        <v>34.9</v>
+        <v>36.99</v>
       </c>
       <c r="AE325" s="23">
-        <v>698</v>
+        <v>369.9</v>
       </c>
       <c r="AF325" s="23">
-        <v>698</v>
+        <v>369.9</v>
       </c>
     </row>
     <row r="326" s="1" customFormat="1" ht="18.1322" customHeight="1">
@@ -32135,25 +32150,25 @@
         <v>33</v>
       </c>
       <c r="C326" s="4">
-        <v>43920</v>
+        <v>44057</v>
       </c>
       <c r="D326" s="5" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
       <c r="E326" s="5" t="s">
         <v>33</v>
       </c>
       <c r="F326" s="6">
-        <v>2260</v>
+        <v>2120</v>
       </c>
       <c r="G326" s="3" t="s">
-        <v>822</v>
+        <v>784</v>
       </c>
       <c r="H326" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I326" s="3" t="s">
-        <v>37</v>
+        <v>806</v>
       </c>
       <c r="J326" s="7">
         <v>0</v>
@@ -32166,10 +32181,10 @@
       <c r="P326" s="9"/>
       <c r="Q326" s="8"/>
       <c r="R326" s="5" t="s">
-        <v>827</v>
+        <v>821</v>
       </c>
       <c r="S326" s="5" t="s">
-        <v>828</v>
+        <v>822</v>
       </c>
       <c r="T326" s="3" t="s">
         <v>33</v>
@@ -32178,37 +32193,37 @@
         <v>33</v>
       </c>
       <c r="V326" s="7">
-        <v>1.69773e6</v>
+        <v>125628</v>
       </c>
       <c r="W326" s="5" t="s">
-        <v>829</v>
+        <v>635</v>
       </c>
       <c r="X326" s="7">
-        <v>2261</v>
+        <v>2121</v>
       </c>
       <c r="Y326" s="5" t="s">
-        <v>822</v>
+        <v>786</v>
       </c>
       <c r="Z326" s="5" t="s">
-        <v>379</v>
+        <v>129</v>
       </c>
       <c r="AA326" s="3" t="s">
-        <v>44</v>
+        <v>295</v>
       </c>
       <c r="AB326" s="10">
-        <v>20000</v>
+        <v>200</v>
       </c>
       <c r="AC326" s="11">
-        <v>12.43</v>
+        <v>2.7</v>
       </c>
       <c r="AD326" s="11">
-        <v>12.43</v>
+        <v>2.7</v>
       </c>
       <c r="AE326" s="12">
-        <v>248600</v>
+        <v>540</v>
       </c>
       <c r="AF326" s="12">
-        <v>248600</v>
+        <v>540</v>
       </c>
     </row>
     <row r="327" s="1" customFormat="1" ht="18.1322" customHeight="1">
@@ -32219,25 +32234,25 @@
         <v>33</v>
       </c>
       <c r="C327" s="14">
-        <v>43920</v>
+        <v>44057</v>
       </c>
       <c r="D327" s="15" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
       <c r="E327" s="15" t="s">
         <v>33</v>
       </c>
       <c r="F327" s="16">
-        <v>2260</v>
+        <v>2120</v>
       </c>
       <c r="G327" s="13" t="s">
-        <v>822</v>
+        <v>784</v>
       </c>
       <c r="H327" s="13" t="s">
         <v>36</v>
       </c>
       <c r="I327" s="13" t="s">
-        <v>37</v>
+        <v>806</v>
       </c>
       <c r="J327" s="17">
         <v>0</v>
@@ -32250,10 +32265,10 @@
       <c r="P327" s="19"/>
       <c r="Q327" s="18"/>
       <c r="R327" s="15" t="s">
-        <v>712</v>
+        <v>823</v>
       </c>
       <c r="S327" s="15" t="s">
-        <v>713</v>
+        <v>824</v>
       </c>
       <c r="T327" s="13" t="s">
         <v>33</v>
@@ -32262,42 +32277,42 @@
         <v>33</v>
       </c>
       <c r="V327" s="17">
-        <v>394890</v>
+        <v>1.755366e6</v>
       </c>
       <c r="W327" s="15" t="s">
-        <v>830</v>
+        <v>724</v>
       </c>
       <c r="X327" s="17">
-        <v>2261</v>
+        <v>2121</v>
       </c>
       <c r="Y327" s="15" t="s">
-        <v>822</v>
+        <v>786</v>
       </c>
       <c r="Z327" s="15" t="s">
-        <v>379</v>
+        <v>272</v>
       </c>
       <c r="AA327" s="13" t="s">
-        <v>44</v>
+        <v>295</v>
       </c>
       <c r="AB327" s="21">
-        <v>450</v>
+        <v>2500</v>
       </c>
       <c r="AC327" s="22">
-        <v>7.98</v>
+        <v>8.31</v>
       </c>
       <c r="AD327" s="22">
-        <v>7.98</v>
+        <v>8.31</v>
       </c>
       <c r="AE327" s="23">
-        <v>3591</v>
+        <v>20775</v>
       </c>
       <c r="AF327" s="23">
-        <v>3591</v>
+        <v>20775</v>
       </c>
     </row>
     <row r="328" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A328" s="3" t="s">
-        <v>820</v>
+        <v>825</v>
       </c>
       <c r="B328" s="3" t="s">
         <v>33</v>
@@ -32306,7 +32321,7 @@
         <v>43920</v>
       </c>
       <c r="D328" s="5" t="s">
-        <v>821</v>
+        <v>826</v>
       </c>
       <c r="E328" s="5" t="s">
         <v>33</v>
@@ -32315,7 +32330,7 @@
         <v>2260</v>
       </c>
       <c r="G328" s="3" t="s">
-        <v>822</v>
+        <v>827</v>
       </c>
       <c r="H328" s="3" t="s">
         <v>36</v>
@@ -32334,10 +32349,10 @@
       <c r="P328" s="9"/>
       <c r="Q328" s="8"/>
       <c r="R328" s="5" t="s">
-        <v>712</v>
+        <v>828</v>
       </c>
       <c r="S328" s="5" t="s">
-        <v>713</v>
+        <v>829</v>
       </c>
       <c r="T328" s="3" t="s">
         <v>33</v>
@@ -32346,16 +32361,16 @@
         <v>33</v>
       </c>
       <c r="V328" s="7">
-        <v>1.368818e6</v>
+        <v>82414</v>
       </c>
       <c r="W328" s="5" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="X328" s="7">
         <v>2261</v>
       </c>
       <c r="Y328" s="5" t="s">
-        <v>822</v>
+        <v>827</v>
       </c>
       <c r="Z328" s="5" t="s">
         <v>379</v>
@@ -32364,24 +32379,24 @@
         <v>44</v>
       </c>
       <c r="AB328" s="10">
-        <v>10</v>
+        <v>10000</v>
       </c>
       <c r="AC328" s="11">
-        <v>293.6</v>
+        <v>676000e-6</v>
       </c>
       <c r="AD328" s="11">
-        <v>293.6</v>
+        <v>676000e-6</v>
       </c>
       <c r="AE328" s="12">
-        <v>2936</v>
+        <v>6760</v>
       </c>
       <c r="AF328" s="12">
-        <v>2936</v>
+        <v>6760</v>
       </c>
     </row>
     <row r="329" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A329" s="13" t="s">
-        <v>820</v>
+        <v>825</v>
       </c>
       <c r="B329" s="13" t="s">
         <v>33</v>
@@ -32390,7 +32405,7 @@
         <v>43920</v>
       </c>
       <c r="D329" s="15" t="s">
-        <v>821</v>
+        <v>826</v>
       </c>
       <c r="E329" s="15" t="s">
         <v>33</v>
@@ -32399,7 +32414,7 @@
         <v>2260</v>
       </c>
       <c r="G329" s="13" t="s">
-        <v>822</v>
+        <v>827</v>
       </c>
       <c r="H329" s="13" t="s">
         <v>36</v>
@@ -32418,10 +32433,10 @@
       <c r="P329" s="19"/>
       <c r="Q329" s="18"/>
       <c r="R329" s="15" t="s">
-        <v>712</v>
+        <v>828</v>
       </c>
       <c r="S329" s="15" t="s">
-        <v>713</v>
+        <v>829</v>
       </c>
       <c r="T329" s="13" t="s">
         <v>33</v>
@@ -32430,42 +32445,42 @@
         <v>33</v>
       </c>
       <c r="V329" s="17">
-        <v>1.497391e6</v>
+        <v>1.670891e6</v>
       </c>
       <c r="W329" s="15" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="X329" s="17">
         <v>2261</v>
       </c>
       <c r="Y329" s="15" t="s">
-        <v>822</v>
+        <v>827</v>
       </c>
       <c r="Z329" s="15" t="s">
-        <v>379</v>
+        <v>129</v>
       </c>
       <c r="AA329" s="13" t="s">
         <v>44</v>
       </c>
       <c r="AB329" s="21">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="AC329" s="22">
-        <v>3420</v>
+        <v>34.9</v>
       </c>
       <c r="AD329" s="22">
-        <v>3420</v>
+        <v>34.9</v>
       </c>
       <c r="AE329" s="23">
-        <v>51300</v>
+        <v>698</v>
       </c>
       <c r="AF329" s="23">
-        <v>51300</v>
+        <v>698</v>
       </c>
     </row>
     <row r="330" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A330" s="3" t="s">
-        <v>820</v>
+        <v>825</v>
       </c>
       <c r="B330" s="3" t="s">
         <v>33</v>
@@ -32474,7 +32489,7 @@
         <v>43920</v>
       </c>
       <c r="D330" s="5" t="s">
-        <v>821</v>
+        <v>826</v>
       </c>
       <c r="E330" s="5" t="s">
         <v>33</v>
@@ -32483,7 +32498,7 @@
         <v>2260</v>
       </c>
       <c r="G330" s="3" t="s">
-        <v>822</v>
+        <v>827</v>
       </c>
       <c r="H330" s="3" t="s">
         <v>36</v>
@@ -32502,28 +32517,28 @@
       <c r="P330" s="9"/>
       <c r="Q330" s="8"/>
       <c r="R330" s="5" t="s">
+        <v>832</v>
+      </c>
+      <c r="S330" s="5" t="s">
         <v>833</v>
       </c>
-      <c r="S330" s="5" t="s">
+      <c r="T330" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U330" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="V330" s="7">
+        <v>1.69773e6</v>
+      </c>
+      <c r="W330" s="5" t="s">
         <v>834</v>
-      </c>
-      <c r="T330" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="U330" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="V330" s="7">
-        <v>1.669613e6</v>
-      </c>
-      <c r="W330" s="5" t="s">
-        <v>835</v>
       </c>
       <c r="X330" s="7">
         <v>2261</v>
       </c>
       <c r="Y330" s="5" t="s">
-        <v>822</v>
+        <v>827</v>
       </c>
       <c r="Z330" s="5" t="s">
         <v>379</v>
@@ -32532,24 +32547,24 @@
         <v>44</v>
       </c>
       <c r="AB330" s="10">
-        <v>10</v>
+        <v>20000</v>
       </c>
       <c r="AC330" s="11">
-        <v>31.96</v>
+        <v>12.43</v>
       </c>
       <c r="AD330" s="11">
-        <v>31.96</v>
+        <v>12.43</v>
       </c>
       <c r="AE330" s="12">
-        <v>319.6</v>
+        <v>248600</v>
       </c>
       <c r="AF330" s="12">
-        <v>319.6</v>
+        <v>248600</v>
       </c>
     </row>
     <row r="331" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A331" s="13" t="s">
-        <v>820</v>
+        <v>825</v>
       </c>
       <c r="B331" s="13" t="s">
         <v>33</v>
@@ -32558,7 +32573,7 @@
         <v>43920</v>
       </c>
       <c r="D331" s="15" t="s">
-        <v>821</v>
+        <v>826</v>
       </c>
       <c r="E331" s="15" t="s">
         <v>33</v>
@@ -32567,7 +32582,7 @@
         <v>2260</v>
       </c>
       <c r="G331" s="13" t="s">
-        <v>822</v>
+        <v>827</v>
       </c>
       <c r="H331" s="13" t="s">
         <v>36</v>
@@ -32586,10 +32601,10 @@
       <c r="P331" s="19"/>
       <c r="Q331" s="18"/>
       <c r="R331" s="15" t="s">
-        <v>836</v>
+        <v>712</v>
       </c>
       <c r="S331" s="15" t="s">
-        <v>837</v>
+        <v>713</v>
       </c>
       <c r="T331" s="13" t="s">
         <v>33</v>
@@ -32598,16 +32613,16 @@
         <v>33</v>
       </c>
       <c r="V331" s="17">
-        <v>857025</v>
+        <v>394890</v>
       </c>
       <c r="W331" s="15" t="s">
-        <v>838</v>
+        <v>835</v>
       </c>
       <c r="X331" s="17">
         <v>2261</v>
       </c>
       <c r="Y331" s="15" t="s">
-        <v>822</v>
+        <v>827</v>
       </c>
       <c r="Z331" s="15" t="s">
         <v>379</v>
@@ -32616,24 +32631,24 @@
         <v>44</v>
       </c>
       <c r="AB331" s="21">
-        <v>100</v>
+        <v>450</v>
       </c>
       <c r="AC331" s="22">
-        <v>16.756</v>
+        <v>7.98</v>
       </c>
       <c r="AD331" s="22">
-        <v>16.756</v>
+        <v>7.98</v>
       </c>
       <c r="AE331" s="23">
-        <v>1675.6</v>
+        <v>3591</v>
       </c>
       <c r="AF331" s="23">
-        <v>1675.6</v>
+        <v>3591</v>
       </c>
     </row>
     <row r="332" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A332" s="3" t="s">
-        <v>820</v>
+        <v>825</v>
       </c>
       <c r="B332" s="3" t="s">
         <v>33</v>
@@ -32642,7 +32657,7 @@
         <v>43920</v>
       </c>
       <c r="D332" s="5" t="s">
-        <v>821</v>
+        <v>826</v>
       </c>
       <c r="E332" s="5" t="s">
         <v>33</v>
@@ -32651,7 +32666,7 @@
         <v>2260</v>
       </c>
       <c r="G332" s="3" t="s">
-        <v>822</v>
+        <v>827</v>
       </c>
       <c r="H332" s="3" t="s">
         <v>36</v>
@@ -32670,10 +32685,10 @@
       <c r="P332" s="9"/>
       <c r="Q332" s="8"/>
       <c r="R332" s="5" t="s">
-        <v>839</v>
+        <v>712</v>
       </c>
       <c r="S332" s="5" t="s">
-        <v>840</v>
+        <v>713</v>
       </c>
       <c r="T332" s="3" t="s">
         <v>33</v>
@@ -32682,16 +32697,16 @@
         <v>33</v>
       </c>
       <c r="V332" s="7">
-        <v>1.151746e6</v>
+        <v>1.368818e6</v>
       </c>
       <c r="W332" s="5" t="s">
-        <v>841</v>
+        <v>836</v>
       </c>
       <c r="X332" s="7">
         <v>2261</v>
       </c>
       <c r="Y332" s="5" t="s">
-        <v>822</v>
+        <v>827</v>
       </c>
       <c r="Z332" s="5" t="s">
         <v>379</v>
@@ -32700,24 +32715,24 @@
         <v>44</v>
       </c>
       <c r="AB332" s="10">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="AC332" s="11">
-        <v>117</v>
+        <v>293.6</v>
       </c>
       <c r="AD332" s="11">
-        <v>117</v>
+        <v>293.6</v>
       </c>
       <c r="AE332" s="12">
-        <v>2340</v>
+        <v>2936</v>
       </c>
       <c r="AF332" s="12">
-        <v>2340</v>
+        <v>2936</v>
       </c>
     </row>
     <row r="333" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A333" s="13" t="s">
-        <v>820</v>
+        <v>825</v>
       </c>
       <c r="B333" s="13" t="s">
         <v>33</v>
@@ -32726,7 +32741,7 @@
         <v>43920</v>
       </c>
       <c r="D333" s="15" t="s">
-        <v>821</v>
+        <v>826</v>
       </c>
       <c r="E333" s="15" t="s">
         <v>33</v>
@@ -32735,7 +32750,7 @@
         <v>2260</v>
       </c>
       <c r="G333" s="13" t="s">
-        <v>822</v>
+        <v>827</v>
       </c>
       <c r="H333" s="13" t="s">
         <v>36</v>
@@ -32744,32 +32759,20 @@
         <v>37</v>
       </c>
       <c r="J333" s="17">
-        <v>9.245762e6</v>
-      </c>
-      <c r="K333" s="15" t="s">
-        <v>842</v>
-      </c>
-      <c r="L333" s="17">
-        <v>2260</v>
-      </c>
-      <c r="M333" s="15" t="s">
-        <v>822</v>
-      </c>
-      <c r="N333" s="18">
-        <v>43936</v>
-      </c>
-      <c r="O333" s="18">
-        <v>43936</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K333" s="15"/>
+      <c r="L333" s="17"/>
+      <c r="M333" s="15"/>
+      <c r="N333" s="18"/>
+      <c r="O333" s="18"/>
       <c r="P333" s="19"/>
-      <c r="Q333" s="18">
-        <v>44115</v>
-      </c>
+      <c r="Q333" s="18"/>
       <c r="R333" s="15" t="s">
-        <v>843</v>
+        <v>712</v>
       </c>
       <c r="S333" s="15" t="s">
-        <v>844</v>
+        <v>713</v>
       </c>
       <c r="T333" s="13" t="s">
         <v>33</v>
@@ -32778,42 +32781,42 @@
         <v>33</v>
       </c>
       <c r="V333" s="17">
-        <v>781673</v>
+        <v>1.497391e6</v>
       </c>
       <c r="W333" s="15" t="s">
-        <v>845</v>
+        <v>837</v>
       </c>
       <c r="X333" s="17">
         <v>2261</v>
       </c>
       <c r="Y333" s="15" t="s">
-        <v>822</v>
+        <v>827</v>
       </c>
       <c r="Z333" s="15" t="s">
-        <v>122</v>
+        <v>379</v>
       </c>
       <c r="AA333" s="13" t="s">
         <v>44</v>
       </c>
       <c r="AB333" s="21">
-        <v>30000</v>
+        <v>15</v>
       </c>
       <c r="AC333" s="22">
-        <v>900000e-6</v>
+        <v>3420</v>
       </c>
       <c r="AD333" s="22">
-        <v>900000e-6</v>
+        <v>3420</v>
       </c>
       <c r="AE333" s="23">
-        <v>27000</v>
+        <v>51300</v>
       </c>
       <c r="AF333" s="23">
-        <v>27000</v>
+        <v>51300</v>
       </c>
     </row>
     <row r="334" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A334" s="3" t="s">
-        <v>820</v>
+        <v>825</v>
       </c>
       <c r="B334" s="3" t="s">
         <v>33</v>
@@ -32822,7 +32825,7 @@
         <v>43920</v>
       </c>
       <c r="D334" s="5" t="s">
-        <v>821</v>
+        <v>826</v>
       </c>
       <c r="E334" s="5" t="s">
         <v>33</v>
@@ -32831,7 +32834,7 @@
         <v>2260</v>
       </c>
       <c r="G334" s="3" t="s">
-        <v>822</v>
+        <v>827</v>
       </c>
       <c r="H334" s="3" t="s">
         <v>36</v>
@@ -32840,32 +32843,20 @@
         <v>37</v>
       </c>
       <c r="J334" s="7">
-        <v>9.245763e6</v>
-      </c>
-      <c r="K334" s="5" t="s">
-        <v>846</v>
-      </c>
-      <c r="L334" s="7">
-        <v>2260</v>
-      </c>
-      <c r="M334" s="5" t="s">
-        <v>822</v>
-      </c>
-      <c r="N334" s="8">
-        <v>43936</v>
-      </c>
-      <c r="O334" s="8">
-        <v>43936</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K334" s="5"/>
+      <c r="L334" s="7"/>
+      <c r="M334" s="5"/>
+      <c r="N334" s="8"/>
+      <c r="O334" s="8"/>
       <c r="P334" s="9"/>
-      <c r="Q334" s="8">
-        <v>44115</v>
-      </c>
+      <c r="Q334" s="8"/>
       <c r="R334" s="5" t="s">
-        <v>847</v>
+        <v>838</v>
       </c>
       <c r="S334" s="5" t="s">
-        <v>848</v>
+        <v>839</v>
       </c>
       <c r="T334" s="3" t="s">
         <v>33</v>
@@ -32874,42 +32865,42 @@
         <v>33</v>
       </c>
       <c r="V334" s="7">
-        <v>538957</v>
+        <v>1.669613e6</v>
       </c>
       <c r="W334" s="5" t="s">
-        <v>849</v>
+        <v>840</v>
       </c>
       <c r="X334" s="7">
         <v>2261</v>
       </c>
       <c r="Y334" s="5" t="s">
-        <v>822</v>
+        <v>827</v>
       </c>
       <c r="Z334" s="5" t="s">
-        <v>122</v>
+        <v>379</v>
       </c>
       <c r="AA334" s="3" t="s">
         <v>44</v>
       </c>
       <c r="AB334" s="10">
-        <v>30000</v>
+        <v>10</v>
       </c>
       <c r="AC334" s="11">
-        <v>550000e-6</v>
+        <v>31.96</v>
       </c>
       <c r="AD334" s="11">
-        <v>550000e-6</v>
+        <v>31.96</v>
       </c>
       <c r="AE334" s="12">
-        <v>16500</v>
+        <v>319.6</v>
       </c>
       <c r="AF334" s="12">
-        <v>16500</v>
+        <v>319.6</v>
       </c>
     </row>
     <row r="335" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A335" s="13" t="s">
-        <v>820</v>
+        <v>825</v>
       </c>
       <c r="B335" s="13" t="s">
         <v>33</v>
@@ -32918,7 +32909,7 @@
         <v>43920</v>
       </c>
       <c r="D335" s="15" t="s">
-        <v>821</v>
+        <v>826</v>
       </c>
       <c r="E335" s="15" t="s">
         <v>33</v>
@@ -32927,7 +32918,7 @@
         <v>2260</v>
       </c>
       <c r="G335" s="13" t="s">
-        <v>822</v>
+        <v>827</v>
       </c>
       <c r="H335" s="13" t="s">
         <v>36</v>
@@ -32936,32 +32927,20 @@
         <v>37</v>
       </c>
       <c r="J335" s="17">
-        <v>9.245763e6</v>
-      </c>
-      <c r="K335" s="15" t="s">
-        <v>846</v>
-      </c>
-      <c r="L335" s="17">
-        <v>2260</v>
-      </c>
-      <c r="M335" s="15" t="s">
-        <v>822</v>
-      </c>
-      <c r="N335" s="18">
-        <v>43936</v>
-      </c>
-      <c r="O335" s="18">
-        <v>43936</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K335" s="15"/>
+      <c r="L335" s="17"/>
+      <c r="M335" s="15"/>
+      <c r="N335" s="18"/>
+      <c r="O335" s="18"/>
       <c r="P335" s="19"/>
-      <c r="Q335" s="18">
-        <v>44115</v>
-      </c>
+      <c r="Q335" s="18"/>
       <c r="R335" s="15" t="s">
-        <v>847</v>
+        <v>841</v>
       </c>
       <c r="S335" s="15" t="s">
-        <v>848</v>
+        <v>842</v>
       </c>
       <c r="T335" s="13" t="s">
         <v>33</v>
@@ -32970,66 +32949,66 @@
         <v>33</v>
       </c>
       <c r="V335" s="17">
-        <v>1.651595e6</v>
+        <v>857025</v>
       </c>
       <c r="W335" s="15" t="s">
-        <v>850</v>
+        <v>843</v>
       </c>
       <c r="X335" s="17">
         <v>2261</v>
       </c>
       <c r="Y335" s="15" t="s">
-        <v>822</v>
+        <v>827</v>
       </c>
       <c r="Z335" s="15" t="s">
-        <v>122</v>
+        <v>379</v>
       </c>
       <c r="AA335" s="13" t="s">
         <v>44</v>
       </c>
       <c r="AB335" s="21">
-        <v>30000</v>
+        <v>100</v>
       </c>
       <c r="AC335" s="22">
-        <v>1.08</v>
+        <v>16.756</v>
       </c>
       <c r="AD335" s="22">
-        <v>1.08</v>
+        <v>16.756</v>
       </c>
       <c r="AE335" s="23">
-        <v>32400</v>
+        <v>1675.6</v>
       </c>
       <c r="AF335" s="23">
-        <v>32400</v>
+        <v>1675.6</v>
       </c>
     </row>
     <row r="336" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A336" s="3" t="s">
-        <v>851</v>
+        <v>825</v>
       </c>
       <c r="B336" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C336" s="4">
-        <v>43972</v>
+        <v>43920</v>
       </c>
       <c r="D336" s="5" t="s">
-        <v>852</v>
+        <v>826</v>
       </c>
       <c r="E336" s="5" t="s">
         <v>33</v>
       </c>
       <c r="F336" s="6">
-        <v>2280</v>
+        <v>2260</v>
       </c>
       <c r="G336" s="3" t="s">
-        <v>853</v>
+        <v>827</v>
       </c>
       <c r="H336" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I336" s="3" t="s">
-        <v>812</v>
+        <v>37</v>
       </c>
       <c r="J336" s="7">
         <v>0</v>
@@ -33042,10 +33021,10 @@
       <c r="P336" s="9"/>
       <c r="Q336" s="8"/>
       <c r="R336" s="5" t="s">
-        <v>813</v>
+        <v>844</v>
       </c>
       <c r="S336" s="5" t="s">
-        <v>814</v>
+        <v>845</v>
       </c>
       <c r="T336" s="3" t="s">
         <v>33</v>
@@ -33054,60 +33033,60 @@
         <v>33</v>
       </c>
       <c r="V336" s="7">
-        <v>1.756699e6</v>
+        <v>1.151746e6</v>
       </c>
       <c r="W336" s="5" t="s">
-        <v>815</v>
+        <v>846</v>
       </c>
       <c r="X336" s="7">
-        <v>2281</v>
+        <v>2261</v>
       </c>
       <c r="Y336" s="5" t="s">
-        <v>854</v>
+        <v>827</v>
       </c>
       <c r="Z336" s="5" t="s">
-        <v>373</v>
+        <v>379</v>
       </c>
       <c r="AA336" s="3" t="s">
-        <v>295</v>
+        <v>44</v>
       </c>
       <c r="AB336" s="10">
-        <v>127</v>
+        <v>20</v>
       </c>
       <c r="AC336" s="11">
-        <v>1.89</v>
+        <v>117</v>
       </c>
       <c r="AD336" s="11">
-        <v>1.89</v>
+        <v>117</v>
       </c>
       <c r="AE336" s="12">
-        <v>240.03</v>
+        <v>2340</v>
       </c>
       <c r="AF336" s="12">
-        <v>240.03</v>
+        <v>2340</v>
       </c>
     </row>
     <row r="337" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A337" s="13" t="s">
-        <v>855</v>
+        <v>825</v>
       </c>
       <c r="B337" s="13" t="s">
         <v>33</v>
       </c>
       <c r="C337" s="14">
-        <v>43921</v>
+        <v>43920</v>
       </c>
       <c r="D337" s="15" t="s">
-        <v>856</v>
+        <v>826</v>
       </c>
       <c r="E337" s="15" t="s">
         <v>33</v>
       </c>
       <c r="F337" s="16">
-        <v>2300</v>
+        <v>2260</v>
       </c>
       <c r="G337" s="13" t="s">
-        <v>857</v>
+        <v>827</v>
       </c>
       <c r="H337" s="13" t="s">
         <v>36</v>
@@ -33116,34 +33095,32 @@
         <v>37</v>
       </c>
       <c r="J337" s="17">
-        <v>9.245674e6</v>
+        <v>9.245762e6</v>
       </c>
       <c r="K337" s="15" t="s">
-        <v>858</v>
+        <v>847</v>
       </c>
       <c r="L337" s="17">
-        <v>2300</v>
+        <v>2260</v>
       </c>
       <c r="M337" s="15" t="s">
-        <v>857</v>
+        <v>827</v>
       </c>
       <c r="N337" s="18">
-        <v>43922</v>
+        <v>43936</v>
       </c>
       <c r="O337" s="18">
-        <v>43922</v>
-      </c>
-      <c r="P337" s="19">
-        <v>44105</v>
-      </c>
+        <v>43936</v>
+      </c>
+      <c r="P337" s="19"/>
       <c r="Q337" s="18">
-        <v>44131</v>
+        <v>44115</v>
       </c>
       <c r="R337" s="15" t="s">
-        <v>859</v>
+        <v>848</v>
       </c>
       <c r="S337" s="15" t="s">
-        <v>860</v>
+        <v>849</v>
       </c>
       <c r="T337" s="13" t="s">
         <v>33</v>
@@ -33152,60 +33129,60 @@
         <v>33</v>
       </c>
       <c r="V337" s="17">
-        <v>1155</v>
+        <v>781673</v>
       </c>
       <c r="W337" s="15" t="s">
-        <v>107</v>
+        <v>850</v>
       </c>
       <c r="X337" s="17">
-        <v>2301</v>
+        <v>2261</v>
       </c>
       <c r="Y337" s="15" t="s">
-        <v>861</v>
+        <v>827</v>
       </c>
       <c r="Z337" s="15" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="AA337" s="13" t="s">
         <v>44</v>
       </c>
       <c r="AB337" s="21">
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="AC337" s="22">
-        <v>4.35942886e6</v>
+        <v>900000e-6</v>
       </c>
       <c r="AD337" s="22">
-        <v>4.35942886e6</v>
+        <v>900000e-6</v>
       </c>
       <c r="AE337" s="23">
-        <v>4.35942886e6</v>
+        <v>27000</v>
       </c>
       <c r="AF337" s="23">
-        <v>4.35942886e6</v>
+        <v>27000</v>
       </c>
     </row>
     <row r="338" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A338" s="3" t="s">
-        <v>862</v>
+        <v>825</v>
       </c>
       <c r="B338" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C338" s="4">
-        <v>43935</v>
+        <v>43920</v>
       </c>
       <c r="D338" s="5" t="s">
-        <v>863</v>
+        <v>826</v>
       </c>
       <c r="E338" s="5" t="s">
         <v>33</v>
       </c>
       <c r="F338" s="6">
-        <v>2300</v>
+        <v>2260</v>
       </c>
       <c r="G338" s="3" t="s">
-        <v>857</v>
+        <v>827</v>
       </c>
       <c r="H338" s="3" t="s">
         <v>36</v>
@@ -33214,16 +33191,16 @@
         <v>37</v>
       </c>
       <c r="J338" s="7">
-        <v>9.24595e6</v>
+        <v>9.245763e6</v>
       </c>
       <c r="K338" s="5" t="s">
-        <v>864</v>
+        <v>851</v>
       </c>
       <c r="L338" s="7">
-        <v>2300</v>
+        <v>2260</v>
       </c>
       <c r="M338" s="5" t="s">
-        <v>857</v>
+        <v>827</v>
       </c>
       <c r="N338" s="8">
         <v>43936</v>
@@ -33231,17 +33208,15 @@
       <c r="O338" s="8">
         <v>43936</v>
       </c>
-      <c r="P338" s="9">
-        <v>44119</v>
-      </c>
+      <c r="P338" s="9"/>
       <c r="Q338" s="8">
-        <v>44119</v>
+        <v>44115</v>
       </c>
       <c r="R338" s="5" t="s">
-        <v>865</v>
+        <v>852</v>
       </c>
       <c r="S338" s="5" t="s">
-        <v>866</v>
+        <v>853</v>
       </c>
       <c r="T338" s="3" t="s">
         <v>33</v>
@@ -33250,60 +33225,60 @@
         <v>33</v>
       </c>
       <c r="V338" s="7">
-        <v>1155</v>
+        <v>538957</v>
       </c>
       <c r="W338" s="5" t="s">
-        <v>107</v>
+        <v>854</v>
       </c>
       <c r="X338" s="7">
-        <v>2301</v>
+        <v>2261</v>
       </c>
       <c r="Y338" s="5" t="s">
-        <v>861</v>
+        <v>827</v>
       </c>
       <c r="Z338" s="5" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="AA338" s="3" t="s">
         <v>44</v>
       </c>
       <c r="AB338" s="10">
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="AC338" s="11">
-        <v>1.04162557e6</v>
+        <v>550000e-6</v>
       </c>
       <c r="AD338" s="11">
-        <v>1.04162557e6</v>
+        <v>550000e-6</v>
       </c>
       <c r="AE338" s="12">
-        <v>1.04162557e6</v>
+        <v>16500</v>
       </c>
       <c r="AF338" s="12">
-        <v>1.04162557e6</v>
+        <v>16500</v>
       </c>
     </row>
     <row r="339" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A339" s="13" t="s">
-        <v>867</v>
+        <v>825</v>
       </c>
       <c r="B339" s="13" t="s">
         <v>33</v>
       </c>
       <c r="C339" s="14">
-        <v>43963</v>
+        <v>43920</v>
       </c>
       <c r="D339" s="15" t="s">
-        <v>868</v>
+        <v>826</v>
       </c>
       <c r="E339" s="15" t="s">
         <v>33</v>
       </c>
       <c r="F339" s="16">
-        <v>2300</v>
+        <v>2260</v>
       </c>
       <c r="G339" s="13" t="s">
-        <v>857</v>
+        <v>827</v>
       </c>
       <c r="H339" s="13" t="s">
         <v>36</v>
@@ -33312,34 +33287,32 @@
         <v>37</v>
       </c>
       <c r="J339" s="17">
-        <v>9.247198e6</v>
+        <v>9.245763e6</v>
       </c>
       <c r="K339" s="15" t="s">
-        <v>869</v>
+        <v>851</v>
       </c>
       <c r="L339" s="17">
-        <v>2300</v>
+        <v>2260</v>
       </c>
       <c r="M339" s="15" t="s">
-        <v>857</v>
+        <v>827</v>
       </c>
       <c r="N339" s="18">
-        <v>43963</v>
+        <v>43936</v>
       </c>
       <c r="O339" s="18">
-        <v>43963</v>
-      </c>
-      <c r="P339" s="19">
-        <v>44195</v>
-      </c>
+        <v>43936</v>
+      </c>
+      <c r="P339" s="19"/>
       <c r="Q339" s="18">
-        <v>44195</v>
+        <v>44115</v>
       </c>
       <c r="R339" s="15" t="s">
-        <v>870</v>
+        <v>852</v>
       </c>
       <c r="S339" s="15" t="s">
-        <v>871</v>
+        <v>853</v>
       </c>
       <c r="T339" s="13" t="s">
         <v>33</v>
@@ -33348,96 +33321,82 @@
         <v>33</v>
       </c>
       <c r="V339" s="17">
-        <v>1155</v>
+        <v>1.651595e6</v>
       </c>
       <c r="W339" s="15" t="s">
-        <v>107</v>
+        <v>855</v>
       </c>
       <c r="X339" s="17">
-        <v>2301</v>
+        <v>2261</v>
       </c>
       <c r="Y339" s="15" t="s">
-        <v>861</v>
+        <v>827</v>
       </c>
       <c r="Z339" s="15" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="AA339" s="13" t="s">
         <v>44</v>
       </c>
       <c r="AB339" s="21">
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="AC339" s="22">
-        <v>7.11634326e6</v>
+        <v>1.08</v>
       </c>
       <c r="AD339" s="22">
-        <v>7.11634326e6</v>
+        <v>1.08</v>
       </c>
       <c r="AE339" s="23">
-        <v>7.11634326e6</v>
+        <v>32400</v>
       </c>
       <c r="AF339" s="23">
-        <v>7.11634326e6</v>
+        <v>32400</v>
       </c>
     </row>
     <row r="340" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A340" s="3" t="s">
-        <v>872</v>
+        <v>856</v>
       </c>
       <c r="B340" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C340" s="4">
-        <v>43928</v>
+        <v>43972</v>
       </c>
       <c r="D340" s="5" t="s">
-        <v>873</v>
+        <v>857</v>
       </c>
       <c r="E340" s="5" t="s">
         <v>33</v>
       </c>
       <c r="F340" s="6">
-        <v>2310</v>
+        <v>2280</v>
       </c>
       <c r="G340" s="3" t="s">
-        <v>874</v>
+        <v>858</v>
       </c>
       <c r="H340" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I340" s="3" t="s">
-        <v>37</v>
+        <v>812</v>
       </c>
       <c r="J340" s="7">
-        <v>9.245982e6</v>
-      </c>
-      <c r="K340" s="5" t="s">
-        <v>875</v>
-      </c>
-      <c r="L340" s="7">
-        <v>2310</v>
-      </c>
-      <c r="M340" s="5" t="s">
-        <v>874</v>
-      </c>
-      <c r="N340" s="8">
-        <v>43943</v>
-      </c>
-      <c r="O340" s="8">
-        <v>43939</v>
-      </c>
-      <c r="P340" s="9">
-        <v>44304</v>
-      </c>
-      <c r="Q340" s="8">
-        <v>44121</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K340" s="5"/>
+      <c r="L340" s="7"/>
+      <c r="M340" s="5"/>
+      <c r="N340" s="8"/>
+      <c r="O340" s="8"/>
+      <c r="P340" s="9"/>
+      <c r="Q340" s="8"/>
       <c r="R340" s="5" t="s">
-        <v>750</v>
+        <v>813</v>
       </c>
       <c r="S340" s="5" t="s">
-        <v>751</v>
+        <v>814</v>
       </c>
       <c r="T340" s="3" t="s">
         <v>33</v>
@@ -33446,60 +33405,60 @@
         <v>33</v>
       </c>
       <c r="V340" s="7">
-        <v>18228</v>
-      </c>
-      <c r="W340" s="24" t="s">
-        <v>876</v>
+        <v>1.756699e6</v>
+      </c>
+      <c r="W340" s="5" t="s">
+        <v>815</v>
       </c>
       <c r="X340" s="7">
-        <v>2311</v>
+        <v>2281</v>
       </c>
       <c r="Y340" s="5" t="s">
-        <v>874</v>
+        <v>859</v>
       </c>
       <c r="Z340" s="5" t="s">
-        <v>365</v>
+        <v>373</v>
       </c>
       <c r="AA340" s="3" t="s">
-        <v>877</v>
+        <v>295</v>
       </c>
       <c r="AB340" s="10">
-        <v>200</v>
+        <v>127</v>
       </c>
       <c r="AC340" s="11">
-        <v>36</v>
+        <v>1.89</v>
       </c>
       <c r="AD340" s="11">
-        <v>36</v>
+        <v>1.89</v>
       </c>
       <c r="AE340" s="12">
-        <v>7200</v>
+        <v>240.03</v>
       </c>
       <c r="AF340" s="12">
-        <v>7200</v>
+        <v>240.03</v>
       </c>
     </row>
     <row r="341" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A341" s="13" t="s">
-        <v>872</v>
+        <v>860</v>
       </c>
       <c r="B341" s="13" t="s">
         <v>33</v>
       </c>
       <c r="C341" s="14">
-        <v>43928</v>
+        <v>43921</v>
       </c>
       <c r="D341" s="15" t="s">
-        <v>873</v>
+        <v>861</v>
       </c>
       <c r="E341" s="15" t="s">
         <v>33</v>
       </c>
       <c r="F341" s="16">
-        <v>2310</v>
+        <v>2300</v>
       </c>
       <c r="G341" s="13" t="s">
-        <v>874</v>
+        <v>862</v>
       </c>
       <c r="H341" s="13" t="s">
         <v>36</v>
@@ -33508,34 +33467,34 @@
         <v>37</v>
       </c>
       <c r="J341" s="17">
-        <v>9.245982e6</v>
+        <v>9.245674e6</v>
       </c>
       <c r="K341" s="15" t="s">
-        <v>875</v>
+        <v>863</v>
       </c>
       <c r="L341" s="17">
-        <v>2310</v>
+        <v>2300</v>
       </c>
       <c r="M341" s="15" t="s">
-        <v>874</v>
+        <v>862</v>
       </c>
       <c r="N341" s="18">
-        <v>43943</v>
+        <v>43922</v>
       </c>
       <c r="O341" s="18">
-        <v>43939</v>
+        <v>43922</v>
       </c>
       <c r="P341" s="19">
-        <v>44304</v>
+        <v>44105</v>
       </c>
       <c r="Q341" s="18">
-        <v>44121</v>
+        <v>44131</v>
       </c>
       <c r="R341" s="15" t="s">
-        <v>750</v>
+        <v>864</v>
       </c>
       <c r="S341" s="15" t="s">
-        <v>751</v>
+        <v>865</v>
       </c>
       <c r="T341" s="13" t="s">
         <v>33</v>
@@ -33544,60 +33503,60 @@
         <v>33</v>
       </c>
       <c r="V341" s="17">
-        <v>236268</v>
+        <v>1155</v>
       </c>
       <c r="W341" s="15" t="s">
-        <v>878</v>
+        <v>107</v>
       </c>
       <c r="X341" s="17">
-        <v>2311</v>
+        <v>2301</v>
       </c>
       <c r="Y341" s="15" t="s">
-        <v>874</v>
+        <v>866</v>
       </c>
       <c r="Z341" s="15" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="AA341" s="13" t="s">
-        <v>877</v>
+        <v>44</v>
       </c>
       <c r="AB341" s="21">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC341" s="22">
-        <v>45</v>
+        <v>4.35942886e6</v>
       </c>
       <c r="AD341" s="22">
-        <v>45</v>
+        <v>4.35942886e6</v>
       </c>
       <c r="AE341" s="23">
-        <v>2250</v>
+        <v>4.35942886e6</v>
       </c>
       <c r="AF341" s="23">
-        <v>2250</v>
+        <v>4.35942886e6</v>
       </c>
     </row>
     <row r="342" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A342" s="3" t="s">
-        <v>872</v>
+        <v>867</v>
       </c>
       <c r="B342" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C342" s="4">
-        <v>43928</v>
+        <v>43935</v>
       </c>
       <c r="D342" s="5" t="s">
-        <v>873</v>
+        <v>868</v>
       </c>
       <c r="E342" s="5" t="s">
         <v>33</v>
       </c>
       <c r="F342" s="6">
-        <v>2310</v>
+        <v>2300</v>
       </c>
       <c r="G342" s="3" t="s">
-        <v>874</v>
+        <v>862</v>
       </c>
       <c r="H342" s="3" t="s">
         <v>36</v>
@@ -33606,34 +33565,34 @@
         <v>37</v>
       </c>
       <c r="J342" s="7">
-        <v>9.245982e6</v>
+        <v>9.24595e6</v>
       </c>
       <c r="K342" s="5" t="s">
-        <v>875</v>
+        <v>869</v>
       </c>
       <c r="L342" s="7">
-        <v>2310</v>
+        <v>2300</v>
       </c>
       <c r="M342" s="5" t="s">
-        <v>874</v>
+        <v>862</v>
       </c>
       <c r="N342" s="8">
-        <v>43943</v>
+        <v>43936</v>
       </c>
       <c r="O342" s="8">
-        <v>43939</v>
+        <v>43936</v>
       </c>
       <c r="P342" s="9">
-        <v>44304</v>
+        <v>44119</v>
       </c>
       <c r="Q342" s="8">
-        <v>44121</v>
+        <v>44119</v>
       </c>
       <c r="R342" s="5" t="s">
-        <v>750</v>
+        <v>870</v>
       </c>
       <c r="S342" s="5" t="s">
-        <v>751</v>
+        <v>871</v>
       </c>
       <c r="T342" s="3" t="s">
         <v>33</v>
@@ -33642,37 +33601,37 @@
         <v>33</v>
       </c>
       <c r="V342" s="7">
-        <v>461920</v>
+        <v>1155</v>
       </c>
       <c r="W342" s="5" t="s">
-        <v>757</v>
+        <v>107</v>
       </c>
       <c r="X342" s="7">
-        <v>2311</v>
+        <v>2301</v>
       </c>
       <c r="Y342" s="5" t="s">
-        <v>874</v>
+        <v>866</v>
       </c>
       <c r="Z342" s="5" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="AA342" s="3" t="s">
-        <v>877</v>
+        <v>44</v>
       </c>
       <c r="AB342" s="10">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="AC342" s="11">
-        <v>8</v>
+        <v>1.04162557e6</v>
       </c>
       <c r="AD342" s="11">
-        <v>8</v>
+        <v>1.04162557e6</v>
       </c>
       <c r="AE342" s="12">
-        <v>4800</v>
+        <v>1.04162557e6</v>
       </c>
       <c r="AF342" s="12">
-        <v>4800</v>
+        <v>1.04162557e6</v>
       </c>
     </row>
     <row r="343" s="1" customFormat="1" ht="18.1322" customHeight="1">
@@ -33683,7 +33642,7 @@
         <v>33</v>
       </c>
       <c r="C343" s="14">
-        <v>43928</v>
+        <v>43963</v>
       </c>
       <c r="D343" s="15" t="s">
         <v>873</v>
@@ -33692,10 +33651,10 @@
         <v>33</v>
       </c>
       <c r="F343" s="16">
-        <v>2310</v>
+        <v>2300</v>
       </c>
       <c r="G343" s="13" t="s">
-        <v>874</v>
+        <v>862</v>
       </c>
       <c r="H343" s="13" t="s">
         <v>36</v>
@@ -33704,34 +33663,34 @@
         <v>37</v>
       </c>
       <c r="J343" s="17">
-        <v>9.245982e6</v>
+        <v>9.247198e6</v>
       </c>
       <c r="K343" s="15" t="s">
+        <v>874</v>
+      </c>
+      <c r="L343" s="17">
+        <v>2300</v>
+      </c>
+      <c r="M343" s="15" t="s">
+        <v>862</v>
+      </c>
+      <c r="N343" s="18">
+        <v>43963</v>
+      </c>
+      <c r="O343" s="18">
+        <v>43963</v>
+      </c>
+      <c r="P343" s="19">
+        <v>44195</v>
+      </c>
+      <c r="Q343" s="18">
+        <v>44195</v>
+      </c>
+      <c r="R343" s="15" t="s">
         <v>875</v>
       </c>
-      <c r="L343" s="17">
-        <v>2310</v>
-      </c>
-      <c r="M343" s="15" t="s">
-        <v>874</v>
-      </c>
-      <c r="N343" s="18">
-        <v>43943</v>
-      </c>
-      <c r="O343" s="18">
-        <v>43939</v>
-      </c>
-      <c r="P343" s="19">
-        <v>44304</v>
-      </c>
-      <c r="Q343" s="18">
-        <v>44121</v>
-      </c>
-      <c r="R343" s="15" t="s">
-        <v>750</v>
-      </c>
       <c r="S343" s="15" t="s">
-        <v>751</v>
+        <v>876</v>
       </c>
       <c r="T343" s="13" t="s">
         <v>33</v>
@@ -33740,42 +33699,42 @@
         <v>33</v>
       </c>
       <c r="V343" s="17">
-        <v>804495</v>
+        <v>1155</v>
       </c>
       <c r="W343" s="15" t="s">
-        <v>752</v>
+        <v>107</v>
       </c>
       <c r="X343" s="17">
-        <v>2311</v>
+        <v>2301</v>
       </c>
       <c r="Y343" s="15" t="s">
-        <v>874</v>
+        <v>866</v>
       </c>
       <c r="Z343" s="15" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="AA343" s="13" t="s">
-        <v>877</v>
+        <v>44</v>
       </c>
       <c r="AB343" s="21">
-        <v>170</v>
+        <v>0</v>
       </c>
       <c r="AC343" s="22">
-        <v>45</v>
+        <v>7.11634326e6</v>
       </c>
       <c r="AD343" s="22">
-        <v>45</v>
+        <v>7.11634326e6</v>
       </c>
       <c r="AE343" s="23">
-        <v>7650</v>
+        <v>7.11634326e6</v>
       </c>
       <c r="AF343" s="23">
-        <v>7650</v>
+        <v>7.11634326e6</v>
       </c>
     </row>
     <row r="344" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A344" s="3" t="s">
-        <v>872</v>
+        <v>877</v>
       </c>
       <c r="B344" s="3" t="s">
         <v>33</v>
@@ -33784,7 +33743,7 @@
         <v>43928</v>
       </c>
       <c r="D344" s="5" t="s">
-        <v>873</v>
+        <v>878</v>
       </c>
       <c r="E344" s="5" t="s">
         <v>33</v>
@@ -33793,7 +33752,7 @@
         <v>2310</v>
       </c>
       <c r="G344" s="3" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="H344" s="3" t="s">
         <v>36</v>
@@ -33805,13 +33764,13 @@
         <v>9.245982e6</v>
       </c>
       <c r="K344" s="5" t="s">
-        <v>875</v>
+        <v>880</v>
       </c>
       <c r="L344" s="7">
         <v>2310</v>
       </c>
       <c r="M344" s="5" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="N344" s="8">
         <v>43943</v>
@@ -33838,42 +33797,42 @@
         <v>33</v>
       </c>
       <c r="V344" s="7">
-        <v>1.129139e6</v>
-      </c>
-      <c r="W344" s="5" t="s">
-        <v>879</v>
+        <v>18228</v>
+      </c>
+      <c r="W344" s="24" t="s">
+        <v>881</v>
       </c>
       <c r="X344" s="7">
         <v>2311</v>
       </c>
       <c r="Y344" s="5" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="Z344" s="5" t="s">
-        <v>129</v>
+        <v>365</v>
       </c>
       <c r="AA344" s="3" t="s">
-        <v>877</v>
+        <v>882</v>
       </c>
       <c r="AB344" s="10">
-        <v>30</v>
+        <v>200</v>
       </c>
       <c r="AC344" s="11">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="AD344" s="11">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="AE344" s="12">
-        <v>1350</v>
+        <v>7200</v>
       </c>
       <c r="AF344" s="12">
-        <v>1350</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="345" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A345" s="13" t="s">
-        <v>872</v>
+        <v>877</v>
       </c>
       <c r="B345" s="13" t="s">
         <v>33</v>
@@ -33882,7 +33841,7 @@
         <v>43928</v>
       </c>
       <c r="D345" s="15" t="s">
-        <v>873</v>
+        <v>878</v>
       </c>
       <c r="E345" s="15" t="s">
         <v>33</v>
@@ -33891,7 +33850,7 @@
         <v>2310</v>
       </c>
       <c r="G345" s="13" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="H345" s="13" t="s">
         <v>36</v>
@@ -33903,13 +33862,13 @@
         <v>9.245982e6</v>
       </c>
       <c r="K345" s="15" t="s">
-        <v>875</v>
+        <v>880</v>
       </c>
       <c r="L345" s="17">
         <v>2310</v>
       </c>
       <c r="M345" s="15" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="N345" s="18">
         <v>43943</v>
@@ -33936,25 +33895,25 @@
         <v>33</v>
       </c>
       <c r="V345" s="17">
-        <v>1.152823e6</v>
+        <v>236268</v>
       </c>
       <c r="W345" s="15" t="s">
-        <v>880</v>
+        <v>883</v>
       </c>
       <c r="X345" s="17">
         <v>2311</v>
       </c>
       <c r="Y345" s="15" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="Z345" s="15" t="s">
         <v>129</v>
       </c>
       <c r="AA345" s="13" t="s">
-        <v>877</v>
+        <v>882</v>
       </c>
       <c r="AB345" s="21">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="AC345" s="22">
         <v>45</v>
@@ -33963,15 +33922,15 @@
         <v>45</v>
       </c>
       <c r="AE345" s="23">
-        <v>1350</v>
+        <v>2250</v>
       </c>
       <c r="AF345" s="23">
-        <v>1350</v>
+        <v>2250</v>
       </c>
     </row>
     <row r="346" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A346" s="3" t="s">
-        <v>872</v>
+        <v>877</v>
       </c>
       <c r="B346" s="3" t="s">
         <v>33</v>
@@ -33980,7 +33939,7 @@
         <v>43928</v>
       </c>
       <c r="D346" s="5" t="s">
-        <v>873</v>
+        <v>878</v>
       </c>
       <c r="E346" s="5" t="s">
         <v>33</v>
@@ -33989,7 +33948,7 @@
         <v>2310</v>
       </c>
       <c r="G346" s="3" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="H346" s="3" t="s">
         <v>36</v>
@@ -34001,13 +33960,13 @@
         <v>9.245982e6</v>
       </c>
       <c r="K346" s="5" t="s">
-        <v>875</v>
+        <v>880</v>
       </c>
       <c r="L346" s="7">
         <v>2310</v>
       </c>
       <c r="M346" s="5" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="N346" s="8">
         <v>43943</v>
@@ -34034,51 +33993,51 @@
         <v>33</v>
       </c>
       <c r="V346" s="7">
-        <v>1.152831e6</v>
+        <v>461920</v>
       </c>
       <c r="W346" s="5" t="s">
-        <v>881</v>
+        <v>757</v>
       </c>
       <c r="X346" s="7">
         <v>2311</v>
       </c>
       <c r="Y346" s="5" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="Z346" s="5" t="s">
         <v>129</v>
       </c>
       <c r="AA346" s="3" t="s">
-        <v>877</v>
+        <v>882</v>
       </c>
       <c r="AB346" s="10">
-        <v>30</v>
+        <v>600</v>
       </c>
       <c r="AC346" s="11">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="AD346" s="11">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="AE346" s="12">
-        <v>1350</v>
+        <v>4800</v>
       </c>
       <c r="AF346" s="12">
-        <v>1350</v>
+        <v>4800</v>
       </c>
     </row>
     <row r="347" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A347" s="13" t="s">
-        <v>882</v>
+        <v>877</v>
       </c>
       <c r="B347" s="13" t="s">
         <v>33</v>
       </c>
       <c r="C347" s="14">
-        <v>43955</v>
+        <v>43928</v>
       </c>
       <c r="D347" s="15" t="s">
-        <v>883</v>
+        <v>878</v>
       </c>
       <c r="E347" s="15" t="s">
         <v>33</v>
@@ -34087,7 +34046,7 @@
         <v>2310</v>
       </c>
       <c r="G347" s="13" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="H347" s="13" t="s">
         <v>36</v>
@@ -34096,34 +34055,34 @@
         <v>37</v>
       </c>
       <c r="J347" s="17">
-        <v>9.251383e6</v>
+        <v>9.245982e6</v>
       </c>
       <c r="K347" s="15" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
       <c r="L347" s="17">
         <v>2310</v>
       </c>
       <c r="M347" s="15" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="N347" s="18">
-        <v>44014</v>
+        <v>43943</v>
       </c>
       <c r="O347" s="18">
-        <v>44013</v>
+        <v>43939</v>
       </c>
       <c r="P347" s="19">
-        <v>44557</v>
+        <v>44304</v>
       </c>
       <c r="Q347" s="18">
-        <v>44192</v>
+        <v>44121</v>
       </c>
       <c r="R347" s="15" t="s">
-        <v>885</v>
+        <v>750</v>
       </c>
       <c r="S347" s="15" t="s">
-        <v>886</v>
+        <v>751</v>
       </c>
       <c r="T347" s="13" t="s">
         <v>33</v>
@@ -34132,51 +34091,51 @@
         <v>33</v>
       </c>
       <c r="V347" s="17">
-        <v>1.755897e6</v>
+        <v>804495</v>
       </c>
       <c r="W347" s="15" t="s">
-        <v>887</v>
+        <v>752</v>
       </c>
       <c r="X347" s="17">
         <v>2311</v>
       </c>
       <c r="Y347" s="15" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="Z347" s="15" t="s">
-        <v>301</v>
+        <v>129</v>
       </c>
       <c r="AA347" s="13" t="s">
-        <v>877</v>
+        <v>882</v>
       </c>
       <c r="AB347" s="21">
-        <v>300</v>
+        <v>170</v>
       </c>
       <c r="AC347" s="22">
-        <v>950000e-6</v>
+        <v>45</v>
       </c>
       <c r="AD347" s="22">
-        <v>950000e-6</v>
+        <v>45</v>
       </c>
       <c r="AE347" s="23">
-        <v>285</v>
+        <v>7650</v>
       </c>
       <c r="AF347" s="23">
-        <v>285</v>
+        <v>7650</v>
       </c>
     </row>
     <row r="348" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A348" s="3" t="s">
-        <v>888</v>
+        <v>877</v>
       </c>
       <c r="B348" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C348" s="4">
-        <v>43966</v>
+        <v>43928</v>
       </c>
       <c r="D348" s="5" t="s">
-        <v>889</v>
+        <v>878</v>
       </c>
       <c r="E348" s="5" t="s">
         <v>33</v>
@@ -34185,7 +34144,7 @@
         <v>2310</v>
       </c>
       <c r="G348" s="3" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="H348" s="3" t="s">
         <v>36</v>
@@ -34194,34 +34153,34 @@
         <v>37</v>
       </c>
       <c r="J348" s="7">
-        <v>9.253515e6</v>
+        <v>9.245982e6</v>
       </c>
       <c r="K348" s="5" t="s">
-        <v>890</v>
+        <v>880</v>
       </c>
       <c r="L348" s="7">
         <v>2310</v>
       </c>
       <c r="M348" s="5" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="N348" s="8">
-        <v>44027</v>
+        <v>43943</v>
       </c>
       <c r="O348" s="8">
-        <v>44027</v>
+        <v>43939</v>
       </c>
       <c r="P348" s="9">
-        <v>44757</v>
+        <v>44304</v>
       </c>
       <c r="Q348" s="8">
-        <v>44206</v>
+        <v>44121</v>
       </c>
       <c r="R348" s="5" t="s">
-        <v>457</v>
+        <v>750</v>
       </c>
       <c r="S348" s="5" t="s">
-        <v>458</v>
+        <v>751</v>
       </c>
       <c r="T348" s="3" t="s">
         <v>33</v>
@@ -34230,51 +34189,51 @@
         <v>33</v>
       </c>
       <c r="V348" s="7">
-        <v>1.722859e6</v>
+        <v>1.129139e6</v>
       </c>
       <c r="W348" s="5" t="s">
-        <v>891</v>
+        <v>884</v>
       </c>
       <c r="X348" s="7">
         <v>2311</v>
       </c>
       <c r="Y348" s="5" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="Z348" s="5" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="AA348" s="3" t="s">
-        <v>877</v>
+        <v>882</v>
       </c>
       <c r="AB348" s="10">
-        <v>50000</v>
+        <v>30</v>
       </c>
       <c r="AC348" s="11">
-        <v>2.68</v>
+        <v>45</v>
       </c>
       <c r="AD348" s="11">
-        <v>2.68</v>
+        <v>45</v>
       </c>
       <c r="AE348" s="12">
-        <v>134000</v>
+        <v>1350</v>
       </c>
       <c r="AF348" s="12">
-        <v>134000</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="349" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A349" s="13" t="s">
-        <v>888</v>
+        <v>877</v>
       </c>
       <c r="B349" s="13" t="s">
         <v>33</v>
       </c>
       <c r="C349" s="14">
-        <v>43966</v>
+        <v>43928</v>
       </c>
       <c r="D349" s="15" t="s">
-        <v>889</v>
+        <v>878</v>
       </c>
       <c r="E349" s="15" t="s">
         <v>33</v>
@@ -34283,7 +34242,7 @@
         <v>2310</v>
       </c>
       <c r="G349" s="13" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="H349" s="13" t="s">
         <v>36</v>
@@ -34292,34 +34251,34 @@
         <v>37</v>
       </c>
       <c r="J349" s="17">
-        <v>9.253515e6</v>
+        <v>9.245982e6</v>
       </c>
       <c r="K349" s="15" t="s">
-        <v>890</v>
+        <v>880</v>
       </c>
       <c r="L349" s="17">
         <v>2310</v>
       </c>
       <c r="M349" s="15" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="N349" s="18">
-        <v>44027</v>
+        <v>43943</v>
       </c>
       <c r="O349" s="18">
-        <v>44027</v>
+        <v>43939</v>
       </c>
       <c r="P349" s="19">
-        <v>44757</v>
+        <v>44304</v>
       </c>
       <c r="Q349" s="18">
-        <v>44206</v>
+        <v>44121</v>
       </c>
       <c r="R349" s="15" t="s">
-        <v>457</v>
+        <v>750</v>
       </c>
       <c r="S349" s="15" t="s">
-        <v>458</v>
+        <v>751</v>
       </c>
       <c r="T349" s="13" t="s">
         <v>33</v>
@@ -34328,51 +34287,51 @@
         <v>33</v>
       </c>
       <c r="V349" s="17">
-        <v>1.722891e6</v>
+        <v>1.152823e6</v>
       </c>
       <c r="W349" s="15" t="s">
-        <v>892</v>
+        <v>885</v>
       </c>
       <c r="X349" s="17">
         <v>2311</v>
       </c>
       <c r="Y349" s="15" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="Z349" s="15" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="AA349" s="13" t="s">
-        <v>877</v>
+        <v>882</v>
       </c>
       <c r="AB349" s="21">
-        <v>20000</v>
+        <v>30</v>
       </c>
       <c r="AC349" s="22">
-        <v>440000e-6</v>
+        <v>45</v>
       </c>
       <c r="AD349" s="22">
-        <v>440000e-6</v>
+        <v>45</v>
       </c>
       <c r="AE349" s="23">
-        <v>8800</v>
+        <v>1350</v>
       </c>
       <c r="AF349" s="23">
-        <v>8800</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="350" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A350" s="3" t="s">
-        <v>888</v>
+        <v>877</v>
       </c>
       <c r="B350" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C350" s="4">
-        <v>43966</v>
+        <v>43928</v>
       </c>
       <c r="D350" s="5" t="s">
-        <v>889</v>
+        <v>878</v>
       </c>
       <c r="E350" s="5" t="s">
         <v>33</v>
@@ -34381,7 +34340,7 @@
         <v>2310</v>
       </c>
       <c r="G350" s="3" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="H350" s="3" t="s">
         <v>36</v>
@@ -34390,34 +34349,34 @@
         <v>37</v>
       </c>
       <c r="J350" s="7">
-        <v>9.253532e6</v>
+        <v>9.245982e6</v>
       </c>
       <c r="K350" s="5" t="s">
-        <v>893</v>
+        <v>880</v>
       </c>
       <c r="L350" s="7">
         <v>2310</v>
       </c>
       <c r="M350" s="5" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="N350" s="8">
-        <v>44027</v>
+        <v>43943</v>
       </c>
       <c r="O350" s="8">
-        <v>44027</v>
+        <v>43939</v>
       </c>
       <c r="P350" s="9">
-        <v>44757</v>
+        <v>44304</v>
       </c>
       <c r="Q350" s="8">
-        <v>44206</v>
+        <v>44121</v>
       </c>
       <c r="R350" s="5" t="s">
-        <v>894</v>
+        <v>750</v>
       </c>
       <c r="S350" s="5" t="s">
-        <v>895</v>
+        <v>751</v>
       </c>
       <c r="T350" s="3" t="s">
         <v>33</v>
@@ -34426,51 +34385,51 @@
         <v>33</v>
       </c>
       <c r="V350" s="7">
-        <v>1.043684e6</v>
+        <v>1.152831e6</v>
       </c>
       <c r="W350" s="5" t="s">
-        <v>896</v>
+        <v>886</v>
       </c>
       <c r="X350" s="7">
         <v>2311</v>
       </c>
       <c r="Y350" s="5" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="Z350" s="5" t="s">
         <v>129</v>
       </c>
       <c r="AA350" s="3" t="s">
-        <v>877</v>
+        <v>882</v>
       </c>
       <c r="AB350" s="10">
-        <v>780</v>
+        <v>30</v>
       </c>
       <c r="AC350" s="11">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="AD350" s="11">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="AE350" s="12">
-        <v>19500</v>
+        <v>1350</v>
       </c>
       <c r="AF350" s="12">
-        <v>19500</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="351" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A351" s="13" t="s">
-        <v>897</v>
+        <v>887</v>
       </c>
       <c r="B351" s="13" t="s">
         <v>33</v>
       </c>
       <c r="C351" s="14">
-        <v>44001</v>
+        <v>43955</v>
       </c>
       <c r="D351" s="15" t="s">
-        <v>898</v>
+        <v>888</v>
       </c>
       <c r="E351" s="15" t="s">
         <v>33</v>
@@ -34479,7 +34438,7 @@
         <v>2310</v>
       </c>
       <c r="G351" s="13" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="H351" s="13" t="s">
         <v>36</v>
@@ -34488,34 +34447,34 @@
         <v>37</v>
       </c>
       <c r="J351" s="17">
-        <v>9.253504e6</v>
+        <v>9.251383e6</v>
       </c>
       <c r="K351" s="15" t="s">
-        <v>899</v>
+        <v>889</v>
       </c>
       <c r="L351" s="17">
         <v>2310</v>
       </c>
       <c r="M351" s="15" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="N351" s="18">
-        <v>44027</v>
+        <v>44014</v>
       </c>
       <c r="O351" s="18">
-        <v>44027</v>
+        <v>44013</v>
       </c>
       <c r="P351" s="19">
-        <v>44756</v>
+        <v>44557</v>
       </c>
       <c r="Q351" s="18">
-        <v>44206</v>
+        <v>44192</v>
       </c>
       <c r="R351" s="15" t="s">
-        <v>457</v>
+        <v>890</v>
       </c>
       <c r="S351" s="15" t="s">
-        <v>458</v>
+        <v>891</v>
       </c>
       <c r="T351" s="13" t="s">
         <v>33</v>
@@ -34524,60 +34483,60 @@
         <v>33</v>
       </c>
       <c r="V351" s="17">
-        <v>1.722905e6</v>
+        <v>1.755897e6</v>
       </c>
       <c r="W351" s="15" t="s">
-        <v>900</v>
+        <v>892</v>
       </c>
       <c r="X351" s="17">
         <v>2311</v>
       </c>
       <c r="Y351" s="15" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="Z351" s="15" t="s">
-        <v>122</v>
+        <v>301</v>
       </c>
       <c r="AA351" s="13" t="s">
-        <v>877</v>
+        <v>882</v>
       </c>
       <c r="AB351" s="21">
-        <v>30000</v>
+        <v>300</v>
       </c>
       <c r="AC351" s="22">
-        <v>1.16</v>
+        <v>950000e-6</v>
       </c>
       <c r="AD351" s="22">
-        <v>1.16</v>
+        <v>950000e-6</v>
       </c>
       <c r="AE351" s="23">
-        <v>34800</v>
+        <v>285</v>
       </c>
       <c r="AF351" s="23">
-        <v>34800</v>
+        <v>285</v>
       </c>
     </row>
     <row r="352" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A352" s="3" t="s">
-        <v>901</v>
+        <v>893</v>
       </c>
       <c r="B352" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C352" s="4">
-        <v>43944</v>
-      </c>
-      <c r="D352" s="26" t="s">
-        <v>902</v>
+        <v>43966</v>
+      </c>
+      <c r="D352" s="5" t="s">
+        <v>894</v>
       </c>
       <c r="E352" s="5" t="s">
         <v>33</v>
       </c>
       <c r="F352" s="6">
-        <v>2320</v>
+        <v>2310</v>
       </c>
       <c r="G352" s="3" t="s">
-        <v>903</v>
+        <v>879</v>
       </c>
       <c r="H352" s="3" t="s">
         <v>36</v>
@@ -34586,20 +34545,34 @@
         <v>37</v>
       </c>
       <c r="J352" s="7">
-        <v>0</v>
-      </c>
-      <c r="K352" s="5"/>
-      <c r="L352" s="7"/>
-      <c r="M352" s="5"/>
-      <c r="N352" s="8"/>
-      <c r="O352" s="8"/>
-      <c r="P352" s="9"/>
-      <c r="Q352" s="8"/>
+        <v>9.253515e6</v>
+      </c>
+      <c r="K352" s="5" t="s">
+        <v>895</v>
+      </c>
+      <c r="L352" s="7">
+        <v>2310</v>
+      </c>
+      <c r="M352" s="5" t="s">
+        <v>879</v>
+      </c>
+      <c r="N352" s="8">
+        <v>44027</v>
+      </c>
+      <c r="O352" s="8">
+        <v>44027</v>
+      </c>
+      <c r="P352" s="9">
+        <v>44757</v>
+      </c>
+      <c r="Q352" s="8">
+        <v>44206</v>
+      </c>
       <c r="R352" s="5" t="s">
-        <v>904</v>
+        <v>457</v>
       </c>
       <c r="S352" s="5" t="s">
-        <v>905</v>
+        <v>458</v>
       </c>
       <c r="T352" s="3" t="s">
         <v>33</v>
@@ -34608,60 +34581,60 @@
         <v>33</v>
       </c>
       <c r="V352" s="7">
-        <v>1.692143e6</v>
+        <v>1.722859e6</v>
       </c>
       <c r="W352" s="5" t="s">
-        <v>476</v>
+        <v>896</v>
       </c>
       <c r="X352" s="7">
-        <v>2321</v>
+        <v>2311</v>
       </c>
       <c r="Y352" s="5" t="s">
-        <v>906</v>
+        <v>879</v>
       </c>
       <c r="Z352" s="5" t="s">
-        <v>307</v>
+        <v>122</v>
       </c>
       <c r="AA352" s="3" t="s">
-        <v>474</v>
+        <v>882</v>
       </c>
       <c r="AB352" s="10">
-        <v>3000</v>
+        <v>50000</v>
       </c>
       <c r="AC352" s="11">
-        <v>8.2</v>
+        <v>2.68</v>
       </c>
       <c r="AD352" s="11">
-        <v>8.2</v>
+        <v>2.68</v>
       </c>
       <c r="AE352" s="12">
-        <v>24600</v>
+        <v>134000</v>
       </c>
       <c r="AF352" s="12">
-        <v>24600</v>
+        <v>134000</v>
       </c>
     </row>
     <row r="353" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A353" s="13" t="s">
-        <v>901</v>
+        <v>893</v>
       </c>
       <c r="B353" s="13" t="s">
         <v>33</v>
       </c>
       <c r="C353" s="14">
-        <v>43944</v>
-      </c>
-      <c r="D353" s="25" t="s">
-        <v>902</v>
+        <v>43966</v>
+      </c>
+      <c r="D353" s="15" t="s">
+        <v>894</v>
       </c>
       <c r="E353" s="15" t="s">
         <v>33</v>
       </c>
       <c r="F353" s="16">
-        <v>2320</v>
+        <v>2310</v>
       </c>
       <c r="G353" s="13" t="s">
-        <v>903</v>
+        <v>879</v>
       </c>
       <c r="H353" s="13" t="s">
         <v>36</v>
@@ -34670,20 +34643,34 @@
         <v>37</v>
       </c>
       <c r="J353" s="17">
-        <v>0</v>
-      </c>
-      <c r="K353" s="15"/>
-      <c r="L353" s="17"/>
-      <c r="M353" s="15"/>
-      <c r="N353" s="18"/>
-      <c r="O353" s="18"/>
-      <c r="P353" s="19"/>
-      <c r="Q353" s="18"/>
+        <v>9.253515e6</v>
+      </c>
+      <c r="K353" s="15" t="s">
+        <v>895</v>
+      </c>
+      <c r="L353" s="17">
+        <v>2310</v>
+      </c>
+      <c r="M353" s="15" t="s">
+        <v>879</v>
+      </c>
+      <c r="N353" s="18">
+        <v>44027</v>
+      </c>
+      <c r="O353" s="18">
+        <v>44027</v>
+      </c>
+      <c r="P353" s="19">
+        <v>44757</v>
+      </c>
+      <c r="Q353" s="18">
+        <v>44206</v>
+      </c>
       <c r="R353" s="15" t="s">
-        <v>907</v>
+        <v>457</v>
       </c>
       <c r="S353" s="15" t="s">
-        <v>908</v>
+        <v>458</v>
       </c>
       <c r="T353" s="13" t="s">
         <v>33</v>
@@ -34692,60 +34679,60 @@
         <v>33</v>
       </c>
       <c r="V353" s="17">
-        <v>1.143883e6</v>
+        <v>1.722891e6</v>
       </c>
       <c r="W353" s="15" t="s">
-        <v>909</v>
+        <v>897</v>
       </c>
       <c r="X353" s="17">
-        <v>2321</v>
+        <v>2311</v>
       </c>
       <c r="Y353" s="15" t="s">
-        <v>906</v>
+        <v>879</v>
       </c>
       <c r="Z353" s="15" t="s">
-        <v>497</v>
+        <v>122</v>
       </c>
       <c r="AA353" s="13" t="s">
-        <v>474</v>
+        <v>882</v>
       </c>
       <c r="AB353" s="21">
-        <v>200000</v>
+        <v>20000</v>
       </c>
       <c r="AC353" s="22">
-        <v>600000e-6</v>
+        <v>440000e-6</v>
       </c>
       <c r="AD353" s="22">
-        <v>600000e-6</v>
+        <v>440000e-6</v>
       </c>
       <c r="AE353" s="23">
-        <v>120000</v>
+        <v>8800</v>
       </c>
       <c r="AF353" s="23">
-        <v>120000</v>
+        <v>8800</v>
       </c>
     </row>
     <row r="354" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A354" s="3" t="s">
-        <v>901</v>
+        <v>893</v>
       </c>
       <c r="B354" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C354" s="4">
-        <v>43944</v>
-      </c>
-      <c r="D354" s="26" t="s">
-        <v>902</v>
+        <v>43966</v>
+      </c>
+      <c r="D354" s="5" t="s">
+        <v>894</v>
       </c>
       <c r="E354" s="5" t="s">
         <v>33</v>
       </c>
       <c r="F354" s="6">
-        <v>2320</v>
+        <v>2310</v>
       </c>
       <c r="G354" s="3" t="s">
-        <v>903</v>
+        <v>879</v>
       </c>
       <c r="H354" s="3" t="s">
         <v>36</v>
@@ -34754,20 +34741,34 @@
         <v>37</v>
       </c>
       <c r="J354" s="7">
-        <v>0</v>
-      </c>
-      <c r="K354" s="5"/>
-      <c r="L354" s="7"/>
-      <c r="M354" s="5"/>
-      <c r="N354" s="8"/>
-      <c r="O354" s="8"/>
-      <c r="P354" s="9"/>
-      <c r="Q354" s="8"/>
+        <v>9.253532e6</v>
+      </c>
+      <c r="K354" s="5" t="s">
+        <v>898</v>
+      </c>
+      <c r="L354" s="7">
+        <v>2310</v>
+      </c>
+      <c r="M354" s="5" t="s">
+        <v>879</v>
+      </c>
+      <c r="N354" s="8">
+        <v>44027</v>
+      </c>
+      <c r="O354" s="8">
+        <v>44027</v>
+      </c>
+      <c r="P354" s="9">
+        <v>44757</v>
+      </c>
+      <c r="Q354" s="8">
+        <v>44206</v>
+      </c>
       <c r="R354" s="5" t="s">
-        <v>910</v>
+        <v>899</v>
       </c>
       <c r="S354" s="5" t="s">
-        <v>911</v>
+        <v>900</v>
       </c>
       <c r="T354" s="3" t="s">
         <v>33</v>
@@ -34776,60 +34777,60 @@
         <v>33</v>
       </c>
       <c r="V354" s="7">
-        <v>1.244515e6</v>
+        <v>1.043684e6</v>
       </c>
       <c r="W354" s="5" t="s">
-        <v>912</v>
+        <v>901</v>
       </c>
       <c r="X354" s="7">
-        <v>2321</v>
+        <v>2311</v>
       </c>
       <c r="Y354" s="5" t="s">
-        <v>906</v>
+        <v>879</v>
       </c>
       <c r="Z354" s="5" t="s">
-        <v>497</v>
+        <v>129</v>
       </c>
       <c r="AA354" s="3" t="s">
-        <v>474</v>
+        <v>882</v>
       </c>
       <c r="AB354" s="10">
-        <v>50</v>
+        <v>780</v>
       </c>
       <c r="AC354" s="11">
-        <v>20.1</v>
+        <v>25</v>
       </c>
       <c r="AD354" s="11">
-        <v>20.1</v>
+        <v>25</v>
       </c>
       <c r="AE354" s="12">
-        <v>1005</v>
+        <v>19500</v>
       </c>
       <c r="AF354" s="12">
-        <v>1005</v>
+        <v>19500</v>
       </c>
     </row>
     <row r="355" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A355" s="13" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="B355" s="13" t="s">
         <v>33</v>
       </c>
       <c r="C355" s="14">
-        <v>43944</v>
-      </c>
-      <c r="D355" s="25" t="s">
-        <v>902</v>
+        <v>44001</v>
+      </c>
+      <c r="D355" s="15" t="s">
+        <v>903</v>
       </c>
       <c r="E355" s="15" t="s">
         <v>33</v>
       </c>
       <c r="F355" s="16">
-        <v>2320</v>
+        <v>2310</v>
       </c>
       <c r="G355" s="13" t="s">
-        <v>903</v>
+        <v>879</v>
       </c>
       <c r="H355" s="13" t="s">
         <v>36</v>
@@ -34838,20 +34839,34 @@
         <v>37</v>
       </c>
       <c r="J355" s="17">
-        <v>0</v>
-      </c>
-      <c r="K355" s="15"/>
-      <c r="L355" s="17"/>
-      <c r="M355" s="15"/>
-      <c r="N355" s="18"/>
-      <c r="O355" s="18"/>
-      <c r="P355" s="19"/>
-      <c r="Q355" s="18"/>
+        <v>9.253504e6</v>
+      </c>
+      <c r="K355" s="15" t="s">
+        <v>904</v>
+      </c>
+      <c r="L355" s="17">
+        <v>2310</v>
+      </c>
+      <c r="M355" s="15" t="s">
+        <v>879</v>
+      </c>
+      <c r="N355" s="18">
+        <v>44027</v>
+      </c>
+      <c r="O355" s="18">
+        <v>44027</v>
+      </c>
+      <c r="P355" s="19">
+        <v>44756</v>
+      </c>
+      <c r="Q355" s="18">
+        <v>44206</v>
+      </c>
       <c r="R355" s="15" t="s">
-        <v>913</v>
+        <v>457</v>
       </c>
       <c r="S355" s="15" t="s">
-        <v>914</v>
+        <v>458</v>
       </c>
       <c r="T355" s="13" t="s">
         <v>33</v>
@@ -34860,42 +34875,42 @@
         <v>33</v>
       </c>
       <c r="V355" s="17">
-        <v>1.244108e6</v>
+        <v>1.722905e6</v>
       </c>
       <c r="W355" s="15" t="s">
-        <v>915</v>
+        <v>905</v>
       </c>
       <c r="X355" s="17">
-        <v>2321</v>
+        <v>2311</v>
       </c>
       <c r="Y355" s="15" t="s">
-        <v>906</v>
+        <v>879</v>
       </c>
       <c r="Z355" s="15" t="s">
-        <v>497</v>
+        <v>122</v>
       </c>
       <c r="AA355" s="13" t="s">
-        <v>474</v>
+        <v>882</v>
       </c>
       <c r="AB355" s="21">
-        <v>90</v>
+        <v>30000</v>
       </c>
       <c r="AC355" s="22">
-        <v>358.24</v>
+        <v>1.16</v>
       </c>
       <c r="AD355" s="22">
-        <v>358.24</v>
+        <v>1.16</v>
       </c>
       <c r="AE355" s="23">
-        <v>32241.6</v>
+        <v>34800</v>
       </c>
       <c r="AF355" s="23">
-        <v>32241.6</v>
+        <v>34800</v>
       </c>
     </row>
     <row r="356" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A356" s="3" t="s">
-        <v>901</v>
+        <v>906</v>
       </c>
       <c r="B356" s="3" t="s">
         <v>33</v>
@@ -34904,7 +34919,7 @@
         <v>43944</v>
       </c>
       <c r="D356" s="26" t="s">
-        <v>902</v>
+        <v>907</v>
       </c>
       <c r="E356" s="5" t="s">
         <v>33</v>
@@ -34913,7 +34928,7 @@
         <v>2320</v>
       </c>
       <c r="G356" s="3" t="s">
-        <v>903</v>
+        <v>908</v>
       </c>
       <c r="H356" s="3" t="s">
         <v>36</v>
@@ -34932,10 +34947,10 @@
       <c r="P356" s="9"/>
       <c r="Q356" s="8"/>
       <c r="R356" s="5" t="s">
-        <v>913</v>
+        <v>909</v>
       </c>
       <c r="S356" s="5" t="s">
-        <v>914</v>
+        <v>910</v>
       </c>
       <c r="T356" s="3" t="s">
         <v>33</v>
@@ -34944,42 +34959,42 @@
         <v>33</v>
       </c>
       <c r="V356" s="7">
-        <v>1.244507e6</v>
+        <v>1.692143e6</v>
       </c>
       <c r="W356" s="5" t="s">
-        <v>916</v>
+        <v>476</v>
       </c>
       <c r="X356" s="7">
         <v>2321</v>
       </c>
       <c r="Y356" s="5" t="s">
-        <v>906</v>
+        <v>911</v>
       </c>
       <c r="Z356" s="5" t="s">
-        <v>497</v>
+        <v>307</v>
       </c>
       <c r="AA356" s="3" t="s">
         <v>474</v>
       </c>
       <c r="AB356" s="10">
-        <v>50</v>
+        <v>3000</v>
       </c>
       <c r="AC356" s="11">
-        <v>34.9</v>
+        <v>8.2</v>
       </c>
       <c r="AD356" s="11">
-        <v>34.9</v>
+        <v>8.2</v>
       </c>
       <c r="AE356" s="12">
-        <v>1745</v>
+        <v>24600</v>
       </c>
       <c r="AF356" s="12">
-        <v>1745</v>
+        <v>24600</v>
       </c>
     </row>
     <row r="357" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A357" s="13" t="s">
-        <v>901</v>
+        <v>906</v>
       </c>
       <c r="B357" s="13" t="s">
         <v>33</v>
@@ -34988,7 +35003,7 @@
         <v>43944</v>
       </c>
       <c r="D357" s="25" t="s">
-        <v>902</v>
+        <v>907</v>
       </c>
       <c r="E357" s="15" t="s">
         <v>33</v>
@@ -34997,7 +35012,7 @@
         <v>2320</v>
       </c>
       <c r="G357" s="13" t="s">
-        <v>903</v>
+        <v>908</v>
       </c>
       <c r="H357" s="13" t="s">
         <v>36</v>
@@ -35016,28 +35031,28 @@
       <c r="P357" s="19"/>
       <c r="Q357" s="18"/>
       <c r="R357" s="15" t="s">
+        <v>912</v>
+      </c>
+      <c r="S357" s="15" t="s">
         <v>913</v>
       </c>
-      <c r="S357" s="15" t="s">
+      <c r="T357" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="U357" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="V357" s="17">
+        <v>1.143883e6</v>
+      </c>
+      <c r="W357" s="15" t="s">
         <v>914</v>
-      </c>
-      <c r="T357" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="U357" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="V357" s="17">
-        <v>1.257587e6</v>
-      </c>
-      <c r="W357" s="15" t="s">
-        <v>917</v>
       </c>
       <c r="X357" s="17">
         <v>2321</v>
       </c>
       <c r="Y357" s="15" t="s">
-        <v>906</v>
+        <v>911</v>
       </c>
       <c r="Z357" s="15" t="s">
         <v>497</v>
@@ -35046,24 +35061,24 @@
         <v>474</v>
       </c>
       <c r="AB357" s="21">
-        <v>80000</v>
+        <v>200000</v>
       </c>
       <c r="AC357" s="22">
-        <v>390000e-6</v>
+        <v>600000e-6</v>
       </c>
       <c r="AD357" s="22">
-        <v>390000e-6</v>
+        <v>600000e-6</v>
       </c>
       <c r="AE357" s="23">
-        <v>31200</v>
+        <v>120000</v>
       </c>
       <c r="AF357" s="23">
-        <v>31200</v>
+        <v>120000</v>
       </c>
     </row>
     <row r="358" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A358" s="3" t="s">
-        <v>901</v>
+        <v>906</v>
       </c>
       <c r="B358" s="3" t="s">
         <v>33</v>
@@ -35072,7 +35087,7 @@
         <v>43944</v>
       </c>
       <c r="D358" s="26" t="s">
-        <v>902</v>
+        <v>907</v>
       </c>
       <c r="E358" s="5" t="s">
         <v>33</v>
@@ -35081,7 +35096,7 @@
         <v>2320</v>
       </c>
       <c r="G358" s="3" t="s">
-        <v>903</v>
+        <v>908</v>
       </c>
       <c r="H358" s="3" t="s">
         <v>36</v>
@@ -35100,10 +35115,10 @@
       <c r="P358" s="9"/>
       <c r="Q358" s="8"/>
       <c r="R358" s="5" t="s">
-        <v>913</v>
+        <v>915</v>
       </c>
       <c r="S358" s="5" t="s">
-        <v>914</v>
+        <v>916</v>
       </c>
       <c r="T358" s="3" t="s">
         <v>33</v>
@@ -35112,42 +35127,42 @@
         <v>33</v>
       </c>
       <c r="V358" s="7">
-        <v>1.257625e6</v>
+        <v>1.244515e6</v>
       </c>
       <c r="W358" s="5" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="X358" s="7">
         <v>2321</v>
       </c>
       <c r="Y358" s="5" t="s">
-        <v>906</v>
+        <v>911</v>
       </c>
       <c r="Z358" s="5" t="s">
-        <v>379</v>
+        <v>497</v>
       </c>
       <c r="AA358" s="3" t="s">
         <v>474</v>
       </c>
       <c r="AB358" s="10">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="AC358" s="11">
-        <v>351</v>
+        <v>20.1</v>
       </c>
       <c r="AD358" s="11">
-        <v>351</v>
+        <v>20.1</v>
       </c>
       <c r="AE358" s="12">
-        <v>31590</v>
+        <v>1005</v>
       </c>
       <c r="AF358" s="12">
-        <v>31590</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="359" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A359" s="13" t="s">
-        <v>901</v>
+        <v>906</v>
       </c>
       <c r="B359" s="13" t="s">
         <v>33</v>
@@ -35156,7 +35171,7 @@
         <v>43944</v>
       </c>
       <c r="D359" s="25" t="s">
-        <v>902</v>
+        <v>907</v>
       </c>
       <c r="E359" s="15" t="s">
         <v>33</v>
@@ -35165,7 +35180,7 @@
         <v>2320</v>
       </c>
       <c r="G359" s="13" t="s">
-        <v>903</v>
+        <v>908</v>
       </c>
       <c r="H359" s="13" t="s">
         <v>36</v>
@@ -35184,10 +35199,10 @@
       <c r="P359" s="19"/>
       <c r="Q359" s="18"/>
       <c r="R359" s="15" t="s">
-        <v>913</v>
+        <v>918</v>
       </c>
       <c r="S359" s="15" t="s">
-        <v>914</v>
+        <v>919</v>
       </c>
       <c r="T359" s="13" t="s">
         <v>33</v>
@@ -35196,16 +35211,16 @@
         <v>33</v>
       </c>
       <c r="V359" s="17">
-        <v>1.258699e6</v>
+        <v>1.244108e6</v>
       </c>
       <c r="W359" s="15" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="X359" s="17">
         <v>2321</v>
       </c>
       <c r="Y359" s="15" t="s">
-        <v>906</v>
+        <v>911</v>
       </c>
       <c r="Z359" s="15" t="s">
         <v>497</v>
@@ -35214,24 +35229,24 @@
         <v>474</v>
       </c>
       <c r="AB359" s="21">
-        <v>2000</v>
+        <v>90</v>
       </c>
       <c r="AC359" s="22">
-        <v>1.39</v>
+        <v>358.24</v>
       </c>
       <c r="AD359" s="22">
-        <v>1.39</v>
+        <v>358.24</v>
       </c>
       <c r="AE359" s="23">
-        <v>2780</v>
+        <v>32241.6</v>
       </c>
       <c r="AF359" s="23">
-        <v>2780</v>
+        <v>32241.6</v>
       </c>
     </row>
     <row r="360" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A360" s="3" t="s">
-        <v>901</v>
+        <v>906</v>
       </c>
       <c r="B360" s="3" t="s">
         <v>33</v>
@@ -35240,7 +35255,7 @@
         <v>43944</v>
       </c>
       <c r="D360" s="26" t="s">
-        <v>902</v>
+        <v>907</v>
       </c>
       <c r="E360" s="5" t="s">
         <v>33</v>
@@ -35249,7 +35264,7 @@
         <v>2320</v>
       </c>
       <c r="G360" s="3" t="s">
-        <v>903</v>
+        <v>908</v>
       </c>
       <c r="H360" s="3" t="s">
         <v>36</v>
@@ -35268,10 +35283,10 @@
       <c r="P360" s="9"/>
       <c r="Q360" s="8"/>
       <c r="R360" s="5" t="s">
-        <v>913</v>
+        <v>918</v>
       </c>
       <c r="S360" s="5" t="s">
-        <v>914</v>
+        <v>919</v>
       </c>
       <c r="T360" s="3" t="s">
         <v>33</v>
@@ -35280,16 +35295,16 @@
         <v>33</v>
       </c>
       <c r="V360" s="7">
-        <v>1.259784e6</v>
+        <v>1.244507e6</v>
       </c>
       <c r="W360" s="5" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="X360" s="7">
         <v>2321</v>
       </c>
       <c r="Y360" s="5" t="s">
-        <v>906</v>
+        <v>911</v>
       </c>
       <c r="Z360" s="5" t="s">
         <v>497</v>
@@ -35298,24 +35313,24 @@
         <v>474</v>
       </c>
       <c r="AB360" s="10">
-        <v>3000</v>
+        <v>50</v>
       </c>
       <c r="AC360" s="11">
-        <v>600000e-6</v>
+        <v>34.9</v>
       </c>
       <c r="AD360" s="11">
-        <v>600000e-6</v>
+        <v>34.9</v>
       </c>
       <c r="AE360" s="12">
-        <v>1800</v>
+        <v>1745</v>
       </c>
       <c r="AF360" s="12">
-        <v>1800</v>
+        <v>1745</v>
       </c>
     </row>
     <row r="361" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A361" s="13" t="s">
-        <v>901</v>
+        <v>906</v>
       </c>
       <c r="B361" s="13" t="s">
         <v>33</v>
@@ -35324,7 +35339,7 @@
         <v>43944</v>
       </c>
       <c r="D361" s="25" t="s">
-        <v>902</v>
+        <v>907</v>
       </c>
       <c r="E361" s="15" t="s">
         <v>33</v>
@@ -35333,7 +35348,7 @@
         <v>2320</v>
       </c>
       <c r="G361" s="13" t="s">
-        <v>903</v>
+        <v>908</v>
       </c>
       <c r="H361" s="13" t="s">
         <v>36</v>
@@ -35352,10 +35367,10 @@
       <c r="P361" s="19"/>
       <c r="Q361" s="18"/>
       <c r="R361" s="15" t="s">
-        <v>913</v>
+        <v>918</v>
       </c>
       <c r="S361" s="15" t="s">
-        <v>914</v>
+        <v>919</v>
       </c>
       <c r="T361" s="13" t="s">
         <v>33</v>
@@ -35364,16 +35379,16 @@
         <v>33</v>
       </c>
       <c r="V361" s="17">
-        <v>1.259792e6</v>
+        <v>1.257587e6</v>
       </c>
       <c r="W361" s="15" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="X361" s="17">
         <v>2321</v>
       </c>
       <c r="Y361" s="15" t="s">
-        <v>906</v>
+        <v>911</v>
       </c>
       <c r="Z361" s="15" t="s">
         <v>497</v>
@@ -35382,24 +35397,24 @@
         <v>474</v>
       </c>
       <c r="AB361" s="21">
-        <v>80</v>
+        <v>80000</v>
       </c>
       <c r="AC361" s="22">
-        <v>15.35</v>
+        <v>390000e-6</v>
       </c>
       <c r="AD361" s="22">
-        <v>15.35</v>
+        <v>390000e-6</v>
       </c>
       <c r="AE361" s="23">
-        <v>1228</v>
+        <v>31200</v>
       </c>
       <c r="AF361" s="23">
-        <v>1228</v>
+        <v>31200</v>
       </c>
     </row>
     <row r="362" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A362" s="3" t="s">
-        <v>901</v>
+        <v>906</v>
       </c>
       <c r="B362" s="3" t="s">
         <v>33</v>
@@ -35408,7 +35423,7 @@
         <v>43944</v>
       </c>
       <c r="D362" s="26" t="s">
-        <v>902</v>
+        <v>907</v>
       </c>
       <c r="E362" s="5" t="s">
         <v>33</v>
@@ -35417,7 +35432,7 @@
         <v>2320</v>
       </c>
       <c r="G362" s="3" t="s">
-        <v>903</v>
+        <v>908</v>
       </c>
       <c r="H362" s="3" t="s">
         <v>36</v>
@@ -35436,10 +35451,10 @@
       <c r="P362" s="9"/>
       <c r="Q362" s="8"/>
       <c r="R362" s="5" t="s">
-        <v>913</v>
+        <v>918</v>
       </c>
       <c r="S362" s="5" t="s">
-        <v>914</v>
+        <v>919</v>
       </c>
       <c r="T362" s="3" t="s">
         <v>33</v>
@@ -35448,42 +35463,42 @@
         <v>33</v>
       </c>
       <c r="V362" s="7">
-        <v>1.260669e6</v>
+        <v>1.257625e6</v>
       </c>
       <c r="W362" s="5" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="X362" s="7">
         <v>2321</v>
       </c>
       <c r="Y362" s="5" t="s">
-        <v>906</v>
+        <v>911</v>
       </c>
       <c r="Z362" s="5" t="s">
-        <v>497</v>
+        <v>379</v>
       </c>
       <c r="AA362" s="3" t="s">
         <v>474</v>
       </c>
       <c r="AB362" s="10">
-        <v>1000</v>
+        <v>90</v>
       </c>
       <c r="AC362" s="11">
-        <v>1.49</v>
+        <v>351</v>
       </c>
       <c r="AD362" s="11">
-        <v>1.49</v>
+        <v>351</v>
       </c>
       <c r="AE362" s="12">
-        <v>1490</v>
+        <v>31590</v>
       </c>
       <c r="AF362" s="12">
-        <v>1490</v>
+        <v>31590</v>
       </c>
     </row>
     <row r="363" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A363" s="13" t="s">
-        <v>901</v>
+        <v>906</v>
       </c>
       <c r="B363" s="13" t="s">
         <v>33</v>
@@ -35492,7 +35507,7 @@
         <v>43944</v>
       </c>
       <c r="D363" s="25" t="s">
-        <v>902</v>
+        <v>907</v>
       </c>
       <c r="E363" s="15" t="s">
         <v>33</v>
@@ -35501,7 +35516,7 @@
         <v>2320</v>
       </c>
       <c r="G363" s="13" t="s">
-        <v>903</v>
+        <v>908</v>
       </c>
       <c r="H363" s="13" t="s">
         <v>36</v>
@@ -35520,10 +35535,10 @@
       <c r="P363" s="19"/>
       <c r="Q363" s="18"/>
       <c r="R363" s="15" t="s">
-        <v>913</v>
+        <v>918</v>
       </c>
       <c r="S363" s="15" t="s">
-        <v>914</v>
+        <v>919</v>
       </c>
       <c r="T363" s="13" t="s">
         <v>33</v>
@@ -35532,16 +35547,16 @@
         <v>33</v>
       </c>
       <c r="V363" s="17">
-        <v>1.260677e6</v>
+        <v>1.258699e6</v>
       </c>
       <c r="W363" s="15" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="X363" s="17">
         <v>2321</v>
       </c>
       <c r="Y363" s="15" t="s">
-        <v>906</v>
+        <v>911</v>
       </c>
       <c r="Z363" s="15" t="s">
         <v>497</v>
@@ -35550,24 +35565,24 @@
         <v>474</v>
       </c>
       <c r="AB363" s="21">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="AC363" s="22">
-        <v>1.59</v>
+        <v>1.39</v>
       </c>
       <c r="AD363" s="22">
-        <v>1.59</v>
+        <v>1.39</v>
       </c>
       <c r="AE363" s="23">
-        <v>4770</v>
+        <v>2780</v>
       </c>
       <c r="AF363" s="23">
-        <v>4770</v>
+        <v>2780</v>
       </c>
     </row>
     <row r="364" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A364" s="3" t="s">
-        <v>901</v>
+        <v>906</v>
       </c>
       <c r="B364" s="3" t="s">
         <v>33</v>
@@ -35576,7 +35591,7 @@
         <v>43944</v>
       </c>
       <c r="D364" s="26" t="s">
-        <v>902</v>
+        <v>907</v>
       </c>
       <c r="E364" s="5" t="s">
         <v>33</v>
@@ -35585,7 +35600,7 @@
         <v>2320</v>
       </c>
       <c r="G364" s="3" t="s">
-        <v>903</v>
+        <v>908</v>
       </c>
       <c r="H364" s="3" t="s">
         <v>36</v>
@@ -35604,10 +35619,10 @@
       <c r="P364" s="9"/>
       <c r="Q364" s="8"/>
       <c r="R364" s="5" t="s">
-        <v>913</v>
+        <v>918</v>
       </c>
       <c r="S364" s="5" t="s">
-        <v>914</v>
+        <v>919</v>
       </c>
       <c r="T364" s="3" t="s">
         <v>33</v>
@@ -35616,16 +35631,16 @@
         <v>33</v>
       </c>
       <c r="V364" s="7">
-        <v>1.260731e6</v>
-      </c>
-      <c r="W364" s="24" t="s">
-        <v>924</v>
+        <v>1.259784e6</v>
+      </c>
+      <c r="W364" s="5" t="s">
+        <v>925</v>
       </c>
       <c r="X364" s="7">
         <v>2321</v>
       </c>
       <c r="Y364" s="5" t="s">
-        <v>906</v>
+        <v>911</v>
       </c>
       <c r="Z364" s="5" t="s">
         <v>497</v>
@@ -35634,24 +35649,24 @@
         <v>474</v>
       </c>
       <c r="AB364" s="10">
-        <v>60</v>
+        <v>3000</v>
       </c>
       <c r="AC364" s="11">
-        <v>271.97</v>
+        <v>600000e-6</v>
       </c>
       <c r="AD364" s="11">
-        <v>271.97</v>
+        <v>600000e-6</v>
       </c>
       <c r="AE364" s="12">
-        <v>16318.2</v>
+        <v>1800</v>
       </c>
       <c r="AF364" s="12">
-        <v>16318.2</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="365" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A365" s="13" t="s">
-        <v>901</v>
+        <v>906</v>
       </c>
       <c r="B365" s="13" t="s">
         <v>33</v>
@@ -35660,7 +35675,7 @@
         <v>43944</v>
       </c>
       <c r="D365" s="25" t="s">
-        <v>902</v>
+        <v>907</v>
       </c>
       <c r="E365" s="15" t="s">
         <v>33</v>
@@ -35669,7 +35684,7 @@
         <v>2320</v>
       </c>
       <c r="G365" s="13" t="s">
-        <v>903</v>
+        <v>908</v>
       </c>
       <c r="H365" s="13" t="s">
         <v>36</v>
@@ -35688,10 +35703,10 @@
       <c r="P365" s="19"/>
       <c r="Q365" s="18"/>
       <c r="R365" s="15" t="s">
-        <v>913</v>
+        <v>918</v>
       </c>
       <c r="S365" s="15" t="s">
-        <v>914</v>
+        <v>919</v>
       </c>
       <c r="T365" s="13" t="s">
         <v>33</v>
@@ -35700,16 +35715,16 @@
         <v>33</v>
       </c>
       <c r="V365" s="17">
-        <v>1.687115e6</v>
+        <v>1.259792e6</v>
       </c>
       <c r="W365" s="15" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="X365" s="17">
         <v>2321</v>
       </c>
       <c r="Y365" s="15" t="s">
-        <v>906</v>
+        <v>911</v>
       </c>
       <c r="Z365" s="15" t="s">
         <v>497</v>
@@ -35718,24 +35733,24 @@
         <v>474</v>
       </c>
       <c r="AB365" s="21">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="AC365" s="22">
-        <v>16.65</v>
+        <v>15.35</v>
       </c>
       <c r="AD365" s="22">
-        <v>16.65</v>
+        <v>15.35</v>
       </c>
       <c r="AE365" s="23">
-        <v>999</v>
+        <v>1228</v>
       </c>
       <c r="AF365" s="23">
-        <v>999</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="366" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A366" s="3" t="s">
-        <v>901</v>
+        <v>906</v>
       </c>
       <c r="B366" s="3" t="s">
         <v>33</v>
@@ -35744,7 +35759,7 @@
         <v>43944</v>
       </c>
       <c r="D366" s="26" t="s">
-        <v>902</v>
+        <v>907</v>
       </c>
       <c r="E366" s="5" t="s">
         <v>33</v>
@@ -35753,7 +35768,7 @@
         <v>2320</v>
       </c>
       <c r="G366" s="3" t="s">
-        <v>903</v>
+        <v>908</v>
       </c>
       <c r="H366" s="3" t="s">
         <v>36</v>
@@ -35772,28 +35787,28 @@
       <c r="P366" s="9"/>
       <c r="Q366" s="8"/>
       <c r="R366" s="5" t="s">
-        <v>926</v>
+        <v>918</v>
       </c>
       <c r="S366" s="5" t="s">
+        <v>919</v>
+      </c>
+      <c r="T366" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U366" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="V366" s="7">
+        <v>1.260669e6</v>
+      </c>
+      <c r="W366" s="5" t="s">
         <v>927</v>
-      </c>
-      <c r="T366" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="U366" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="V366" s="7">
-        <v>1.257463e6</v>
-      </c>
-      <c r="W366" s="5" t="s">
-        <v>928</v>
       </c>
       <c r="X366" s="7">
         <v>2321</v>
       </c>
       <c r="Y366" s="5" t="s">
-        <v>906</v>
+        <v>911</v>
       </c>
       <c r="Z366" s="5" t="s">
         <v>497</v>
@@ -35802,33 +35817,33 @@
         <v>474</v>
       </c>
       <c r="AB366" s="10">
-        <v>200</v>
+        <v>1000</v>
       </c>
       <c r="AC366" s="11">
-        <v>34.2</v>
+        <v>1.49</v>
       </c>
       <c r="AD366" s="11">
-        <v>34.2</v>
+        <v>1.49</v>
       </c>
       <c r="AE366" s="12">
-        <v>6840</v>
+        <v>1490</v>
       </c>
       <c r="AF366" s="12">
-        <v>6840</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="367" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A367" s="13" t="s">
-        <v>929</v>
+        <v>906</v>
       </c>
       <c r="B367" s="13" t="s">
         <v>33</v>
       </c>
       <c r="C367" s="14">
-        <v>44012</v>
-      </c>
-      <c r="D367" s="15" t="s">
-        <v>930</v>
+        <v>43944</v>
+      </c>
+      <c r="D367" s="25" t="s">
+        <v>907</v>
       </c>
       <c r="E367" s="15" t="s">
         <v>33</v>
@@ -35837,7 +35852,7 @@
         <v>2320</v>
       </c>
       <c r="G367" s="13" t="s">
-        <v>903</v>
+        <v>908</v>
       </c>
       <c r="H367" s="13" t="s">
         <v>36</v>
@@ -35856,10 +35871,10 @@
       <c r="P367" s="19"/>
       <c r="Q367" s="18"/>
       <c r="R367" s="15" t="s">
-        <v>457</v>
+        <v>918</v>
       </c>
       <c r="S367" s="15" t="s">
-        <v>458</v>
+        <v>919</v>
       </c>
       <c r="T367" s="13" t="s">
         <v>33</v>
@@ -35868,40 +35883,376 @@
         <v>33</v>
       </c>
       <c r="V367" s="17">
-        <v>1.408623e6</v>
+        <v>1.260677e6</v>
       </c>
       <c r="W367" s="15" t="s">
-        <v>931</v>
+        <v>928</v>
       </c>
       <c r="X367" s="17">
         <v>2321</v>
       </c>
       <c r="Y367" s="15" t="s">
-        <v>906</v>
+        <v>911</v>
       </c>
       <c r="Z367" s="15" t="s">
-        <v>373</v>
+        <v>497</v>
       </c>
       <c r="AA367" s="13" t="s">
         <v>474</v>
       </c>
       <c r="AB367" s="21">
+        <v>3000</v>
+      </c>
+      <c r="AC367" s="22">
+        <v>1.59</v>
+      </c>
+      <c r="AD367" s="22">
+        <v>1.59</v>
+      </c>
+      <c r="AE367" s="23">
+        <v>4770</v>
+      </c>
+      <c r="AF367" s="23">
+        <v>4770</v>
+      </c>
+    </row>
+    <row r="368" s="1" customFormat="1" ht="18.1322" customHeight="1">
+      <c r="A368" s="3" t="s">
+        <v>906</v>
+      </c>
+      <c r="B368" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C368" s="4">
+        <v>43944</v>
+      </c>
+      <c r="D368" s="26" t="s">
+        <v>907</v>
+      </c>
+      <c r="E368" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F368" s="6">
+        <v>2320</v>
+      </c>
+      <c r="G368" s="3" t="s">
+        <v>908</v>
+      </c>
+      <c r="H368" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I368" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J368" s="7">
+        <v>0</v>
+      </c>
+      <c r="K368" s="5"/>
+      <c r="L368" s="7"/>
+      <c r="M368" s="5"/>
+      <c r="N368" s="8"/>
+      <c r="O368" s="8"/>
+      <c r="P368" s="9"/>
+      <c r="Q368" s="8"/>
+      <c r="R368" s="5" t="s">
+        <v>918</v>
+      </c>
+      <c r="S368" s="5" t="s">
+        <v>919</v>
+      </c>
+      <c r="T368" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U368" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="V368" s="7">
+        <v>1.260731e6</v>
+      </c>
+      <c r="W368" s="24" t="s">
+        <v>929</v>
+      </c>
+      <c r="X368" s="7">
+        <v>2321</v>
+      </c>
+      <c r="Y368" s="5" t="s">
+        <v>911</v>
+      </c>
+      <c r="Z368" s="5" t="s">
+        <v>497</v>
+      </c>
+      <c r="AA368" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="AB368" s="10">
+        <v>60</v>
+      </c>
+      <c r="AC368" s="11">
+        <v>271.97</v>
+      </c>
+      <c r="AD368" s="11">
+        <v>271.97</v>
+      </c>
+      <c r="AE368" s="12">
+        <v>16318.2</v>
+      </c>
+      <c r="AF368" s="12">
+        <v>16318.2</v>
+      </c>
+    </row>
+    <row r="369" s="1" customFormat="1" ht="18.1322" customHeight="1">
+      <c r="A369" s="13" t="s">
+        <v>906</v>
+      </c>
+      <c r="B369" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C369" s="14">
+        <v>43944</v>
+      </c>
+      <c r="D369" s="25" t="s">
+        <v>907</v>
+      </c>
+      <c r="E369" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F369" s="16">
+        <v>2320</v>
+      </c>
+      <c r="G369" s="13" t="s">
+        <v>908</v>
+      </c>
+      <c r="H369" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I369" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="J369" s="17">
+        <v>0</v>
+      </c>
+      <c r="K369" s="15"/>
+      <c r="L369" s="17"/>
+      <c r="M369" s="15"/>
+      <c r="N369" s="18"/>
+      <c r="O369" s="18"/>
+      <c r="P369" s="19"/>
+      <c r="Q369" s="18"/>
+      <c r="R369" s="15" t="s">
+        <v>918</v>
+      </c>
+      <c r="S369" s="15" t="s">
+        <v>919</v>
+      </c>
+      <c r="T369" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="U369" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="V369" s="17">
+        <v>1.687115e6</v>
+      </c>
+      <c r="W369" s="15" t="s">
+        <v>930</v>
+      </c>
+      <c r="X369" s="17">
+        <v>2321</v>
+      </c>
+      <c r="Y369" s="15" t="s">
+        <v>911</v>
+      </c>
+      <c r="Z369" s="15" t="s">
+        <v>497</v>
+      </c>
+      <c r="AA369" s="13" t="s">
+        <v>474</v>
+      </c>
+      <c r="AB369" s="21">
+        <v>60</v>
+      </c>
+      <c r="AC369" s="22">
+        <v>16.65</v>
+      </c>
+      <c r="AD369" s="22">
+        <v>16.65</v>
+      </c>
+      <c r="AE369" s="23">
+        <v>999</v>
+      </c>
+      <c r="AF369" s="23">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="370" s="1" customFormat="1" ht="18.1322" customHeight="1">
+      <c r="A370" s="3" t="s">
+        <v>906</v>
+      </c>
+      <c r="B370" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C370" s="4">
+        <v>43944</v>
+      </c>
+      <c r="D370" s="26" t="s">
+        <v>907</v>
+      </c>
+      <c r="E370" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F370" s="6">
+        <v>2320</v>
+      </c>
+      <c r="G370" s="3" t="s">
+        <v>908</v>
+      </c>
+      <c r="H370" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I370" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J370" s="7">
+        <v>0</v>
+      </c>
+      <c r="K370" s="5"/>
+      <c r="L370" s="7"/>
+      <c r="M370" s="5"/>
+      <c r="N370" s="8"/>
+      <c r="O370" s="8"/>
+      <c r="P370" s="9"/>
+      <c r="Q370" s="8"/>
+      <c r="R370" s="5" t="s">
+        <v>931</v>
+      </c>
+      <c r="S370" s="5" t="s">
+        <v>932</v>
+      </c>
+      <c r="T370" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U370" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="V370" s="7">
+        <v>1.257463e6</v>
+      </c>
+      <c r="W370" s="5" t="s">
+        <v>933</v>
+      </c>
+      <c r="X370" s="7">
+        <v>2321</v>
+      </c>
+      <c r="Y370" s="5" t="s">
+        <v>911</v>
+      </c>
+      <c r="Z370" s="5" t="s">
+        <v>497</v>
+      </c>
+      <c r="AA370" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="AB370" s="10">
+        <v>200</v>
+      </c>
+      <c r="AC370" s="11">
+        <v>34.2</v>
+      </c>
+      <c r="AD370" s="11">
+        <v>34.2</v>
+      </c>
+      <c r="AE370" s="12">
+        <v>6840</v>
+      </c>
+      <c r="AF370" s="12">
+        <v>6840</v>
+      </c>
+    </row>
+    <row r="371" s="1" customFormat="1" ht="18.1322" customHeight="1">
+      <c r="A371" s="13" t="s">
+        <v>934</v>
+      </c>
+      <c r="B371" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C371" s="14">
+        <v>44012</v>
+      </c>
+      <c r="D371" s="15" t="s">
+        <v>935</v>
+      </c>
+      <c r="E371" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F371" s="16">
+        <v>2320</v>
+      </c>
+      <c r="G371" s="13" t="s">
+        <v>908</v>
+      </c>
+      <c r="H371" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I371" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="J371" s="17">
+        <v>0</v>
+      </c>
+      <c r="K371" s="15"/>
+      <c r="L371" s="17"/>
+      <c r="M371" s="15"/>
+      <c r="N371" s="18"/>
+      <c r="O371" s="18"/>
+      <c r="P371" s="19"/>
+      <c r="Q371" s="18"/>
+      <c r="R371" s="15" t="s">
+        <v>457</v>
+      </c>
+      <c r="S371" s="15" t="s">
+        <v>458</v>
+      </c>
+      <c r="T371" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="U371" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="V371" s="17">
+        <v>1.408623e6</v>
+      </c>
+      <c r="W371" s="15" t="s">
+        <v>936</v>
+      </c>
+      <c r="X371" s="17">
+        <v>2321</v>
+      </c>
+      <c r="Y371" s="15" t="s">
+        <v>911</v>
+      </c>
+      <c r="Z371" s="15" t="s">
+        <v>373</v>
+      </c>
+      <c r="AA371" s="13" t="s">
+        <v>474</v>
+      </c>
+      <c r="AB371" s="21">
         <v>2000</v>
       </c>
-      <c r="AC367" s="22">
+      <c r="AC371" s="22">
         <v>18.69</v>
       </c>
-      <c r="AD367" s="22">
+      <c r="AD371" s="22">
         <v>14.95</v>
       </c>
-      <c r="AE367" s="23">
+      <c r="AE371" s="23">
         <v>37380</v>
       </c>
-      <c r="AF367" s="23">
+      <c r="AF371" s="23">
         <v>29900</v>
       </c>
     </row>
-    <row r="368" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
+    <row r="372" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
   </sheetData>
   <pageSetup paperSize="9" scale="100" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>

<commit_message>
atualiza planilha de compras - processo IPSM
</commit_message>
<xml_diff>
--- a/data-raw/compras-coronavirus.xlsx
+++ b/data-raw/compras-coronavirus.xlsx
@@ -8,7 +8,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6073" uniqueCount="966">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6133" uniqueCount="972">
   <si>
     <t>Número Processo -  Formatado</t>
   </si>
@@ -2580,6 +2580,30 @@
     <t>MASCARA DE PROTECAO -  MODELO: FACIAL; MATERIA-PRIMA: ACETATO; FILTRO: NAO APLICAVEL; CLASSE DO FILTRO: NAO APLICAVEL; PROTECAO: VIAS AEREAS SUPERIORES; VALVULA: NAO APLICAVEL; VISOR: SEM VISOR; FIXACAO: AJUSTAVEL COM FIXACAO UNIVERSAL;</t>
   </si>
   <si>
+    <t>2121022 000044/2020</t>
+  </si>
+  <si>
+    <t>Aquisição de materiais de limpeza para a prevenção e combate ao COVID 19.</t>
+  </si>
+  <si>
+    <t>04.654.861/0001-44</t>
+  </si>
+  <si>
+    <t>INDALABOR INDAIA LABORATORIO FARMACEUTICO LTDA</t>
+  </si>
+  <si>
+    <t>18.285.097/0001-91</t>
+  </si>
+  <si>
+    <t>BRUMADINHO PAPEL E COMERCIO LTDA - ME</t>
+  </si>
+  <si>
+    <t>24.291.891/0001-40</t>
+  </si>
+  <si>
+    <t>DISTRIBUIR COMERCIO EIRELI - EPP</t>
+  </si>
+  <si>
     <t>2261032 000112/2020</t>
   </si>
   <si>
@@ -2849,12 +2873,6 @@
   </si>
   <si>
     <t>PANO PARA LIMPEZA - MATERIA-PRIMA: NAO TECIDO; COMPOSICAO (1): 100 POR CENTO VISCOSE; COMPONENTE (2): LATEX SINTETICO; FRAGRANCIA: SEM FRAGANCIA; DIMENSOES: 30 X 29 CM;</t>
-  </si>
-  <si>
-    <t>24.291.891/0001-40</t>
-  </si>
-  <si>
-    <t>DISTRIBUIR COMERCIO EIRELI - EPP</t>
   </si>
   <si>
     <t>RODO - BASE: INJETADA EM ABS, COM BORRACHA DUPLA; DIMENSAO BASE: 45 CM; CABO: DE ALUMINIO FRISADO, DE 1,40 M;</t>
@@ -3109,7 +3127,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AF386"/>
+  <dimension ref="A1:AF390"/>
   <cols>
     <col min="1" max="1" width="27.8093" customWidth="1"/>
     <col min="2" max="2" width="23.8165" customWidth="1"/>
@@ -33610,7 +33628,7 @@
         <v>33</v>
       </c>
       <c r="C342" s="4">
-        <v>43920</v>
+        <v>44070</v>
       </c>
       <c r="D342" s="5" t="s">
         <v>855</v>
@@ -33619,16 +33637,16 @@
         <v>33</v>
       </c>
       <c r="F342" s="6">
-        <v>2260</v>
+        <v>2120</v>
       </c>
       <c r="G342" s="3" t="s">
-        <v>856</v>
+        <v>814</v>
       </c>
       <c r="H342" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I342" s="3" t="s">
-        <v>37</v>
+        <v>441</v>
       </c>
       <c r="J342" s="7">
         <v>0</v>
@@ -33641,11 +33659,11 @@
       <c r="P342" s="9"/>
       <c r="Q342" s="8"/>
       <c r="R342" s="5" t="s">
+        <v>856</v>
+      </c>
+      <c r="S342" s="5" t="s">
         <v>857</v>
       </c>
-      <c r="S342" s="5" t="s">
-        <v>858</v>
-      </c>
       <c r="T342" s="3" t="s">
         <v>33</v>
       </c>
@@ -33653,37 +33671,37 @@
         <v>33</v>
       </c>
       <c r="V342" s="7">
-        <v>82414</v>
+        <v>1.692143e6</v>
       </c>
       <c r="W342" s="5" t="s">
-        <v>859</v>
+        <v>510</v>
       </c>
       <c r="X342" s="7">
-        <v>2261</v>
+        <v>2121</v>
       </c>
       <c r="Y342" s="5" t="s">
-        <v>856</v>
+        <v>816</v>
       </c>
       <c r="Z342" s="5" t="s">
-        <v>379</v>
+        <v>307</v>
       </c>
       <c r="AA342" s="3" t="s">
-        <v>44</v>
+        <v>295</v>
       </c>
       <c r="AB342" s="10">
-        <v>10000</v>
+        <v>10</v>
       </c>
       <c r="AC342" s="11">
-        <v>676000e-6</v>
+        <v>5.48</v>
       </c>
       <c r="AD342" s="11">
-        <v>676000e-6</v>
+        <v>5.48</v>
       </c>
       <c r="AE342" s="12">
-        <v>6760</v>
+        <v>54.8</v>
       </c>
       <c r="AF342" s="12">
-        <v>6760</v>
+        <v>54.8</v>
       </c>
     </row>
     <row r="343" s="1" customFormat="1" ht="18.1322" customHeight="1">
@@ -33694,7 +33712,7 @@
         <v>33</v>
       </c>
       <c r="C343" s="14">
-        <v>43920</v>
+        <v>44070</v>
       </c>
       <c r="D343" s="15" t="s">
         <v>855</v>
@@ -33703,16 +33721,16 @@
         <v>33</v>
       </c>
       <c r="F343" s="16">
-        <v>2260</v>
+        <v>2120</v>
       </c>
       <c r="G343" s="13" t="s">
-        <v>856</v>
+        <v>814</v>
       </c>
       <c r="H343" s="13" t="s">
         <v>36</v>
       </c>
       <c r="I343" s="13" t="s">
-        <v>37</v>
+        <v>441</v>
       </c>
       <c r="J343" s="17">
         <v>0</v>
@@ -33725,10 +33743,10 @@
       <c r="P343" s="19"/>
       <c r="Q343" s="18"/>
       <c r="R343" s="15" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="S343" s="15" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="T343" s="13" t="s">
         <v>33</v>
@@ -33737,37 +33755,37 @@
         <v>33</v>
       </c>
       <c r="V343" s="17">
-        <v>1.670891e6</v>
+        <v>50245</v>
       </c>
       <c r="W343" s="15" t="s">
-        <v>860</v>
+        <v>533</v>
       </c>
       <c r="X343" s="17">
-        <v>2261</v>
+        <v>2121</v>
       </c>
       <c r="Y343" s="15" t="s">
-        <v>856</v>
+        <v>816</v>
       </c>
       <c r="Z343" s="15" t="s">
-        <v>129</v>
+        <v>531</v>
       </c>
       <c r="AA343" s="13" t="s">
-        <v>44</v>
+        <v>295</v>
       </c>
       <c r="AB343" s="21">
-        <v>20</v>
+        <v>950</v>
       </c>
       <c r="AC343" s="22">
-        <v>34.9</v>
+        <v>1.75</v>
       </c>
       <c r="AD343" s="22">
-        <v>34.9</v>
+        <v>1.75</v>
       </c>
       <c r="AE343" s="23">
-        <v>698</v>
+        <v>1662.5</v>
       </c>
       <c r="AF343" s="23">
-        <v>698</v>
+        <v>1662.5</v>
       </c>
     </row>
     <row r="344" s="1" customFormat="1" ht="18.1322" customHeight="1">
@@ -33778,7 +33796,7 @@
         <v>33</v>
       </c>
       <c r="C344" s="4">
-        <v>43920</v>
+        <v>44070</v>
       </c>
       <c r="D344" s="5" t="s">
         <v>855</v>
@@ -33787,16 +33805,16 @@
         <v>33</v>
       </c>
       <c r="F344" s="6">
-        <v>2260</v>
+        <v>2120</v>
       </c>
       <c r="G344" s="3" t="s">
-        <v>856</v>
+        <v>814</v>
       </c>
       <c r="H344" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I344" s="3" t="s">
-        <v>37</v>
+        <v>441</v>
       </c>
       <c r="J344" s="7">
         <v>0</v>
@@ -33809,10 +33827,10 @@
       <c r="P344" s="9"/>
       <c r="Q344" s="8"/>
       <c r="R344" s="5" t="s">
-        <v>861</v>
+        <v>858</v>
       </c>
       <c r="S344" s="5" t="s">
-        <v>862</v>
+        <v>859</v>
       </c>
       <c r="T344" s="3" t="s">
         <v>33</v>
@@ -33821,37 +33839,37 @@
         <v>33</v>
       </c>
       <c r="V344" s="7">
-        <v>1.69773e6</v>
+        <v>367451</v>
       </c>
       <c r="W344" s="5" t="s">
-        <v>863</v>
+        <v>524</v>
       </c>
       <c r="X344" s="7">
-        <v>2261</v>
+        <v>2121</v>
       </c>
       <c r="Y344" s="5" t="s">
-        <v>856</v>
+        <v>816</v>
       </c>
       <c r="Z344" s="5" t="s">
         <v>379</v>
       </c>
       <c r="AA344" s="3" t="s">
-        <v>44</v>
+        <v>295</v>
       </c>
       <c r="AB344" s="10">
-        <v>20000</v>
+        <v>30</v>
       </c>
       <c r="AC344" s="11">
-        <v>12.43</v>
+        <v>8.5</v>
       </c>
       <c r="AD344" s="11">
-        <v>12.43</v>
+        <v>8.5</v>
       </c>
       <c r="AE344" s="12">
-        <v>248600</v>
+        <v>255</v>
       </c>
       <c r="AF344" s="12">
-        <v>248600</v>
+        <v>255</v>
       </c>
     </row>
     <row r="345" s="1" customFormat="1" ht="18.1322" customHeight="1">
@@ -33862,7 +33880,7 @@
         <v>33</v>
       </c>
       <c r="C345" s="14">
-        <v>43920</v>
+        <v>44070</v>
       </c>
       <c r="D345" s="15" t="s">
         <v>855</v>
@@ -33871,16 +33889,16 @@
         <v>33</v>
       </c>
       <c r="F345" s="16">
-        <v>2260</v>
+        <v>2120</v>
       </c>
       <c r="G345" s="13" t="s">
-        <v>856</v>
+        <v>814</v>
       </c>
       <c r="H345" s="13" t="s">
         <v>36</v>
       </c>
       <c r="I345" s="13" t="s">
-        <v>37</v>
+        <v>441</v>
       </c>
       <c r="J345" s="17">
         <v>0</v>
@@ -33893,10 +33911,10 @@
       <c r="P345" s="19"/>
       <c r="Q345" s="18"/>
       <c r="R345" s="15" t="s">
-        <v>744</v>
+        <v>860</v>
       </c>
       <c r="S345" s="15" t="s">
-        <v>745</v>
+        <v>861</v>
       </c>
       <c r="T345" s="13" t="s">
         <v>33</v>
@@ -33905,42 +33923,42 @@
         <v>33</v>
       </c>
       <c r="V345" s="17">
-        <v>394890</v>
+        <v>1.69216e6</v>
       </c>
       <c r="W345" s="15" t="s">
-        <v>864</v>
+        <v>511</v>
       </c>
       <c r="X345" s="17">
-        <v>2261</v>
+        <v>2121</v>
       </c>
       <c r="Y345" s="15" t="s">
-        <v>856</v>
+        <v>816</v>
       </c>
       <c r="Z345" s="15" t="s">
-        <v>379</v>
+        <v>307</v>
       </c>
       <c r="AA345" s="13" t="s">
-        <v>44</v>
+        <v>295</v>
       </c>
       <c r="AB345" s="21">
-        <v>450</v>
+        <v>150</v>
       </c>
       <c r="AC345" s="22">
-        <v>7.98</v>
+        <v>16.9</v>
       </c>
       <c r="AD345" s="22">
-        <v>7.98</v>
+        <v>16.9</v>
       </c>
       <c r="AE345" s="23">
-        <v>3591</v>
+        <v>2535</v>
       </c>
       <c r="AF345" s="23">
-        <v>3591</v>
+        <v>2535</v>
       </c>
     </row>
     <row r="346" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A346" s="3" t="s">
-        <v>854</v>
+        <v>862</v>
       </c>
       <c r="B346" s="3" t="s">
         <v>33</v>
@@ -33949,7 +33967,7 @@
         <v>43920</v>
       </c>
       <c r="D346" s="5" t="s">
-        <v>855</v>
+        <v>863</v>
       </c>
       <c r="E346" s="5" t="s">
         <v>33</v>
@@ -33958,7 +33976,7 @@
         <v>2260</v>
       </c>
       <c r="G346" s="3" t="s">
-        <v>856</v>
+        <v>864</v>
       </c>
       <c r="H346" s="3" t="s">
         <v>36</v>
@@ -33977,10 +33995,10 @@
       <c r="P346" s="9"/>
       <c r="Q346" s="8"/>
       <c r="R346" s="5" t="s">
-        <v>744</v>
+        <v>865</v>
       </c>
       <c r="S346" s="5" t="s">
-        <v>745</v>
+        <v>866</v>
       </c>
       <c r="T346" s="3" t="s">
         <v>33</v>
@@ -33989,16 +34007,16 @@
         <v>33</v>
       </c>
       <c r="V346" s="7">
-        <v>1.368818e6</v>
+        <v>82414</v>
       </c>
       <c r="W346" s="5" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
       <c r="X346" s="7">
         <v>2261</v>
       </c>
       <c r="Y346" s="5" t="s">
-        <v>856</v>
+        <v>864</v>
       </c>
       <c r="Z346" s="5" t="s">
         <v>379</v>
@@ -34007,24 +34025,24 @@
         <v>44</v>
       </c>
       <c r="AB346" s="10">
-        <v>10</v>
+        <v>10000</v>
       </c>
       <c r="AC346" s="11">
-        <v>293.6</v>
+        <v>676000e-6</v>
       </c>
       <c r="AD346" s="11">
-        <v>293.6</v>
+        <v>676000e-6</v>
       </c>
       <c r="AE346" s="12">
-        <v>2936</v>
+        <v>6760</v>
       </c>
       <c r="AF346" s="12">
-        <v>2936</v>
+        <v>6760</v>
       </c>
     </row>
     <row r="347" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A347" s="13" t="s">
-        <v>854</v>
+        <v>862</v>
       </c>
       <c r="B347" s="13" t="s">
         <v>33</v>
@@ -34033,7 +34051,7 @@
         <v>43920</v>
       </c>
       <c r="D347" s="15" t="s">
-        <v>855</v>
+        <v>863</v>
       </c>
       <c r="E347" s="15" t="s">
         <v>33</v>
@@ -34042,7 +34060,7 @@
         <v>2260</v>
       </c>
       <c r="G347" s="13" t="s">
-        <v>856</v>
+        <v>864</v>
       </c>
       <c r="H347" s="13" t="s">
         <v>36</v>
@@ -34061,10 +34079,10 @@
       <c r="P347" s="19"/>
       <c r="Q347" s="18"/>
       <c r="R347" s="15" t="s">
-        <v>744</v>
+        <v>865</v>
       </c>
       <c r="S347" s="15" t="s">
-        <v>745</v>
+        <v>866</v>
       </c>
       <c r="T347" s="13" t="s">
         <v>33</v>
@@ -34073,42 +34091,42 @@
         <v>33</v>
       </c>
       <c r="V347" s="17">
-        <v>1.497391e6</v>
+        <v>1.670891e6</v>
       </c>
       <c r="W347" s="15" t="s">
-        <v>866</v>
+        <v>868</v>
       </c>
       <c r="X347" s="17">
         <v>2261</v>
       </c>
       <c r="Y347" s="15" t="s">
-        <v>856</v>
+        <v>864</v>
       </c>
       <c r="Z347" s="15" t="s">
-        <v>379</v>
+        <v>129</v>
       </c>
       <c r="AA347" s="13" t="s">
         <v>44</v>
       </c>
       <c r="AB347" s="21">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="AC347" s="22">
-        <v>3420</v>
+        <v>34.9</v>
       </c>
       <c r="AD347" s="22">
-        <v>3420</v>
+        <v>34.9</v>
       </c>
       <c r="AE347" s="23">
-        <v>51300</v>
+        <v>698</v>
       </c>
       <c r="AF347" s="23">
-        <v>51300</v>
+        <v>698</v>
       </c>
     </row>
     <row r="348" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A348" s="3" t="s">
-        <v>854</v>
+        <v>862</v>
       </c>
       <c r="B348" s="3" t="s">
         <v>33</v>
@@ -34117,7 +34135,7 @@
         <v>43920</v>
       </c>
       <c r="D348" s="5" t="s">
-        <v>855</v>
+        <v>863</v>
       </c>
       <c r="E348" s="5" t="s">
         <v>33</v>
@@ -34126,7 +34144,7 @@
         <v>2260</v>
       </c>
       <c r="G348" s="3" t="s">
-        <v>856</v>
+        <v>864</v>
       </c>
       <c r="H348" s="3" t="s">
         <v>36</v>
@@ -34145,10 +34163,10 @@
       <c r="P348" s="9"/>
       <c r="Q348" s="8"/>
       <c r="R348" s="5" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="S348" s="5" t="s">
-        <v>868</v>
+        <v>870</v>
       </c>
       <c r="T348" s="3" t="s">
         <v>33</v>
@@ -34157,16 +34175,16 @@
         <v>33</v>
       </c>
       <c r="V348" s="7">
-        <v>1.669613e6</v>
+        <v>1.69773e6</v>
       </c>
       <c r="W348" s="5" t="s">
-        <v>869</v>
+        <v>871</v>
       </c>
       <c r="X348" s="7">
         <v>2261</v>
       </c>
       <c r="Y348" s="5" t="s">
-        <v>856</v>
+        <v>864</v>
       </c>
       <c r="Z348" s="5" t="s">
         <v>379</v>
@@ -34175,24 +34193,24 @@
         <v>44</v>
       </c>
       <c r="AB348" s="10">
-        <v>10</v>
+        <v>20000</v>
       </c>
       <c r="AC348" s="11">
-        <v>31.96</v>
+        <v>12.43</v>
       </c>
       <c r="AD348" s="11">
-        <v>31.96</v>
+        <v>12.43</v>
       </c>
       <c r="AE348" s="12">
-        <v>319.6</v>
+        <v>248600</v>
       </c>
       <c r="AF348" s="12">
-        <v>319.6</v>
+        <v>248600</v>
       </c>
     </row>
     <row r="349" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A349" s="13" t="s">
-        <v>854</v>
+        <v>862</v>
       </c>
       <c r="B349" s="13" t="s">
         <v>33</v>
@@ -34201,7 +34219,7 @@
         <v>43920</v>
       </c>
       <c r="D349" s="15" t="s">
-        <v>855</v>
+        <v>863</v>
       </c>
       <c r="E349" s="15" t="s">
         <v>33</v>
@@ -34210,7 +34228,7 @@
         <v>2260</v>
       </c>
       <c r="G349" s="13" t="s">
-        <v>856</v>
+        <v>864</v>
       </c>
       <c r="H349" s="13" t="s">
         <v>36</v>
@@ -34229,10 +34247,10 @@
       <c r="P349" s="19"/>
       <c r="Q349" s="18"/>
       <c r="R349" s="15" t="s">
-        <v>870</v>
+        <v>744</v>
       </c>
       <c r="S349" s="15" t="s">
-        <v>871</v>
+        <v>745</v>
       </c>
       <c r="T349" s="13" t="s">
         <v>33</v>
@@ -34241,7 +34259,7 @@
         <v>33</v>
       </c>
       <c r="V349" s="17">
-        <v>857025</v>
+        <v>394890</v>
       </c>
       <c r="W349" s="15" t="s">
         <v>872</v>
@@ -34250,7 +34268,7 @@
         <v>2261</v>
       </c>
       <c r="Y349" s="15" t="s">
-        <v>856</v>
+        <v>864</v>
       </c>
       <c r="Z349" s="15" t="s">
         <v>379</v>
@@ -34259,24 +34277,24 @@
         <v>44</v>
       </c>
       <c r="AB349" s="21">
-        <v>100</v>
+        <v>450</v>
       </c>
       <c r="AC349" s="22">
-        <v>16.756</v>
+        <v>7.98</v>
       </c>
       <c r="AD349" s="22">
-        <v>16.756</v>
+        <v>7.98</v>
       </c>
       <c r="AE349" s="23">
-        <v>1675.6</v>
+        <v>3591</v>
       </c>
       <c r="AF349" s="23">
-        <v>1675.6</v>
+        <v>3591</v>
       </c>
     </row>
     <row r="350" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A350" s="3" t="s">
-        <v>854</v>
+        <v>862</v>
       </c>
       <c r="B350" s="3" t="s">
         <v>33</v>
@@ -34285,7 +34303,7 @@
         <v>43920</v>
       </c>
       <c r="D350" s="5" t="s">
-        <v>855</v>
+        <v>863</v>
       </c>
       <c r="E350" s="5" t="s">
         <v>33</v>
@@ -34294,7 +34312,7 @@
         <v>2260</v>
       </c>
       <c r="G350" s="3" t="s">
-        <v>856</v>
+        <v>864</v>
       </c>
       <c r="H350" s="3" t="s">
         <v>36</v>
@@ -34313,28 +34331,28 @@
       <c r="P350" s="9"/>
       <c r="Q350" s="8"/>
       <c r="R350" s="5" t="s">
+        <v>744</v>
+      </c>
+      <c r="S350" s="5" t="s">
+        <v>745</v>
+      </c>
+      <c r="T350" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U350" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="V350" s="7">
+        <v>1.368818e6</v>
+      </c>
+      <c r="W350" s="5" t="s">
         <v>873</v>
-      </c>
-      <c r="S350" s="5" t="s">
-        <v>874</v>
-      </c>
-      <c r="T350" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="U350" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="V350" s="7">
-        <v>1.151746e6</v>
-      </c>
-      <c r="W350" s="5" t="s">
-        <v>875</v>
       </c>
       <c r="X350" s="7">
         <v>2261</v>
       </c>
       <c r="Y350" s="5" t="s">
-        <v>856</v>
+        <v>864</v>
       </c>
       <c r="Z350" s="5" t="s">
         <v>379</v>
@@ -34343,24 +34361,24 @@
         <v>44</v>
       </c>
       <c r="AB350" s="10">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="AC350" s="11">
-        <v>117</v>
+        <v>293.6</v>
       </c>
       <c r="AD350" s="11">
-        <v>117</v>
+        <v>293.6</v>
       </c>
       <c r="AE350" s="12">
-        <v>2340</v>
+        <v>2936</v>
       </c>
       <c r="AF350" s="12">
-        <v>2340</v>
+        <v>2936</v>
       </c>
     </row>
     <row r="351" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A351" s="13" t="s">
-        <v>854</v>
+        <v>862</v>
       </c>
       <c r="B351" s="13" t="s">
         <v>33</v>
@@ -34369,7 +34387,7 @@
         <v>43920</v>
       </c>
       <c r="D351" s="15" t="s">
-        <v>855</v>
+        <v>863</v>
       </c>
       <c r="E351" s="15" t="s">
         <v>33</v>
@@ -34378,7 +34396,7 @@
         <v>2260</v>
       </c>
       <c r="G351" s="13" t="s">
-        <v>856</v>
+        <v>864</v>
       </c>
       <c r="H351" s="13" t="s">
         <v>36</v>
@@ -34387,32 +34405,20 @@
         <v>37</v>
       </c>
       <c r="J351" s="17">
-        <v>9.245762e6</v>
-      </c>
-      <c r="K351" s="15" t="s">
-        <v>876</v>
-      </c>
-      <c r="L351" s="17">
-        <v>2260</v>
-      </c>
-      <c r="M351" s="15" t="s">
-        <v>856</v>
-      </c>
-      <c r="N351" s="18">
-        <v>43936</v>
-      </c>
-      <c r="O351" s="18">
-        <v>43936</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K351" s="15"/>
+      <c r="L351" s="17"/>
+      <c r="M351" s="15"/>
+      <c r="N351" s="18"/>
+      <c r="O351" s="18"/>
       <c r="P351" s="19"/>
-      <c r="Q351" s="18">
-        <v>44115</v>
-      </c>
+      <c r="Q351" s="18"/>
       <c r="R351" s="15" t="s">
-        <v>877</v>
+        <v>744</v>
       </c>
       <c r="S351" s="15" t="s">
-        <v>878</v>
+        <v>745</v>
       </c>
       <c r="T351" s="13" t="s">
         <v>33</v>
@@ -34421,42 +34427,42 @@
         <v>33</v>
       </c>
       <c r="V351" s="17">
-        <v>781673</v>
+        <v>1.497391e6</v>
       </c>
       <c r="W351" s="15" t="s">
-        <v>879</v>
+        <v>874</v>
       </c>
       <c r="X351" s="17">
         <v>2261</v>
       </c>
       <c r="Y351" s="15" t="s">
-        <v>856</v>
+        <v>864</v>
       </c>
       <c r="Z351" s="15" t="s">
-        <v>122</v>
+        <v>379</v>
       </c>
       <c r="AA351" s="13" t="s">
         <v>44</v>
       </c>
       <c r="AB351" s="21">
-        <v>30000</v>
+        <v>15</v>
       </c>
       <c r="AC351" s="22">
-        <v>900000e-6</v>
+        <v>3420</v>
       </c>
       <c r="AD351" s="22">
-        <v>900000e-6</v>
+        <v>3420</v>
       </c>
       <c r="AE351" s="23">
-        <v>27000</v>
+        <v>51300</v>
       </c>
       <c r="AF351" s="23">
-        <v>27000</v>
+        <v>51300</v>
       </c>
     </row>
     <row r="352" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A352" s="3" t="s">
-        <v>854</v>
+        <v>862</v>
       </c>
       <c r="B352" s="3" t="s">
         <v>33</v>
@@ -34465,7 +34471,7 @@
         <v>43920</v>
       </c>
       <c r="D352" s="5" t="s">
-        <v>855</v>
+        <v>863</v>
       </c>
       <c r="E352" s="5" t="s">
         <v>33</v>
@@ -34474,7 +34480,7 @@
         <v>2260</v>
       </c>
       <c r="G352" s="3" t="s">
-        <v>856</v>
+        <v>864</v>
       </c>
       <c r="H352" s="3" t="s">
         <v>36</v>
@@ -34483,32 +34489,20 @@
         <v>37</v>
       </c>
       <c r="J352" s="7">
-        <v>9.245763e6</v>
-      </c>
-      <c r="K352" s="5" t="s">
-        <v>880</v>
-      </c>
-      <c r="L352" s="7">
-        <v>2260</v>
-      </c>
-      <c r="M352" s="5" t="s">
-        <v>856</v>
-      </c>
-      <c r="N352" s="8">
-        <v>43936</v>
-      </c>
-      <c r="O352" s="8">
-        <v>43936</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K352" s="5"/>
+      <c r="L352" s="7"/>
+      <c r="M352" s="5"/>
+      <c r="N352" s="8"/>
+      <c r="O352" s="8"/>
       <c r="P352" s="9"/>
-      <c r="Q352" s="8">
-        <v>44115</v>
-      </c>
+      <c r="Q352" s="8"/>
       <c r="R352" s="5" t="s">
-        <v>881</v>
+        <v>875</v>
       </c>
       <c r="S352" s="5" t="s">
-        <v>882</v>
+        <v>876</v>
       </c>
       <c r="T352" s="3" t="s">
         <v>33</v>
@@ -34517,42 +34511,42 @@
         <v>33</v>
       </c>
       <c r="V352" s="7">
-        <v>538957</v>
+        <v>1.669613e6</v>
       </c>
       <c r="W352" s="5" t="s">
-        <v>883</v>
+        <v>877</v>
       </c>
       <c r="X352" s="7">
         <v>2261</v>
       </c>
       <c r="Y352" s="5" t="s">
-        <v>856</v>
+        <v>864</v>
       </c>
       <c r="Z352" s="5" t="s">
-        <v>122</v>
+        <v>379</v>
       </c>
       <c r="AA352" s="3" t="s">
         <v>44</v>
       </c>
       <c r="AB352" s="10">
-        <v>30000</v>
+        <v>10</v>
       </c>
       <c r="AC352" s="11">
-        <v>550000e-6</v>
+        <v>31.96</v>
       </c>
       <c r="AD352" s="11">
-        <v>550000e-6</v>
+        <v>31.96</v>
       </c>
       <c r="AE352" s="12">
-        <v>16500</v>
+        <v>319.6</v>
       </c>
       <c r="AF352" s="12">
-        <v>16500</v>
+        <v>319.6</v>
       </c>
     </row>
     <row r="353" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A353" s="13" t="s">
-        <v>854</v>
+        <v>862</v>
       </c>
       <c r="B353" s="13" t="s">
         <v>33</v>
@@ -34561,7 +34555,7 @@
         <v>43920</v>
       </c>
       <c r="D353" s="15" t="s">
-        <v>855</v>
+        <v>863</v>
       </c>
       <c r="E353" s="15" t="s">
         <v>33</v>
@@ -34570,7 +34564,7 @@
         <v>2260</v>
       </c>
       <c r="G353" s="13" t="s">
-        <v>856</v>
+        <v>864</v>
       </c>
       <c r="H353" s="13" t="s">
         <v>36</v>
@@ -34579,100 +34573,88 @@
         <v>37</v>
       </c>
       <c r="J353" s="17">
-        <v>9.245763e6</v>
-      </c>
-      <c r="K353" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="K353" s="15"/>
+      <c r="L353" s="17"/>
+      <c r="M353" s="15"/>
+      <c r="N353" s="18"/>
+      <c r="O353" s="18"/>
+      <c r="P353" s="19"/>
+      <c r="Q353" s="18"/>
+      <c r="R353" s="15" t="s">
+        <v>878</v>
+      </c>
+      <c r="S353" s="15" t="s">
+        <v>879</v>
+      </c>
+      <c r="T353" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="U353" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="V353" s="17">
+        <v>857025</v>
+      </c>
+      <c r="W353" s="15" t="s">
         <v>880</v>
-      </c>
-      <c r="L353" s="17">
-        <v>2260</v>
-      </c>
-      <c r="M353" s="15" t="s">
-        <v>856</v>
-      </c>
-      <c r="N353" s="18">
-        <v>43936</v>
-      </c>
-      <c r="O353" s="18">
-        <v>43936</v>
-      </c>
-      <c r="P353" s="19"/>
-      <c r="Q353" s="18">
-        <v>44115</v>
-      </c>
-      <c r="R353" s="15" t="s">
-        <v>881</v>
-      </c>
-      <c r="S353" s="15" t="s">
-        <v>882</v>
-      </c>
-      <c r="T353" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="U353" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="V353" s="17">
-        <v>1.651595e6</v>
-      </c>
-      <c r="W353" s="15" t="s">
-        <v>884</v>
       </c>
       <c r="X353" s="17">
         <v>2261</v>
       </c>
       <c r="Y353" s="15" t="s">
-        <v>856</v>
+        <v>864</v>
       </c>
       <c r="Z353" s="15" t="s">
-        <v>122</v>
+        <v>379</v>
       </c>
       <c r="AA353" s="13" t="s">
         <v>44</v>
       </c>
       <c r="AB353" s="21">
-        <v>30000</v>
+        <v>100</v>
       </c>
       <c r="AC353" s="22">
-        <v>1.08</v>
+        <v>16.756</v>
       </c>
       <c r="AD353" s="22">
-        <v>1.08</v>
+        <v>16.756</v>
       </c>
       <c r="AE353" s="23">
-        <v>32400</v>
+        <v>1675.6</v>
       </c>
       <c r="AF353" s="23">
-        <v>32400</v>
+        <v>1675.6</v>
       </c>
     </row>
     <row r="354" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A354" s="3" t="s">
-        <v>885</v>
+        <v>862</v>
       </c>
       <c r="B354" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C354" s="4">
-        <v>43972</v>
+        <v>43920</v>
       </c>
       <c r="D354" s="5" t="s">
-        <v>886</v>
+        <v>863</v>
       </c>
       <c r="E354" s="5" t="s">
         <v>33</v>
       </c>
       <c r="F354" s="6">
-        <v>2280</v>
+        <v>2260</v>
       </c>
       <c r="G354" s="3" t="s">
-        <v>887</v>
+        <v>864</v>
       </c>
       <c r="H354" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I354" s="3" t="s">
-        <v>468</v>
+        <v>37</v>
       </c>
       <c r="J354" s="7">
         <v>0</v>
@@ -34685,10 +34667,10 @@
       <c r="P354" s="9"/>
       <c r="Q354" s="8"/>
       <c r="R354" s="5" t="s">
-        <v>469</v>
+        <v>881</v>
       </c>
       <c r="S354" s="5" t="s">
-        <v>470</v>
+        <v>882</v>
       </c>
       <c r="T354" s="3" t="s">
         <v>33</v>
@@ -34697,60 +34679,60 @@
         <v>33</v>
       </c>
       <c r="V354" s="7">
-        <v>1.756699e6</v>
+        <v>1.151746e6</v>
       </c>
       <c r="W354" s="5" t="s">
-        <v>471</v>
+        <v>883</v>
       </c>
       <c r="X354" s="7">
-        <v>2281</v>
+        <v>2261</v>
       </c>
       <c r="Y354" s="5" t="s">
-        <v>888</v>
+        <v>864</v>
       </c>
       <c r="Z354" s="5" t="s">
-        <v>373</v>
+        <v>379</v>
       </c>
       <c r="AA354" s="3" t="s">
-        <v>295</v>
+        <v>44</v>
       </c>
       <c r="AB354" s="10">
-        <v>127</v>
+        <v>20</v>
       </c>
       <c r="AC354" s="11">
-        <v>1.89</v>
+        <v>117</v>
       </c>
       <c r="AD354" s="11">
-        <v>1.89</v>
+        <v>117</v>
       </c>
       <c r="AE354" s="12">
-        <v>240.03</v>
+        <v>2340</v>
       </c>
       <c r="AF354" s="12">
-        <v>240.03</v>
+        <v>2340</v>
       </c>
     </row>
     <row r="355" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A355" s="13" t="s">
-        <v>889</v>
+        <v>862</v>
       </c>
       <c r="B355" s="13" t="s">
         <v>33</v>
       </c>
       <c r="C355" s="14">
-        <v>43921</v>
+        <v>43920</v>
       </c>
       <c r="D355" s="15" t="s">
-        <v>890</v>
+        <v>863</v>
       </c>
       <c r="E355" s="15" t="s">
         <v>33</v>
       </c>
       <c r="F355" s="16">
-        <v>2300</v>
+        <v>2260</v>
       </c>
       <c r="G355" s="13" t="s">
-        <v>891</v>
+        <v>864</v>
       </c>
       <c r="H355" s="13" t="s">
         <v>36</v>
@@ -34759,34 +34741,32 @@
         <v>37</v>
       </c>
       <c r="J355" s="17">
-        <v>9.245674e6</v>
+        <v>9.245762e6</v>
       </c>
       <c r="K355" s="15" t="s">
-        <v>892</v>
+        <v>884</v>
       </c>
       <c r="L355" s="17">
-        <v>2300</v>
+        <v>2260</v>
       </c>
       <c r="M355" s="15" t="s">
-        <v>891</v>
+        <v>864</v>
       </c>
       <c r="N355" s="18">
-        <v>43922</v>
+        <v>43936</v>
       </c>
       <c r="O355" s="18">
-        <v>43922</v>
-      </c>
-      <c r="P355" s="19">
-        <v>44105</v>
-      </c>
+        <v>43936</v>
+      </c>
+      <c r="P355" s="19"/>
       <c r="Q355" s="18">
-        <v>44131</v>
+        <v>44115</v>
       </c>
       <c r="R355" s="15" t="s">
-        <v>893</v>
+        <v>885</v>
       </c>
       <c r="S355" s="15" t="s">
-        <v>894</v>
+        <v>886</v>
       </c>
       <c r="T355" s="13" t="s">
         <v>33</v>
@@ -34795,60 +34775,60 @@
         <v>33</v>
       </c>
       <c r="V355" s="17">
-        <v>1155</v>
+        <v>781673</v>
       </c>
       <c r="W355" s="15" t="s">
-        <v>107</v>
+        <v>887</v>
       </c>
       <c r="X355" s="17">
-        <v>2301</v>
+        <v>2261</v>
       </c>
       <c r="Y355" s="15" t="s">
-        <v>895</v>
+        <v>864</v>
       </c>
       <c r="Z355" s="15" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="AA355" s="13" t="s">
         <v>44</v>
       </c>
       <c r="AB355" s="21">
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="AC355" s="22">
-        <v>4.35942886e6</v>
+        <v>900000e-6</v>
       </c>
       <c r="AD355" s="22">
-        <v>4.35942886e6</v>
+        <v>900000e-6</v>
       </c>
       <c r="AE355" s="23">
-        <v>4.35942886e6</v>
+        <v>27000</v>
       </c>
       <c r="AF355" s="23">
-        <v>4.35942886e6</v>
+        <v>27000</v>
       </c>
     </row>
     <row r="356" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A356" s="3" t="s">
-        <v>896</v>
+        <v>862</v>
       </c>
       <c r="B356" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C356" s="4">
-        <v>43935</v>
+        <v>43920</v>
       </c>
       <c r="D356" s="5" t="s">
-        <v>897</v>
+        <v>863</v>
       </c>
       <c r="E356" s="5" t="s">
         <v>33</v>
       </c>
       <c r="F356" s="6">
-        <v>2300</v>
+        <v>2260</v>
       </c>
       <c r="G356" s="3" t="s">
-        <v>891</v>
+        <v>864</v>
       </c>
       <c r="H356" s="3" t="s">
         <v>36</v>
@@ -34857,16 +34837,16 @@
         <v>37</v>
       </c>
       <c r="J356" s="7">
-        <v>9.24595e6</v>
+        <v>9.245763e6</v>
       </c>
       <c r="K356" s="5" t="s">
-        <v>898</v>
+        <v>888</v>
       </c>
       <c r="L356" s="7">
-        <v>2300</v>
+        <v>2260</v>
       </c>
       <c r="M356" s="5" t="s">
-        <v>891</v>
+        <v>864</v>
       </c>
       <c r="N356" s="8">
         <v>43936</v>
@@ -34874,17 +34854,15 @@
       <c r="O356" s="8">
         <v>43936</v>
       </c>
-      <c r="P356" s="9">
-        <v>44119</v>
-      </c>
+      <c r="P356" s="9"/>
       <c r="Q356" s="8">
-        <v>44119</v>
+        <v>44115</v>
       </c>
       <c r="R356" s="5" t="s">
-        <v>899</v>
+        <v>889</v>
       </c>
       <c r="S356" s="5" t="s">
-        <v>900</v>
+        <v>890</v>
       </c>
       <c r="T356" s="3" t="s">
         <v>33</v>
@@ -34893,60 +34871,60 @@
         <v>33</v>
       </c>
       <c r="V356" s="7">
-        <v>1155</v>
+        <v>538957</v>
       </c>
       <c r="W356" s="5" t="s">
-        <v>107</v>
+        <v>891</v>
       </c>
       <c r="X356" s="7">
-        <v>2301</v>
+        <v>2261</v>
       </c>
       <c r="Y356" s="5" t="s">
-        <v>895</v>
+        <v>864</v>
       </c>
       <c r="Z356" s="5" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="AA356" s="3" t="s">
         <v>44</v>
       </c>
       <c r="AB356" s="10">
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="AC356" s="11">
-        <v>1.04162557e6</v>
+        <v>550000e-6</v>
       </c>
       <c r="AD356" s="11">
-        <v>1.04162557e6</v>
+        <v>550000e-6</v>
       </c>
       <c r="AE356" s="12">
-        <v>1.04162557e6</v>
+        <v>16500</v>
       </c>
       <c r="AF356" s="12">
-        <v>1.04162557e6</v>
+        <v>16500</v>
       </c>
     </row>
     <row r="357" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A357" s="13" t="s">
-        <v>901</v>
+        <v>862</v>
       </c>
       <c r="B357" s="13" t="s">
         <v>33</v>
       </c>
       <c r="C357" s="14">
-        <v>43963</v>
+        <v>43920</v>
       </c>
       <c r="D357" s="15" t="s">
-        <v>902</v>
+        <v>863</v>
       </c>
       <c r="E357" s="15" t="s">
         <v>33</v>
       </c>
       <c r="F357" s="16">
-        <v>2300</v>
+        <v>2260</v>
       </c>
       <c r="G357" s="13" t="s">
-        <v>891</v>
+        <v>864</v>
       </c>
       <c r="H357" s="13" t="s">
         <v>36</v>
@@ -34955,34 +34933,32 @@
         <v>37</v>
       </c>
       <c r="J357" s="17">
-        <v>9.247198e6</v>
+        <v>9.245763e6</v>
       </c>
       <c r="K357" s="15" t="s">
-        <v>903</v>
+        <v>888</v>
       </c>
       <c r="L357" s="17">
-        <v>2300</v>
+        <v>2260</v>
       </c>
       <c r="M357" s="15" t="s">
-        <v>891</v>
+        <v>864</v>
       </c>
       <c r="N357" s="18">
-        <v>43963</v>
+        <v>43936</v>
       </c>
       <c r="O357" s="18">
-        <v>43963</v>
-      </c>
-      <c r="P357" s="19">
-        <v>44195</v>
-      </c>
+        <v>43936</v>
+      </c>
+      <c r="P357" s="19"/>
       <c r="Q357" s="18">
-        <v>44195</v>
+        <v>44115</v>
       </c>
       <c r="R357" s="15" t="s">
-        <v>904</v>
+        <v>889</v>
       </c>
       <c r="S357" s="15" t="s">
-        <v>905</v>
+        <v>890</v>
       </c>
       <c r="T357" s="13" t="s">
         <v>33</v>
@@ -34991,96 +34967,82 @@
         <v>33</v>
       </c>
       <c r="V357" s="17">
-        <v>1155</v>
+        <v>1.651595e6</v>
       </c>
       <c r="W357" s="15" t="s">
-        <v>107</v>
+        <v>892</v>
       </c>
       <c r="X357" s="17">
-        <v>2301</v>
+        <v>2261</v>
       </c>
       <c r="Y357" s="15" t="s">
-        <v>895</v>
+        <v>864</v>
       </c>
       <c r="Z357" s="15" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="AA357" s="13" t="s">
         <v>44</v>
       </c>
       <c r="AB357" s="21">
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="AC357" s="22">
-        <v>7.11634326e6</v>
+        <v>1.08</v>
       </c>
       <c r="AD357" s="22">
-        <v>7.11634326e6</v>
+        <v>1.08</v>
       </c>
       <c r="AE357" s="23">
-        <v>7.11634326e6</v>
+        <v>32400</v>
       </c>
       <c r="AF357" s="23">
-        <v>7.11634326e6</v>
+        <v>32400</v>
       </c>
     </row>
     <row r="358" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A358" s="3" t="s">
-        <v>906</v>
+        <v>893</v>
       </c>
       <c r="B358" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C358" s="4">
-        <v>43928</v>
+        <v>43972</v>
       </c>
       <c r="D358" s="5" t="s">
-        <v>907</v>
+        <v>894</v>
       </c>
       <c r="E358" s="5" t="s">
         <v>33</v>
       </c>
       <c r="F358" s="6">
-        <v>2310</v>
+        <v>2280</v>
       </c>
       <c r="G358" s="3" t="s">
-        <v>908</v>
+        <v>895</v>
       </c>
       <c r="H358" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I358" s="3" t="s">
-        <v>37</v>
+        <v>468</v>
       </c>
       <c r="J358" s="7">
-        <v>9.245982e6</v>
-      </c>
-      <c r="K358" s="5" t="s">
-        <v>909</v>
-      </c>
-      <c r="L358" s="7">
-        <v>2310</v>
-      </c>
-      <c r="M358" s="5" t="s">
-        <v>908</v>
-      </c>
-      <c r="N358" s="8">
-        <v>43943</v>
-      </c>
-      <c r="O358" s="8">
-        <v>43939</v>
-      </c>
-      <c r="P358" s="9">
-        <v>44304</v>
-      </c>
-      <c r="Q358" s="8">
-        <v>44121</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K358" s="5"/>
+      <c r="L358" s="7"/>
+      <c r="M358" s="5"/>
+      <c r="N358" s="8"/>
+      <c r="O358" s="8"/>
+      <c r="P358" s="9"/>
+      <c r="Q358" s="8"/>
       <c r="R358" s="5" t="s">
-        <v>782</v>
+        <v>469</v>
       </c>
       <c r="S358" s="5" t="s">
-        <v>783</v>
+        <v>470</v>
       </c>
       <c r="T358" s="3" t="s">
         <v>33</v>
@@ -35089,60 +35051,60 @@
         <v>33</v>
       </c>
       <c r="V358" s="7">
-        <v>18228</v>
-      </c>
-      <c r="W358" s="24" t="s">
-        <v>910</v>
+        <v>1.756699e6</v>
+      </c>
+      <c r="W358" s="5" t="s">
+        <v>471</v>
       </c>
       <c r="X358" s="7">
-        <v>2311</v>
+        <v>2281</v>
       </c>
       <c r="Y358" s="5" t="s">
-        <v>908</v>
+        <v>896</v>
       </c>
       <c r="Z358" s="5" t="s">
-        <v>365</v>
+        <v>373</v>
       </c>
       <c r="AA358" s="3" t="s">
-        <v>911</v>
+        <v>295</v>
       </c>
       <c r="AB358" s="10">
-        <v>200</v>
+        <v>127</v>
       </c>
       <c r="AC358" s="11">
-        <v>36</v>
+        <v>1.89</v>
       </c>
       <c r="AD358" s="11">
-        <v>36</v>
+        <v>1.89</v>
       </c>
       <c r="AE358" s="12">
-        <v>7200</v>
+        <v>240.03</v>
       </c>
       <c r="AF358" s="12">
-        <v>7200</v>
+        <v>240.03</v>
       </c>
     </row>
     <row r="359" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A359" s="13" t="s">
-        <v>906</v>
+        <v>897</v>
       </c>
       <c r="B359" s="13" t="s">
         <v>33</v>
       </c>
       <c r="C359" s="14">
-        <v>43928</v>
+        <v>43921</v>
       </c>
       <c r="D359" s="15" t="s">
-        <v>907</v>
+        <v>898</v>
       </c>
       <c r="E359" s="15" t="s">
         <v>33</v>
       </c>
       <c r="F359" s="16">
-        <v>2310</v>
+        <v>2300</v>
       </c>
       <c r="G359" s="13" t="s">
-        <v>908</v>
+        <v>899</v>
       </c>
       <c r="H359" s="13" t="s">
         <v>36</v>
@@ -35151,34 +35113,34 @@
         <v>37</v>
       </c>
       <c r="J359" s="17">
-        <v>9.245982e6</v>
+        <v>9.245674e6</v>
       </c>
       <c r="K359" s="15" t="s">
-        <v>909</v>
+        <v>900</v>
       </c>
       <c r="L359" s="17">
-        <v>2310</v>
+        <v>2300</v>
       </c>
       <c r="M359" s="15" t="s">
-        <v>908</v>
+        <v>899</v>
       </c>
       <c r="N359" s="18">
-        <v>43943</v>
+        <v>43922</v>
       </c>
       <c r="O359" s="18">
-        <v>43939</v>
+        <v>43922</v>
       </c>
       <c r="P359" s="19">
-        <v>44304</v>
+        <v>44105</v>
       </c>
       <c r="Q359" s="18">
-        <v>44121</v>
+        <v>44131</v>
       </c>
       <c r="R359" s="15" t="s">
-        <v>782</v>
+        <v>901</v>
       </c>
       <c r="S359" s="15" t="s">
-        <v>783</v>
+        <v>902</v>
       </c>
       <c r="T359" s="13" t="s">
         <v>33</v>
@@ -35187,60 +35149,60 @@
         <v>33</v>
       </c>
       <c r="V359" s="17">
-        <v>236268</v>
+        <v>1155</v>
       </c>
       <c r="W359" s="15" t="s">
-        <v>912</v>
+        <v>107</v>
       </c>
       <c r="X359" s="17">
-        <v>2311</v>
+        <v>2301</v>
       </c>
       <c r="Y359" s="15" t="s">
-        <v>908</v>
+        <v>903</v>
       </c>
       <c r="Z359" s="15" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="AA359" s="13" t="s">
-        <v>911</v>
+        <v>44</v>
       </c>
       <c r="AB359" s="21">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC359" s="22">
-        <v>45</v>
+        <v>4.35942886e6</v>
       </c>
       <c r="AD359" s="22">
-        <v>45</v>
+        <v>4.35942886e6</v>
       </c>
       <c r="AE359" s="23">
-        <v>2250</v>
+        <v>4.35942886e6</v>
       </c>
       <c r="AF359" s="23">
-        <v>2250</v>
+        <v>4.35942886e6</v>
       </c>
     </row>
     <row r="360" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A360" s="3" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="B360" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C360" s="4">
-        <v>43928</v>
+        <v>43935</v>
       </c>
       <c r="D360" s="5" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="E360" s="5" t="s">
         <v>33</v>
       </c>
       <c r="F360" s="6">
-        <v>2310</v>
+        <v>2300</v>
       </c>
       <c r="G360" s="3" t="s">
-        <v>908</v>
+        <v>899</v>
       </c>
       <c r="H360" s="3" t="s">
         <v>36</v>
@@ -35249,35 +35211,35 @@
         <v>37</v>
       </c>
       <c r="J360" s="7">
-        <v>9.245982e6</v>
+        <v>9.24595e6</v>
       </c>
       <c r="K360" s="5" t="s">
-        <v>909</v>
+        <v>906</v>
       </c>
       <c r="L360" s="7">
-        <v>2310</v>
+        <v>2300</v>
       </c>
       <c r="M360" s="5" t="s">
+        <v>899</v>
+      </c>
+      <c r="N360" s="8">
+        <v>43936</v>
+      </c>
+      <c r="O360" s="8">
+        <v>43936</v>
+      </c>
+      <c r="P360" s="9">
+        <v>44119</v>
+      </c>
+      <c r="Q360" s="8">
+        <v>44119</v>
+      </c>
+      <c r="R360" s="5" t="s">
+        <v>907</v>
+      </c>
+      <c r="S360" s="5" t="s">
         <v>908</v>
       </c>
-      <c r="N360" s="8">
-        <v>43943</v>
-      </c>
-      <c r="O360" s="8">
-        <v>43939</v>
-      </c>
-      <c r="P360" s="9">
-        <v>44304</v>
-      </c>
-      <c r="Q360" s="8">
-        <v>44121</v>
-      </c>
-      <c r="R360" s="5" t="s">
-        <v>782</v>
-      </c>
-      <c r="S360" s="5" t="s">
-        <v>783</v>
-      </c>
       <c r="T360" s="3" t="s">
         <v>33</v>
       </c>
@@ -35285,60 +35247,60 @@
         <v>33</v>
       </c>
       <c r="V360" s="7">
-        <v>461920</v>
+        <v>1155</v>
       </c>
       <c r="W360" s="5" t="s">
-        <v>789</v>
+        <v>107</v>
       </c>
       <c r="X360" s="7">
-        <v>2311</v>
+        <v>2301</v>
       </c>
       <c r="Y360" s="5" t="s">
-        <v>908</v>
+        <v>903</v>
       </c>
       <c r="Z360" s="5" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="AA360" s="3" t="s">
-        <v>911</v>
+        <v>44</v>
       </c>
       <c r="AB360" s="10">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="AC360" s="11">
-        <v>8</v>
+        <v>1.04162557e6</v>
       </c>
       <c r="AD360" s="11">
-        <v>8</v>
+        <v>1.04162557e6</v>
       </c>
       <c r="AE360" s="12">
-        <v>4800</v>
+        <v>1.04162557e6</v>
       </c>
       <c r="AF360" s="12">
-        <v>4800</v>
+        <v>1.04162557e6</v>
       </c>
     </row>
     <row r="361" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A361" s="13" t="s">
-        <v>906</v>
+        <v>909</v>
       </c>
       <c r="B361" s="13" t="s">
         <v>33</v>
       </c>
       <c r="C361" s="14">
-        <v>43928</v>
+        <v>43963</v>
       </c>
       <c r="D361" s="15" t="s">
-        <v>907</v>
+        <v>910</v>
       </c>
       <c r="E361" s="15" t="s">
         <v>33</v>
       </c>
       <c r="F361" s="16">
-        <v>2310</v>
+        <v>2300</v>
       </c>
       <c r="G361" s="13" t="s">
-        <v>908</v>
+        <v>899</v>
       </c>
       <c r="H361" s="13" t="s">
         <v>36</v>
@@ -35347,34 +35309,34 @@
         <v>37</v>
       </c>
       <c r="J361" s="17">
-        <v>9.245982e6</v>
+        <v>9.247198e6</v>
       </c>
       <c r="K361" s="15" t="s">
-        <v>909</v>
+        <v>911</v>
       </c>
       <c r="L361" s="17">
-        <v>2310</v>
+        <v>2300</v>
       </c>
       <c r="M361" s="15" t="s">
-        <v>908</v>
+        <v>899</v>
       </c>
       <c r="N361" s="18">
-        <v>43943</v>
+        <v>43963</v>
       </c>
       <c r="O361" s="18">
-        <v>43939</v>
+        <v>43963</v>
       </c>
       <c r="P361" s="19">
-        <v>44304</v>
+        <v>44195</v>
       </c>
       <c r="Q361" s="18">
-        <v>44121</v>
+        <v>44195</v>
       </c>
       <c r="R361" s="15" t="s">
-        <v>782</v>
+        <v>912</v>
       </c>
       <c r="S361" s="15" t="s">
-        <v>783</v>
+        <v>913</v>
       </c>
       <c r="T361" s="13" t="s">
         <v>33</v>
@@ -35383,42 +35345,42 @@
         <v>33</v>
       </c>
       <c r="V361" s="17">
-        <v>804495</v>
+        <v>1155</v>
       </c>
       <c r="W361" s="15" t="s">
-        <v>784</v>
+        <v>107</v>
       </c>
       <c r="X361" s="17">
-        <v>2311</v>
+        <v>2301</v>
       </c>
       <c r="Y361" s="15" t="s">
-        <v>908</v>
+        <v>903</v>
       </c>
       <c r="Z361" s="15" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="AA361" s="13" t="s">
-        <v>911</v>
+        <v>44</v>
       </c>
       <c r="AB361" s="21">
-        <v>170</v>
+        <v>0</v>
       </c>
       <c r="AC361" s="22">
-        <v>45</v>
+        <v>7.11634326e6</v>
       </c>
       <c r="AD361" s="22">
-        <v>45</v>
+        <v>7.11634326e6</v>
       </c>
       <c r="AE361" s="23">
-        <v>7650</v>
+        <v>7.11634326e6</v>
       </c>
       <c r="AF361" s="23">
-        <v>7650</v>
+        <v>7.11634326e6</v>
       </c>
     </row>
     <row r="362" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A362" s="3" t="s">
-        <v>906</v>
+        <v>914</v>
       </c>
       <c r="B362" s="3" t="s">
         <v>33</v>
@@ -35427,7 +35389,7 @@
         <v>43928</v>
       </c>
       <c r="D362" s="5" t="s">
-        <v>907</v>
+        <v>915</v>
       </c>
       <c r="E362" s="5" t="s">
         <v>33</v>
@@ -35436,7 +35398,7 @@
         <v>2310</v>
       </c>
       <c r="G362" s="3" t="s">
-        <v>908</v>
+        <v>916</v>
       </c>
       <c r="H362" s="3" t="s">
         <v>36</v>
@@ -35448,13 +35410,13 @@
         <v>9.245982e6</v>
       </c>
       <c r="K362" s="5" t="s">
-        <v>909</v>
+        <v>917</v>
       </c>
       <c r="L362" s="7">
         <v>2310</v>
       </c>
       <c r="M362" s="5" t="s">
-        <v>908</v>
+        <v>916</v>
       </c>
       <c r="N362" s="8">
         <v>43943</v>
@@ -35481,42 +35443,42 @@
         <v>33</v>
       </c>
       <c r="V362" s="7">
-        <v>1.129139e6</v>
-      </c>
-      <c r="W362" s="5" t="s">
-        <v>913</v>
+        <v>18228</v>
+      </c>
+      <c r="W362" s="24" t="s">
+        <v>918</v>
       </c>
       <c r="X362" s="7">
         <v>2311</v>
       </c>
       <c r="Y362" s="5" t="s">
-        <v>908</v>
+        <v>916</v>
       </c>
       <c r="Z362" s="5" t="s">
-        <v>129</v>
+        <v>365</v>
       </c>
       <c r="AA362" s="3" t="s">
-        <v>911</v>
+        <v>919</v>
       </c>
       <c r="AB362" s="10">
-        <v>30</v>
+        <v>200</v>
       </c>
       <c r="AC362" s="11">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="AD362" s="11">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="AE362" s="12">
-        <v>1350</v>
+        <v>7200</v>
       </c>
       <c r="AF362" s="12">
-        <v>1350</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="363" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A363" s="13" t="s">
-        <v>906</v>
+        <v>914</v>
       </c>
       <c r="B363" s="13" t="s">
         <v>33</v>
@@ -35525,7 +35487,7 @@
         <v>43928</v>
       </c>
       <c r="D363" s="15" t="s">
-        <v>907</v>
+        <v>915</v>
       </c>
       <c r="E363" s="15" t="s">
         <v>33</v>
@@ -35534,7 +35496,7 @@
         <v>2310</v>
       </c>
       <c r="G363" s="13" t="s">
-        <v>908</v>
+        <v>916</v>
       </c>
       <c r="H363" s="13" t="s">
         <v>36</v>
@@ -35546,13 +35508,13 @@
         <v>9.245982e6</v>
       </c>
       <c r="K363" s="15" t="s">
-        <v>909</v>
+        <v>917</v>
       </c>
       <c r="L363" s="17">
         <v>2310</v>
       </c>
       <c r="M363" s="15" t="s">
-        <v>908</v>
+        <v>916</v>
       </c>
       <c r="N363" s="18">
         <v>43943</v>
@@ -35579,25 +35541,25 @@
         <v>33</v>
       </c>
       <c r="V363" s="17">
-        <v>1.152823e6</v>
+        <v>236268</v>
       </c>
       <c r="W363" s="15" t="s">
-        <v>914</v>
+        <v>920</v>
       </c>
       <c r="X363" s="17">
         <v>2311</v>
       </c>
       <c r="Y363" s="15" t="s">
-        <v>908</v>
+        <v>916</v>
       </c>
       <c r="Z363" s="15" t="s">
         <v>129</v>
       </c>
       <c r="AA363" s="13" t="s">
-        <v>911</v>
+        <v>919</v>
       </c>
       <c r="AB363" s="21">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="AC363" s="22">
         <v>45</v>
@@ -35606,15 +35568,15 @@
         <v>45</v>
       </c>
       <c r="AE363" s="23">
-        <v>1350</v>
+        <v>2250</v>
       </c>
       <c r="AF363" s="23">
-        <v>1350</v>
+        <v>2250</v>
       </c>
     </row>
     <row r="364" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A364" s="3" t="s">
-        <v>906</v>
+        <v>914</v>
       </c>
       <c r="B364" s="3" t="s">
         <v>33</v>
@@ -35623,7 +35585,7 @@
         <v>43928</v>
       </c>
       <c r="D364" s="5" t="s">
-        <v>907</v>
+        <v>915</v>
       </c>
       <c r="E364" s="5" t="s">
         <v>33</v>
@@ -35632,7 +35594,7 @@
         <v>2310</v>
       </c>
       <c r="G364" s="3" t="s">
-        <v>908</v>
+        <v>916</v>
       </c>
       <c r="H364" s="3" t="s">
         <v>36</v>
@@ -35644,13 +35606,13 @@
         <v>9.245982e6</v>
       </c>
       <c r="K364" s="5" t="s">
-        <v>909</v>
+        <v>917</v>
       </c>
       <c r="L364" s="7">
         <v>2310</v>
       </c>
       <c r="M364" s="5" t="s">
-        <v>908</v>
+        <v>916</v>
       </c>
       <c r="N364" s="8">
         <v>43943</v>
@@ -35677,51 +35639,51 @@
         <v>33</v>
       </c>
       <c r="V364" s="7">
-        <v>1.152831e6</v>
+        <v>461920</v>
       </c>
       <c r="W364" s="5" t="s">
-        <v>915</v>
+        <v>789</v>
       </c>
       <c r="X364" s="7">
         <v>2311</v>
       </c>
       <c r="Y364" s="5" t="s">
-        <v>908</v>
+        <v>916</v>
       </c>
       <c r="Z364" s="5" t="s">
         <v>129</v>
       </c>
       <c r="AA364" s="3" t="s">
-        <v>911</v>
+        <v>919</v>
       </c>
       <c r="AB364" s="10">
-        <v>30</v>
+        <v>600</v>
       </c>
       <c r="AC364" s="11">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="AD364" s="11">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="AE364" s="12">
-        <v>1350</v>
+        <v>4800</v>
       </c>
       <c r="AF364" s="12">
-        <v>1350</v>
+        <v>4800</v>
       </c>
     </row>
     <row r="365" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A365" s="13" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="B365" s="13" t="s">
         <v>33</v>
       </c>
       <c r="C365" s="14">
-        <v>43955</v>
+        <v>43928</v>
       </c>
       <c r="D365" s="15" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="E365" s="15" t="s">
         <v>33</v>
@@ -35730,7 +35692,7 @@
         <v>2310</v>
       </c>
       <c r="G365" s="13" t="s">
-        <v>908</v>
+        <v>916</v>
       </c>
       <c r="H365" s="13" t="s">
         <v>36</v>
@@ -35739,34 +35701,34 @@
         <v>37</v>
       </c>
       <c r="J365" s="17">
-        <v>9.251383e6</v>
+        <v>9.245982e6</v>
       </c>
       <c r="K365" s="15" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="L365" s="17">
         <v>2310</v>
       </c>
       <c r="M365" s="15" t="s">
-        <v>908</v>
+        <v>916</v>
       </c>
       <c r="N365" s="18">
-        <v>44014</v>
+        <v>43943</v>
       </c>
       <c r="O365" s="18">
-        <v>44013</v>
+        <v>43939</v>
       </c>
       <c r="P365" s="19">
-        <v>44557</v>
+        <v>44304</v>
       </c>
       <c r="Q365" s="18">
-        <v>44192</v>
+        <v>44121</v>
       </c>
       <c r="R365" s="15" t="s">
-        <v>919</v>
+        <v>782</v>
       </c>
       <c r="S365" s="15" t="s">
-        <v>920</v>
+        <v>783</v>
       </c>
       <c r="T365" s="13" t="s">
         <v>33</v>
@@ -35775,51 +35737,51 @@
         <v>33</v>
       </c>
       <c r="V365" s="17">
-        <v>1.755897e6</v>
+        <v>804495</v>
       </c>
       <c r="W365" s="15" t="s">
-        <v>921</v>
+        <v>784</v>
       </c>
       <c r="X365" s="17">
         <v>2311</v>
       </c>
       <c r="Y365" s="15" t="s">
-        <v>908</v>
+        <v>916</v>
       </c>
       <c r="Z365" s="15" t="s">
-        <v>301</v>
+        <v>129</v>
       </c>
       <c r="AA365" s="13" t="s">
-        <v>911</v>
+        <v>919</v>
       </c>
       <c r="AB365" s="21">
-        <v>300</v>
+        <v>170</v>
       </c>
       <c r="AC365" s="22">
-        <v>950000e-6</v>
+        <v>45</v>
       </c>
       <c r="AD365" s="22">
-        <v>950000e-6</v>
+        <v>45</v>
       </c>
       <c r="AE365" s="23">
-        <v>285</v>
+        <v>7650</v>
       </c>
       <c r="AF365" s="23">
-        <v>285</v>
+        <v>7650</v>
       </c>
     </row>
     <row r="366" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A366" s="3" t="s">
-        <v>922</v>
+        <v>914</v>
       </c>
       <c r="B366" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C366" s="4">
-        <v>43966</v>
+        <v>43928</v>
       </c>
       <c r="D366" s="5" t="s">
-        <v>923</v>
+        <v>915</v>
       </c>
       <c r="E366" s="5" t="s">
         <v>33</v>
@@ -35828,7 +35790,7 @@
         <v>2310</v>
       </c>
       <c r="G366" s="3" t="s">
-        <v>908</v>
+        <v>916</v>
       </c>
       <c r="H366" s="3" t="s">
         <v>36</v>
@@ -35837,34 +35799,34 @@
         <v>37</v>
       </c>
       <c r="J366" s="7">
-        <v>9.253515e6</v>
+        <v>9.245982e6</v>
       </c>
       <c r="K366" s="5" t="s">
-        <v>924</v>
+        <v>917</v>
       </c>
       <c r="L366" s="7">
         <v>2310</v>
       </c>
       <c r="M366" s="5" t="s">
-        <v>908</v>
+        <v>916</v>
       </c>
       <c r="N366" s="8">
-        <v>44027</v>
+        <v>43943</v>
       </c>
       <c r="O366" s="8">
-        <v>44027</v>
+        <v>43939</v>
       </c>
       <c r="P366" s="9">
-        <v>44757</v>
+        <v>44304</v>
       </c>
       <c r="Q366" s="8">
-        <v>44206</v>
+        <v>44121</v>
       </c>
       <c r="R366" s="5" t="s">
-        <v>491</v>
+        <v>782</v>
       </c>
       <c r="S366" s="5" t="s">
-        <v>492</v>
+        <v>783</v>
       </c>
       <c r="T366" s="3" t="s">
         <v>33</v>
@@ -35873,51 +35835,51 @@
         <v>33</v>
       </c>
       <c r="V366" s="7">
-        <v>1.722859e6</v>
+        <v>1.129139e6</v>
       </c>
       <c r="W366" s="5" t="s">
-        <v>925</v>
+        <v>921</v>
       </c>
       <c r="X366" s="7">
         <v>2311</v>
       </c>
       <c r="Y366" s="5" t="s">
-        <v>908</v>
+        <v>916</v>
       </c>
       <c r="Z366" s="5" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="AA366" s="3" t="s">
-        <v>911</v>
+        <v>919</v>
       </c>
       <c r="AB366" s="10">
-        <v>50000</v>
+        <v>30</v>
       </c>
       <c r="AC366" s="11">
-        <v>2.68</v>
+        <v>45</v>
       </c>
       <c r="AD366" s="11">
-        <v>2.68</v>
+        <v>45</v>
       </c>
       <c r="AE366" s="12">
-        <v>134000</v>
+        <v>1350</v>
       </c>
       <c r="AF366" s="12">
-        <v>134000</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="367" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A367" s="13" t="s">
-        <v>922</v>
+        <v>914</v>
       </c>
       <c r="B367" s="13" t="s">
         <v>33</v>
       </c>
       <c r="C367" s="14">
-        <v>43966</v>
+        <v>43928</v>
       </c>
       <c r="D367" s="15" t="s">
-        <v>923</v>
+        <v>915</v>
       </c>
       <c r="E367" s="15" t="s">
         <v>33</v>
@@ -35926,7 +35888,7 @@
         <v>2310</v>
       </c>
       <c r="G367" s="13" t="s">
-        <v>908</v>
+        <v>916</v>
       </c>
       <c r="H367" s="13" t="s">
         <v>36</v>
@@ -35935,34 +35897,34 @@
         <v>37</v>
       </c>
       <c r="J367" s="17">
-        <v>9.253515e6</v>
+        <v>9.245982e6</v>
       </c>
       <c r="K367" s="15" t="s">
-        <v>924</v>
+        <v>917</v>
       </c>
       <c r="L367" s="17">
         <v>2310</v>
       </c>
       <c r="M367" s="15" t="s">
-        <v>908</v>
+        <v>916</v>
       </c>
       <c r="N367" s="18">
-        <v>44027</v>
+        <v>43943</v>
       </c>
       <c r="O367" s="18">
-        <v>44027</v>
+        <v>43939</v>
       </c>
       <c r="P367" s="19">
-        <v>44757</v>
+        <v>44304</v>
       </c>
       <c r="Q367" s="18">
-        <v>44206</v>
+        <v>44121</v>
       </c>
       <c r="R367" s="15" t="s">
-        <v>491</v>
+        <v>782</v>
       </c>
       <c r="S367" s="15" t="s">
-        <v>492</v>
+        <v>783</v>
       </c>
       <c r="T367" s="13" t="s">
         <v>33</v>
@@ -35971,51 +35933,51 @@
         <v>33</v>
       </c>
       <c r="V367" s="17">
-        <v>1.722891e6</v>
+        <v>1.152823e6</v>
       </c>
       <c r="W367" s="15" t="s">
-        <v>926</v>
+        <v>922</v>
       </c>
       <c r="X367" s="17">
         <v>2311</v>
       </c>
       <c r="Y367" s="15" t="s">
-        <v>908</v>
+        <v>916</v>
       </c>
       <c r="Z367" s="15" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="AA367" s="13" t="s">
-        <v>911</v>
+        <v>919</v>
       </c>
       <c r="AB367" s="21">
-        <v>20000</v>
+        <v>30</v>
       </c>
       <c r="AC367" s="22">
-        <v>440000e-6</v>
+        <v>45</v>
       </c>
       <c r="AD367" s="22">
-        <v>440000e-6</v>
+        <v>45</v>
       </c>
       <c r="AE367" s="23">
-        <v>8800</v>
+        <v>1350</v>
       </c>
       <c r="AF367" s="23">
-        <v>8800</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="368" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A368" s="3" t="s">
-        <v>922</v>
+        <v>914</v>
       </c>
       <c r="B368" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C368" s="4">
-        <v>43966</v>
+        <v>43928</v>
       </c>
       <c r="D368" s="5" t="s">
-        <v>923</v>
+        <v>915</v>
       </c>
       <c r="E368" s="5" t="s">
         <v>33</v>
@@ -36024,7 +35986,7 @@
         <v>2310</v>
       </c>
       <c r="G368" s="3" t="s">
-        <v>908</v>
+        <v>916</v>
       </c>
       <c r="H368" s="3" t="s">
         <v>36</v>
@@ -36033,34 +35995,34 @@
         <v>37</v>
       </c>
       <c r="J368" s="7">
-        <v>9.253532e6</v>
+        <v>9.245982e6</v>
       </c>
       <c r="K368" s="5" t="s">
-        <v>927</v>
+        <v>917</v>
       </c>
       <c r="L368" s="7">
         <v>2310</v>
       </c>
       <c r="M368" s="5" t="s">
-        <v>908</v>
+        <v>916</v>
       </c>
       <c r="N368" s="8">
-        <v>44027</v>
+        <v>43943</v>
       </c>
       <c r="O368" s="8">
-        <v>44027</v>
+        <v>43939</v>
       </c>
       <c r="P368" s="9">
-        <v>44757</v>
+        <v>44304</v>
       </c>
       <c r="Q368" s="8">
-        <v>44206</v>
+        <v>44121</v>
       </c>
       <c r="R368" s="5" t="s">
-        <v>928</v>
+        <v>782</v>
       </c>
       <c r="S368" s="5" t="s">
-        <v>929</v>
+        <v>783</v>
       </c>
       <c r="T368" s="3" t="s">
         <v>33</v>
@@ -36069,51 +36031,51 @@
         <v>33</v>
       </c>
       <c r="V368" s="7">
-        <v>1.043684e6</v>
+        <v>1.152831e6</v>
       </c>
       <c r="W368" s="5" t="s">
-        <v>930</v>
+        <v>923</v>
       </c>
       <c r="X368" s="7">
         <v>2311</v>
       </c>
       <c r="Y368" s="5" t="s">
-        <v>908</v>
+        <v>916</v>
       </c>
       <c r="Z368" s="5" t="s">
         <v>129</v>
       </c>
       <c r="AA368" s="3" t="s">
-        <v>911</v>
+        <v>919</v>
       </c>
       <c r="AB368" s="10">
-        <v>780</v>
+        <v>30</v>
       </c>
       <c r="AC368" s="11">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="AD368" s="11">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="AE368" s="12">
-        <v>19500</v>
+        <v>1350</v>
       </c>
       <c r="AF368" s="12">
-        <v>19500</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="369" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A369" s="13" t="s">
-        <v>931</v>
+        <v>924</v>
       </c>
       <c r="B369" s="13" t="s">
         <v>33</v>
       </c>
       <c r="C369" s="14">
-        <v>44001</v>
+        <v>43955</v>
       </c>
       <c r="D369" s="15" t="s">
-        <v>932</v>
+        <v>925</v>
       </c>
       <c r="E369" s="15" t="s">
         <v>33</v>
@@ -36122,7 +36084,7 @@
         <v>2310</v>
       </c>
       <c r="G369" s="13" t="s">
-        <v>908</v>
+        <v>916</v>
       </c>
       <c r="H369" s="13" t="s">
         <v>36</v>
@@ -36131,34 +36093,34 @@
         <v>37</v>
       </c>
       <c r="J369" s="17">
-        <v>9.253504e6</v>
+        <v>9.251383e6</v>
       </c>
       <c r="K369" s="15" t="s">
-        <v>933</v>
+        <v>926</v>
       </c>
       <c r="L369" s="17">
         <v>2310</v>
       </c>
       <c r="M369" s="15" t="s">
-        <v>908</v>
+        <v>916</v>
       </c>
       <c r="N369" s="18">
-        <v>44027</v>
+        <v>44014</v>
       </c>
       <c r="O369" s="18">
-        <v>44027</v>
+        <v>44013</v>
       </c>
       <c r="P369" s="19">
-        <v>44756</v>
+        <v>44557</v>
       </c>
       <c r="Q369" s="18">
-        <v>44206</v>
+        <v>44192</v>
       </c>
       <c r="R369" s="15" t="s">
-        <v>491</v>
+        <v>927</v>
       </c>
       <c r="S369" s="15" t="s">
-        <v>492</v>
+        <v>928</v>
       </c>
       <c r="T369" s="13" t="s">
         <v>33</v>
@@ -36167,60 +36129,60 @@
         <v>33</v>
       </c>
       <c r="V369" s="17">
-        <v>1.722905e6</v>
+        <v>1.755897e6</v>
       </c>
       <c r="W369" s="15" t="s">
-        <v>934</v>
+        <v>929</v>
       </c>
       <c r="X369" s="17">
         <v>2311</v>
       </c>
       <c r="Y369" s="15" t="s">
-        <v>908</v>
+        <v>916</v>
       </c>
       <c r="Z369" s="15" t="s">
-        <v>122</v>
+        <v>301</v>
       </c>
       <c r="AA369" s="13" t="s">
-        <v>911</v>
+        <v>919</v>
       </c>
       <c r="AB369" s="21">
-        <v>30000</v>
+        <v>300</v>
       </c>
       <c r="AC369" s="22">
-        <v>1.16</v>
+        <v>950000e-6</v>
       </c>
       <c r="AD369" s="22">
-        <v>1.16</v>
+        <v>950000e-6</v>
       </c>
       <c r="AE369" s="23">
-        <v>34800</v>
+        <v>285</v>
       </c>
       <c r="AF369" s="23">
-        <v>34800</v>
+        <v>285</v>
       </c>
     </row>
     <row r="370" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A370" s="3" t="s">
-        <v>935</v>
+        <v>930</v>
       </c>
       <c r="B370" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C370" s="4">
-        <v>43944</v>
-      </c>
-      <c r="D370" s="26" t="s">
-        <v>936</v>
+        <v>43966</v>
+      </c>
+      <c r="D370" s="5" t="s">
+        <v>931</v>
       </c>
       <c r="E370" s="5" t="s">
         <v>33</v>
       </c>
       <c r="F370" s="6">
-        <v>2320</v>
+        <v>2310</v>
       </c>
       <c r="G370" s="3" t="s">
-        <v>937</v>
+        <v>916</v>
       </c>
       <c r="H370" s="3" t="s">
         <v>36</v>
@@ -36229,20 +36191,34 @@
         <v>37</v>
       </c>
       <c r="J370" s="7">
-        <v>0</v>
-      </c>
-      <c r="K370" s="5"/>
-      <c r="L370" s="7"/>
-      <c r="M370" s="5"/>
-      <c r="N370" s="8"/>
-      <c r="O370" s="8"/>
-      <c r="P370" s="9"/>
-      <c r="Q370" s="8"/>
+        <v>9.253515e6</v>
+      </c>
+      <c r="K370" s="5" t="s">
+        <v>932</v>
+      </c>
+      <c r="L370" s="7">
+        <v>2310</v>
+      </c>
+      <c r="M370" s="5" t="s">
+        <v>916</v>
+      </c>
+      <c r="N370" s="8">
+        <v>44027</v>
+      </c>
+      <c r="O370" s="8">
+        <v>44027</v>
+      </c>
+      <c r="P370" s="9">
+        <v>44757</v>
+      </c>
+      <c r="Q370" s="8">
+        <v>44206</v>
+      </c>
       <c r="R370" s="5" t="s">
-        <v>938</v>
+        <v>491</v>
       </c>
       <c r="S370" s="5" t="s">
-        <v>939</v>
+        <v>492</v>
       </c>
       <c r="T370" s="3" t="s">
         <v>33</v>
@@ -36251,60 +36227,60 @@
         <v>33</v>
       </c>
       <c r="V370" s="7">
-        <v>1.692143e6</v>
+        <v>1.722859e6</v>
       </c>
       <c r="W370" s="5" t="s">
-        <v>510</v>
+        <v>933</v>
       </c>
       <c r="X370" s="7">
-        <v>2321</v>
+        <v>2311</v>
       </c>
       <c r="Y370" s="5" t="s">
-        <v>940</v>
+        <v>916</v>
       </c>
       <c r="Z370" s="5" t="s">
-        <v>307</v>
+        <v>122</v>
       </c>
       <c r="AA370" s="3" t="s">
-        <v>508</v>
+        <v>919</v>
       </c>
       <c r="AB370" s="10">
-        <v>3000</v>
+        <v>50000</v>
       </c>
       <c r="AC370" s="11">
-        <v>8.2</v>
+        <v>2.68</v>
       </c>
       <c r="AD370" s="11">
-        <v>8.2</v>
+        <v>2.68</v>
       </c>
       <c r="AE370" s="12">
-        <v>24600</v>
+        <v>134000</v>
       </c>
       <c r="AF370" s="12">
-        <v>24600</v>
+        <v>134000</v>
       </c>
     </row>
     <row r="371" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A371" s="13" t="s">
-        <v>935</v>
+        <v>930</v>
       </c>
       <c r="B371" s="13" t="s">
         <v>33</v>
       </c>
       <c r="C371" s="14">
-        <v>43944</v>
-      </c>
-      <c r="D371" s="25" t="s">
-        <v>936</v>
+        <v>43966</v>
+      </c>
+      <c r="D371" s="15" t="s">
+        <v>931</v>
       </c>
       <c r="E371" s="15" t="s">
         <v>33</v>
       </c>
       <c r="F371" s="16">
-        <v>2320</v>
+        <v>2310</v>
       </c>
       <c r="G371" s="13" t="s">
-        <v>937</v>
+        <v>916</v>
       </c>
       <c r="H371" s="13" t="s">
         <v>36</v>
@@ -36313,20 +36289,34 @@
         <v>37</v>
       </c>
       <c r="J371" s="17">
-        <v>0</v>
-      </c>
-      <c r="K371" s="15"/>
-      <c r="L371" s="17"/>
-      <c r="M371" s="15"/>
-      <c r="N371" s="18"/>
-      <c r="O371" s="18"/>
-      <c r="P371" s="19"/>
-      <c r="Q371" s="18"/>
+        <v>9.253515e6</v>
+      </c>
+      <c r="K371" s="15" t="s">
+        <v>932</v>
+      </c>
+      <c r="L371" s="17">
+        <v>2310</v>
+      </c>
+      <c r="M371" s="15" t="s">
+        <v>916</v>
+      </c>
+      <c r="N371" s="18">
+        <v>44027</v>
+      </c>
+      <c r="O371" s="18">
+        <v>44027</v>
+      </c>
+      <c r="P371" s="19">
+        <v>44757</v>
+      </c>
+      <c r="Q371" s="18">
+        <v>44206</v>
+      </c>
       <c r="R371" s="15" t="s">
-        <v>941</v>
+        <v>491</v>
       </c>
       <c r="S371" s="15" t="s">
-        <v>942</v>
+        <v>492</v>
       </c>
       <c r="T371" s="13" t="s">
         <v>33</v>
@@ -36335,60 +36325,60 @@
         <v>33</v>
       </c>
       <c r="V371" s="17">
-        <v>1.143883e6</v>
+        <v>1.722891e6</v>
       </c>
       <c r="W371" s="15" t="s">
-        <v>943</v>
+        <v>934</v>
       </c>
       <c r="X371" s="17">
-        <v>2321</v>
+        <v>2311</v>
       </c>
       <c r="Y371" s="15" t="s">
-        <v>940</v>
+        <v>916</v>
       </c>
       <c r="Z371" s="15" t="s">
-        <v>531</v>
+        <v>122</v>
       </c>
       <c r="AA371" s="13" t="s">
-        <v>508</v>
+        <v>919</v>
       </c>
       <c r="AB371" s="21">
-        <v>200000</v>
+        <v>20000</v>
       </c>
       <c r="AC371" s="22">
-        <v>600000e-6</v>
+        <v>440000e-6</v>
       </c>
       <c r="AD371" s="22">
-        <v>600000e-6</v>
+        <v>440000e-6</v>
       </c>
       <c r="AE371" s="23">
-        <v>120000</v>
+        <v>8800</v>
       </c>
       <c r="AF371" s="23">
-        <v>120000</v>
+        <v>8800</v>
       </c>
     </row>
     <row r="372" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A372" s="3" t="s">
-        <v>935</v>
+        <v>930</v>
       </c>
       <c r="B372" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C372" s="4">
-        <v>43944</v>
-      </c>
-      <c r="D372" s="26" t="s">
-        <v>936</v>
+        <v>43966</v>
+      </c>
+      <c r="D372" s="5" t="s">
+        <v>931</v>
       </c>
       <c r="E372" s="5" t="s">
         <v>33</v>
       </c>
       <c r="F372" s="6">
-        <v>2320</v>
+        <v>2310</v>
       </c>
       <c r="G372" s="3" t="s">
-        <v>937</v>
+        <v>916</v>
       </c>
       <c r="H372" s="3" t="s">
         <v>36</v>
@@ -36397,20 +36387,34 @@
         <v>37</v>
       </c>
       <c r="J372" s="7">
-        <v>0</v>
-      </c>
-      <c r="K372" s="5"/>
-      <c r="L372" s="7"/>
-      <c r="M372" s="5"/>
-      <c r="N372" s="8"/>
-      <c r="O372" s="8"/>
-      <c r="P372" s="9"/>
-      <c r="Q372" s="8"/>
+        <v>9.253532e6</v>
+      </c>
+      <c r="K372" s="5" t="s">
+        <v>935</v>
+      </c>
+      <c r="L372" s="7">
+        <v>2310</v>
+      </c>
+      <c r="M372" s="5" t="s">
+        <v>916</v>
+      </c>
+      <c r="N372" s="8">
+        <v>44027</v>
+      </c>
+      <c r="O372" s="8">
+        <v>44027</v>
+      </c>
+      <c r="P372" s="9">
+        <v>44757</v>
+      </c>
+      <c r="Q372" s="8">
+        <v>44206</v>
+      </c>
       <c r="R372" s="5" t="s">
-        <v>944</v>
+        <v>936</v>
       </c>
       <c r="S372" s="5" t="s">
-        <v>945</v>
+        <v>937</v>
       </c>
       <c r="T372" s="3" t="s">
         <v>33</v>
@@ -36419,60 +36423,60 @@
         <v>33</v>
       </c>
       <c r="V372" s="7">
-        <v>1.244515e6</v>
+        <v>1.043684e6</v>
       </c>
       <c r="W372" s="5" t="s">
-        <v>946</v>
+        <v>938</v>
       </c>
       <c r="X372" s="7">
-        <v>2321</v>
+        <v>2311</v>
       </c>
       <c r="Y372" s="5" t="s">
-        <v>940</v>
+        <v>916</v>
       </c>
       <c r="Z372" s="5" t="s">
-        <v>531</v>
+        <v>129</v>
       </c>
       <c r="AA372" s="3" t="s">
-        <v>508</v>
+        <v>919</v>
       </c>
       <c r="AB372" s="10">
-        <v>50</v>
+        <v>780</v>
       </c>
       <c r="AC372" s="11">
-        <v>20.1</v>
+        <v>25</v>
       </c>
       <c r="AD372" s="11">
-        <v>20.1</v>
+        <v>25</v>
       </c>
       <c r="AE372" s="12">
-        <v>1005</v>
+        <v>19500</v>
       </c>
       <c r="AF372" s="12">
-        <v>1005</v>
+        <v>19500</v>
       </c>
     </row>
     <row r="373" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A373" s="13" t="s">
-        <v>935</v>
+        <v>939</v>
       </c>
       <c r="B373" s="13" t="s">
         <v>33</v>
       </c>
       <c r="C373" s="14">
-        <v>43944</v>
-      </c>
-      <c r="D373" s="25" t="s">
-        <v>936</v>
+        <v>44001</v>
+      </c>
+      <c r="D373" s="15" t="s">
+        <v>940</v>
       </c>
       <c r="E373" s="15" t="s">
         <v>33</v>
       </c>
       <c r="F373" s="16">
-        <v>2320</v>
+        <v>2310</v>
       </c>
       <c r="G373" s="13" t="s">
-        <v>937</v>
+        <v>916</v>
       </c>
       <c r="H373" s="13" t="s">
         <v>36</v>
@@ -36481,20 +36485,34 @@
         <v>37</v>
       </c>
       <c r="J373" s="17">
-        <v>0</v>
-      </c>
-      <c r="K373" s="15"/>
-      <c r="L373" s="17"/>
-      <c r="M373" s="15"/>
-      <c r="N373" s="18"/>
-      <c r="O373" s="18"/>
-      <c r="P373" s="19"/>
-      <c r="Q373" s="18"/>
+        <v>9.253504e6</v>
+      </c>
+      <c r="K373" s="15" t="s">
+        <v>941</v>
+      </c>
+      <c r="L373" s="17">
+        <v>2310</v>
+      </c>
+      <c r="M373" s="15" t="s">
+        <v>916</v>
+      </c>
+      <c r="N373" s="18">
+        <v>44027</v>
+      </c>
+      <c r="O373" s="18">
+        <v>44027</v>
+      </c>
+      <c r="P373" s="19">
+        <v>44756</v>
+      </c>
+      <c r="Q373" s="18">
+        <v>44206</v>
+      </c>
       <c r="R373" s="15" t="s">
-        <v>947</v>
+        <v>491</v>
       </c>
       <c r="S373" s="15" t="s">
-        <v>948</v>
+        <v>492</v>
       </c>
       <c r="T373" s="13" t="s">
         <v>33</v>
@@ -36503,42 +36521,42 @@
         <v>33</v>
       </c>
       <c r="V373" s="17">
-        <v>1.244108e6</v>
+        <v>1.722905e6</v>
       </c>
       <c r="W373" s="15" t="s">
-        <v>949</v>
+        <v>942</v>
       </c>
       <c r="X373" s="17">
-        <v>2321</v>
+        <v>2311</v>
       </c>
       <c r="Y373" s="15" t="s">
-        <v>940</v>
+        <v>916</v>
       </c>
       <c r="Z373" s="15" t="s">
-        <v>531</v>
+        <v>122</v>
       </c>
       <c r="AA373" s="13" t="s">
-        <v>508</v>
+        <v>919</v>
       </c>
       <c r="AB373" s="21">
-        <v>90</v>
+        <v>30000</v>
       </c>
       <c r="AC373" s="22">
-        <v>358.24</v>
+        <v>1.16</v>
       </c>
       <c r="AD373" s="22">
-        <v>358.24</v>
+        <v>1.16</v>
       </c>
       <c r="AE373" s="23">
-        <v>32241.6</v>
+        <v>34800</v>
       </c>
       <c r="AF373" s="23">
-        <v>32241.6</v>
+        <v>34800</v>
       </c>
     </row>
     <row r="374" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A374" s="3" t="s">
-        <v>935</v>
+        <v>943</v>
       </c>
       <c r="B374" s="3" t="s">
         <v>33</v>
@@ -36547,7 +36565,7 @@
         <v>43944</v>
       </c>
       <c r="D374" s="26" t="s">
-        <v>936</v>
+        <v>944</v>
       </c>
       <c r="E374" s="5" t="s">
         <v>33</v>
@@ -36556,7 +36574,7 @@
         <v>2320</v>
       </c>
       <c r="G374" s="3" t="s">
-        <v>937</v>
+        <v>945</v>
       </c>
       <c r="H374" s="3" t="s">
         <v>36</v>
@@ -36575,11 +36593,11 @@
       <c r="P374" s="9"/>
       <c r="Q374" s="8"/>
       <c r="R374" s="5" t="s">
+        <v>946</v>
+      </c>
+      <c r="S374" s="5" t="s">
         <v>947</v>
       </c>
-      <c r="S374" s="5" t="s">
-        <v>948</v>
-      </c>
       <c r="T374" s="3" t="s">
         <v>33</v>
       </c>
@@ -36587,42 +36605,42 @@
         <v>33</v>
       </c>
       <c r="V374" s="7">
-        <v>1.244507e6</v>
+        <v>1.692143e6</v>
       </c>
       <c r="W374" s="5" t="s">
-        <v>950</v>
+        <v>510</v>
       </c>
       <c r="X374" s="7">
         <v>2321</v>
       </c>
       <c r="Y374" s="5" t="s">
-        <v>940</v>
+        <v>948</v>
       </c>
       <c r="Z374" s="5" t="s">
-        <v>531</v>
+        <v>307</v>
       </c>
       <c r="AA374" s="3" t="s">
         <v>508</v>
       </c>
       <c r="AB374" s="10">
-        <v>50</v>
+        <v>3000</v>
       </c>
       <c r="AC374" s="11">
-        <v>34.9</v>
+        <v>8.2</v>
       </c>
       <c r="AD374" s="11">
-        <v>34.9</v>
+        <v>8.2</v>
       </c>
       <c r="AE374" s="12">
-        <v>1745</v>
+        <v>24600</v>
       </c>
       <c r="AF374" s="12">
-        <v>1745</v>
+        <v>24600</v>
       </c>
     </row>
     <row r="375" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A375" s="13" t="s">
-        <v>935</v>
+        <v>943</v>
       </c>
       <c r="B375" s="13" t="s">
         <v>33</v>
@@ -36631,7 +36649,7 @@
         <v>43944</v>
       </c>
       <c r="D375" s="25" t="s">
-        <v>936</v>
+        <v>944</v>
       </c>
       <c r="E375" s="15" t="s">
         <v>33</v>
@@ -36640,7 +36658,7 @@
         <v>2320</v>
       </c>
       <c r="G375" s="13" t="s">
-        <v>937</v>
+        <v>945</v>
       </c>
       <c r="H375" s="13" t="s">
         <v>36</v>
@@ -36659,10 +36677,10 @@
       <c r="P375" s="19"/>
       <c r="Q375" s="18"/>
       <c r="R375" s="15" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="S375" s="15" t="s">
-        <v>948</v>
+        <v>950</v>
       </c>
       <c r="T375" s="13" t="s">
         <v>33</v>
@@ -36671,7 +36689,7 @@
         <v>33</v>
       </c>
       <c r="V375" s="17">
-        <v>1.257587e6</v>
+        <v>1.143883e6</v>
       </c>
       <c r="W375" s="15" t="s">
         <v>951</v>
@@ -36680,7 +36698,7 @@
         <v>2321</v>
       </c>
       <c r="Y375" s="15" t="s">
-        <v>940</v>
+        <v>948</v>
       </c>
       <c r="Z375" s="15" t="s">
         <v>531</v>
@@ -36689,24 +36707,24 @@
         <v>508</v>
       </c>
       <c r="AB375" s="21">
-        <v>80000</v>
+        <v>200000</v>
       </c>
       <c r="AC375" s="22">
-        <v>390000e-6</v>
+        <v>600000e-6</v>
       </c>
       <c r="AD375" s="22">
-        <v>390000e-6</v>
+        <v>600000e-6</v>
       </c>
       <c r="AE375" s="23">
-        <v>31200</v>
+        <v>120000</v>
       </c>
       <c r="AF375" s="23">
-        <v>31200</v>
+        <v>120000</v>
       </c>
     </row>
     <row r="376" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A376" s="3" t="s">
-        <v>935</v>
+        <v>943</v>
       </c>
       <c r="B376" s="3" t="s">
         <v>33</v>
@@ -36715,7 +36733,7 @@
         <v>43944</v>
       </c>
       <c r="D376" s="26" t="s">
-        <v>936</v>
+        <v>944</v>
       </c>
       <c r="E376" s="5" t="s">
         <v>33</v>
@@ -36724,7 +36742,7 @@
         <v>2320</v>
       </c>
       <c r="G376" s="3" t="s">
-        <v>937</v>
+        <v>945</v>
       </c>
       <c r="H376" s="3" t="s">
         <v>36</v>
@@ -36743,10 +36761,10 @@
       <c r="P376" s="9"/>
       <c r="Q376" s="8"/>
       <c r="R376" s="5" t="s">
-        <v>947</v>
+        <v>860</v>
       </c>
       <c r="S376" s="5" t="s">
-        <v>948</v>
+        <v>861</v>
       </c>
       <c r="T376" s="3" t="s">
         <v>33</v>
@@ -36755,7 +36773,7 @@
         <v>33</v>
       </c>
       <c r="V376" s="7">
-        <v>1.257625e6</v>
+        <v>1.244515e6</v>
       </c>
       <c r="W376" s="5" t="s">
         <v>952</v>
@@ -36764,33 +36782,33 @@
         <v>2321</v>
       </c>
       <c r="Y376" s="5" t="s">
-        <v>940</v>
+        <v>948</v>
       </c>
       <c r="Z376" s="5" t="s">
-        <v>379</v>
+        <v>531</v>
       </c>
       <c r="AA376" s="3" t="s">
         <v>508</v>
       </c>
       <c r="AB376" s="10">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="AC376" s="11">
-        <v>351</v>
+        <v>20.1</v>
       </c>
       <c r="AD376" s="11">
-        <v>351</v>
+        <v>20.1</v>
       </c>
       <c r="AE376" s="12">
-        <v>31590</v>
+        <v>1005</v>
       </c>
       <c r="AF376" s="12">
-        <v>31590</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="377" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A377" s="13" t="s">
-        <v>935</v>
+        <v>943</v>
       </c>
       <c r="B377" s="13" t="s">
         <v>33</v>
@@ -36799,7 +36817,7 @@
         <v>43944</v>
       </c>
       <c r="D377" s="25" t="s">
-        <v>936</v>
+        <v>944</v>
       </c>
       <c r="E377" s="15" t="s">
         <v>33</v>
@@ -36808,7 +36826,7 @@
         <v>2320</v>
       </c>
       <c r="G377" s="13" t="s">
-        <v>937</v>
+        <v>945</v>
       </c>
       <c r="H377" s="13" t="s">
         <v>36</v>
@@ -36827,10 +36845,10 @@
       <c r="P377" s="19"/>
       <c r="Q377" s="18"/>
       <c r="R377" s="15" t="s">
-        <v>947</v>
+        <v>953</v>
       </c>
       <c r="S377" s="15" t="s">
-        <v>948</v>
+        <v>954</v>
       </c>
       <c r="T377" s="13" t="s">
         <v>33</v>
@@ -36839,16 +36857,16 @@
         <v>33</v>
       </c>
       <c r="V377" s="17">
-        <v>1.258699e6</v>
+        <v>1.244108e6</v>
       </c>
       <c r="W377" s="15" t="s">
-        <v>953</v>
+        <v>955</v>
       </c>
       <c r="X377" s="17">
         <v>2321</v>
       </c>
       <c r="Y377" s="15" t="s">
-        <v>940</v>
+        <v>948</v>
       </c>
       <c r="Z377" s="15" t="s">
         <v>531</v>
@@ -36857,24 +36875,24 @@
         <v>508</v>
       </c>
       <c r="AB377" s="21">
-        <v>2000</v>
+        <v>90</v>
       </c>
       <c r="AC377" s="22">
-        <v>1.39</v>
+        <v>358.24</v>
       </c>
       <c r="AD377" s="22">
-        <v>1.39</v>
+        <v>358.24</v>
       </c>
       <c r="AE377" s="23">
-        <v>2780</v>
+        <v>32241.6</v>
       </c>
       <c r="AF377" s="23">
-        <v>2780</v>
+        <v>32241.6</v>
       </c>
     </row>
     <row r="378" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A378" s="3" t="s">
-        <v>935</v>
+        <v>943</v>
       </c>
       <c r="B378" s="3" t="s">
         <v>33</v>
@@ -36883,7 +36901,7 @@
         <v>43944</v>
       </c>
       <c r="D378" s="26" t="s">
-        <v>936</v>
+        <v>944</v>
       </c>
       <c r="E378" s="5" t="s">
         <v>33</v>
@@ -36892,7 +36910,7 @@
         <v>2320</v>
       </c>
       <c r="G378" s="3" t="s">
-        <v>937</v>
+        <v>945</v>
       </c>
       <c r="H378" s="3" t="s">
         <v>36</v>
@@ -36911,10 +36929,10 @@
       <c r="P378" s="9"/>
       <c r="Q378" s="8"/>
       <c r="R378" s="5" t="s">
-        <v>947</v>
+        <v>953</v>
       </c>
       <c r="S378" s="5" t="s">
-        <v>948</v>
+        <v>954</v>
       </c>
       <c r="T378" s="3" t="s">
         <v>33</v>
@@ -36923,16 +36941,16 @@
         <v>33</v>
       </c>
       <c r="V378" s="7">
-        <v>1.259784e6</v>
+        <v>1.244507e6</v>
       </c>
       <c r="W378" s="5" t="s">
-        <v>954</v>
+        <v>956</v>
       </c>
       <c r="X378" s="7">
         <v>2321</v>
       </c>
       <c r="Y378" s="5" t="s">
-        <v>940</v>
+        <v>948</v>
       </c>
       <c r="Z378" s="5" t="s">
         <v>531</v>
@@ -36941,24 +36959,24 @@
         <v>508</v>
       </c>
       <c r="AB378" s="10">
-        <v>3000</v>
+        <v>50</v>
       </c>
       <c r="AC378" s="11">
-        <v>600000e-6</v>
+        <v>34.9</v>
       </c>
       <c r="AD378" s="11">
-        <v>600000e-6</v>
+        <v>34.9</v>
       </c>
       <c r="AE378" s="12">
-        <v>1800</v>
+        <v>1745</v>
       </c>
       <c r="AF378" s="12">
-        <v>1800</v>
+        <v>1745</v>
       </c>
     </row>
     <row r="379" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A379" s="13" t="s">
-        <v>935</v>
+        <v>943</v>
       </c>
       <c r="B379" s="13" t="s">
         <v>33</v>
@@ -36967,7 +36985,7 @@
         <v>43944</v>
       </c>
       <c r="D379" s="25" t="s">
-        <v>936</v>
+        <v>944</v>
       </c>
       <c r="E379" s="15" t="s">
         <v>33</v>
@@ -36976,7 +36994,7 @@
         <v>2320</v>
       </c>
       <c r="G379" s="13" t="s">
-        <v>937</v>
+        <v>945</v>
       </c>
       <c r="H379" s="13" t="s">
         <v>36</v>
@@ -36995,10 +37013,10 @@
       <c r="P379" s="19"/>
       <c r="Q379" s="18"/>
       <c r="R379" s="15" t="s">
-        <v>947</v>
+        <v>953</v>
       </c>
       <c r="S379" s="15" t="s">
-        <v>948</v>
+        <v>954</v>
       </c>
       <c r="T379" s="13" t="s">
         <v>33</v>
@@ -37007,16 +37025,16 @@
         <v>33</v>
       </c>
       <c r="V379" s="17">
-        <v>1.259792e6</v>
+        <v>1.257587e6</v>
       </c>
       <c r="W379" s="15" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="X379" s="17">
         <v>2321</v>
       </c>
       <c r="Y379" s="15" t="s">
-        <v>940</v>
+        <v>948</v>
       </c>
       <c r="Z379" s="15" t="s">
         <v>531</v>
@@ -37025,24 +37043,24 @@
         <v>508</v>
       </c>
       <c r="AB379" s="21">
-        <v>80</v>
+        <v>80000</v>
       </c>
       <c r="AC379" s="22">
-        <v>15.35</v>
+        <v>390000e-6</v>
       </c>
       <c r="AD379" s="22">
-        <v>15.35</v>
+        <v>390000e-6</v>
       </c>
       <c r="AE379" s="23">
-        <v>1228</v>
+        <v>31200</v>
       </c>
       <c r="AF379" s="23">
-        <v>1228</v>
+        <v>31200</v>
       </c>
     </row>
     <row r="380" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A380" s="3" t="s">
-        <v>935</v>
+        <v>943</v>
       </c>
       <c r="B380" s="3" t="s">
         <v>33</v>
@@ -37051,7 +37069,7 @@
         <v>43944</v>
       </c>
       <c r="D380" s="26" t="s">
-        <v>936</v>
+        <v>944</v>
       </c>
       <c r="E380" s="5" t="s">
         <v>33</v>
@@ -37060,7 +37078,7 @@
         <v>2320</v>
       </c>
       <c r="G380" s="3" t="s">
-        <v>937</v>
+        <v>945</v>
       </c>
       <c r="H380" s="3" t="s">
         <v>36</v>
@@ -37079,10 +37097,10 @@
       <c r="P380" s="9"/>
       <c r="Q380" s="8"/>
       <c r="R380" s="5" t="s">
-        <v>947</v>
+        <v>953</v>
       </c>
       <c r="S380" s="5" t="s">
-        <v>948</v>
+        <v>954</v>
       </c>
       <c r="T380" s="3" t="s">
         <v>33</v>
@@ -37091,42 +37109,42 @@
         <v>33</v>
       </c>
       <c r="V380" s="7">
-        <v>1.260669e6</v>
+        <v>1.257625e6</v>
       </c>
       <c r="W380" s="5" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="X380" s="7">
         <v>2321</v>
       </c>
       <c r="Y380" s="5" t="s">
-        <v>940</v>
+        <v>948</v>
       </c>
       <c r="Z380" s="5" t="s">
-        <v>531</v>
+        <v>379</v>
       </c>
       <c r="AA380" s="3" t="s">
         <v>508</v>
       </c>
       <c r="AB380" s="10">
-        <v>1000</v>
+        <v>90</v>
       </c>
       <c r="AC380" s="11">
-        <v>1.49</v>
+        <v>351</v>
       </c>
       <c r="AD380" s="11">
-        <v>1.49</v>
+        <v>351</v>
       </c>
       <c r="AE380" s="12">
-        <v>1490</v>
+        <v>31590</v>
       </c>
       <c r="AF380" s="12">
-        <v>1490</v>
+        <v>31590</v>
       </c>
     </row>
     <row r="381" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A381" s="13" t="s">
-        <v>935</v>
+        <v>943</v>
       </c>
       <c r="B381" s="13" t="s">
         <v>33</v>
@@ -37135,7 +37153,7 @@
         <v>43944</v>
       </c>
       <c r="D381" s="25" t="s">
-        <v>936</v>
+        <v>944</v>
       </c>
       <c r="E381" s="15" t="s">
         <v>33</v>
@@ -37144,7 +37162,7 @@
         <v>2320</v>
       </c>
       <c r="G381" s="13" t="s">
-        <v>937</v>
+        <v>945</v>
       </c>
       <c r="H381" s="13" t="s">
         <v>36</v>
@@ -37163,10 +37181,10 @@
       <c r="P381" s="19"/>
       <c r="Q381" s="18"/>
       <c r="R381" s="15" t="s">
-        <v>947</v>
+        <v>953</v>
       </c>
       <c r="S381" s="15" t="s">
-        <v>948</v>
+        <v>954</v>
       </c>
       <c r="T381" s="13" t="s">
         <v>33</v>
@@ -37175,16 +37193,16 @@
         <v>33</v>
       </c>
       <c r="V381" s="17">
-        <v>1.260677e6</v>
+        <v>1.258699e6</v>
       </c>
       <c r="W381" s="15" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="X381" s="17">
         <v>2321</v>
       </c>
       <c r="Y381" s="15" t="s">
-        <v>940</v>
+        <v>948</v>
       </c>
       <c r="Z381" s="15" t="s">
         <v>531</v>
@@ -37193,24 +37211,24 @@
         <v>508</v>
       </c>
       <c r="AB381" s="21">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="AC381" s="22">
-        <v>1.59</v>
+        <v>1.39</v>
       </c>
       <c r="AD381" s="22">
-        <v>1.59</v>
+        <v>1.39</v>
       </c>
       <c r="AE381" s="23">
-        <v>4770</v>
+        <v>2780</v>
       </c>
       <c r="AF381" s="23">
-        <v>4770</v>
+        <v>2780</v>
       </c>
     </row>
     <row r="382" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A382" s="3" t="s">
-        <v>935</v>
+        <v>943</v>
       </c>
       <c r="B382" s="3" t="s">
         <v>33</v>
@@ -37219,7 +37237,7 @@
         <v>43944</v>
       </c>
       <c r="D382" s="26" t="s">
-        <v>936</v>
+        <v>944</v>
       </c>
       <c r="E382" s="5" t="s">
         <v>33</v>
@@ -37228,7 +37246,7 @@
         <v>2320</v>
       </c>
       <c r="G382" s="3" t="s">
-        <v>937</v>
+        <v>945</v>
       </c>
       <c r="H382" s="3" t="s">
         <v>36</v>
@@ -37247,10 +37265,10 @@
       <c r="P382" s="9"/>
       <c r="Q382" s="8"/>
       <c r="R382" s="5" t="s">
-        <v>947</v>
+        <v>953</v>
       </c>
       <c r="S382" s="5" t="s">
-        <v>948</v>
+        <v>954</v>
       </c>
       <c r="T382" s="3" t="s">
         <v>33</v>
@@ -37259,16 +37277,16 @@
         <v>33</v>
       </c>
       <c r="V382" s="7">
-        <v>1.260731e6</v>
-      </c>
-      <c r="W382" s="24" t="s">
-        <v>958</v>
+        <v>1.259784e6</v>
+      </c>
+      <c r="W382" s="5" t="s">
+        <v>960</v>
       </c>
       <c r="X382" s="7">
         <v>2321</v>
       </c>
       <c r="Y382" s="5" t="s">
-        <v>940</v>
+        <v>948</v>
       </c>
       <c r="Z382" s="5" t="s">
         <v>531</v>
@@ -37277,24 +37295,24 @@
         <v>508</v>
       </c>
       <c r="AB382" s="10">
-        <v>60</v>
+        <v>3000</v>
       </c>
       <c r="AC382" s="11">
-        <v>271.97</v>
+        <v>600000e-6</v>
       </c>
       <c r="AD382" s="11">
-        <v>271.97</v>
+        <v>600000e-6</v>
       </c>
       <c r="AE382" s="12">
-        <v>16318.2</v>
+        <v>1800</v>
       </c>
       <c r="AF382" s="12">
-        <v>16318.2</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="383" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A383" s="13" t="s">
-        <v>935</v>
+        <v>943</v>
       </c>
       <c r="B383" s="13" t="s">
         <v>33</v>
@@ -37303,7 +37321,7 @@
         <v>43944</v>
       </c>
       <c r="D383" s="25" t="s">
-        <v>936</v>
+        <v>944</v>
       </c>
       <c r="E383" s="15" t="s">
         <v>33</v>
@@ -37312,7 +37330,7 @@
         <v>2320</v>
       </c>
       <c r="G383" s="13" t="s">
-        <v>937</v>
+        <v>945</v>
       </c>
       <c r="H383" s="13" t="s">
         <v>36</v>
@@ -37331,10 +37349,10 @@
       <c r="P383" s="19"/>
       <c r="Q383" s="18"/>
       <c r="R383" s="15" t="s">
-        <v>947</v>
+        <v>953</v>
       </c>
       <c r="S383" s="15" t="s">
-        <v>948</v>
+        <v>954</v>
       </c>
       <c r="T383" s="13" t="s">
         <v>33</v>
@@ -37343,16 +37361,16 @@
         <v>33</v>
       </c>
       <c r="V383" s="17">
-        <v>1.687115e6</v>
+        <v>1.259792e6</v>
       </c>
       <c r="W383" s="15" t="s">
-        <v>959</v>
+        <v>961</v>
       </c>
       <c r="X383" s="17">
         <v>2321</v>
       </c>
       <c r="Y383" s="15" t="s">
-        <v>940</v>
+        <v>948</v>
       </c>
       <c r="Z383" s="15" t="s">
         <v>531</v>
@@ -37361,24 +37379,24 @@
         <v>508</v>
       </c>
       <c r="AB383" s="21">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="AC383" s="22">
-        <v>16.65</v>
+        <v>15.35</v>
       </c>
       <c r="AD383" s="22">
-        <v>16.65</v>
+        <v>15.35</v>
       </c>
       <c r="AE383" s="23">
-        <v>999</v>
+        <v>1228</v>
       </c>
       <c r="AF383" s="23">
-        <v>999</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="384" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A384" s="3" t="s">
-        <v>935</v>
+        <v>943</v>
       </c>
       <c r="B384" s="3" t="s">
         <v>33</v>
@@ -37387,7 +37405,7 @@
         <v>43944</v>
       </c>
       <c r="D384" s="26" t="s">
-        <v>936</v>
+        <v>944</v>
       </c>
       <c r="E384" s="5" t="s">
         <v>33</v>
@@ -37396,7 +37414,7 @@
         <v>2320</v>
       </c>
       <c r="G384" s="3" t="s">
-        <v>937</v>
+        <v>945</v>
       </c>
       <c r="H384" s="3" t="s">
         <v>36</v>
@@ -37415,10 +37433,10 @@
       <c r="P384" s="9"/>
       <c r="Q384" s="8"/>
       <c r="R384" s="5" t="s">
-        <v>960</v>
+        <v>953</v>
       </c>
       <c r="S384" s="5" t="s">
-        <v>961</v>
+        <v>954</v>
       </c>
       <c r="T384" s="3" t="s">
         <v>33</v>
@@ -37427,7 +37445,7 @@
         <v>33</v>
       </c>
       <c r="V384" s="7">
-        <v>1.257463e6</v>
+        <v>1.260669e6</v>
       </c>
       <c r="W384" s="5" t="s">
         <v>962</v>
@@ -37436,7 +37454,7 @@
         <v>2321</v>
       </c>
       <c r="Y384" s="5" t="s">
-        <v>940</v>
+        <v>948</v>
       </c>
       <c r="Z384" s="5" t="s">
         <v>531</v>
@@ -37445,33 +37463,33 @@
         <v>508</v>
       </c>
       <c r="AB384" s="10">
-        <v>200</v>
+        <v>1000</v>
       </c>
       <c r="AC384" s="11">
-        <v>34.2</v>
+        <v>1.49</v>
       </c>
       <c r="AD384" s="11">
-        <v>34.2</v>
+        <v>1.49</v>
       </c>
       <c r="AE384" s="12">
-        <v>6840</v>
+        <v>1490</v>
       </c>
       <c r="AF384" s="12">
-        <v>6840</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="385" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A385" s="13" t="s">
-        <v>963</v>
+        <v>943</v>
       </c>
       <c r="B385" s="13" t="s">
         <v>33</v>
       </c>
       <c r="C385" s="14">
-        <v>44012</v>
-      </c>
-      <c r="D385" s="15" t="s">
-        <v>964</v>
+        <v>43944</v>
+      </c>
+      <c r="D385" s="25" t="s">
+        <v>944</v>
       </c>
       <c r="E385" s="15" t="s">
         <v>33</v>
@@ -37480,7 +37498,7 @@
         <v>2320</v>
       </c>
       <c r="G385" s="13" t="s">
-        <v>937</v>
+        <v>945</v>
       </c>
       <c r="H385" s="13" t="s">
         <v>36</v>
@@ -37499,10 +37517,10 @@
       <c r="P385" s="19"/>
       <c r="Q385" s="18"/>
       <c r="R385" s="15" t="s">
-        <v>491</v>
+        <v>953</v>
       </c>
       <c r="S385" s="15" t="s">
-        <v>492</v>
+        <v>954</v>
       </c>
       <c r="T385" s="13" t="s">
         <v>33</v>
@@ -37511,40 +37529,376 @@
         <v>33</v>
       </c>
       <c r="V385" s="17">
-        <v>1.408623e6</v>
+        <v>1.260677e6</v>
       </c>
       <c r="W385" s="15" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="X385" s="17">
         <v>2321</v>
       </c>
       <c r="Y385" s="15" t="s">
-        <v>940</v>
+        <v>948</v>
       </c>
       <c r="Z385" s="15" t="s">
-        <v>373</v>
+        <v>531</v>
       </c>
       <c r="AA385" s="13" t="s">
         <v>508</v>
       </c>
       <c r="AB385" s="21">
+        <v>3000</v>
+      </c>
+      <c r="AC385" s="22">
+        <v>1.59</v>
+      </c>
+      <c r="AD385" s="22">
+        <v>1.59</v>
+      </c>
+      <c r="AE385" s="23">
+        <v>4770</v>
+      </c>
+      <c r="AF385" s="23">
+        <v>4770</v>
+      </c>
+    </row>
+    <row r="386" s="1" customFormat="1" ht="18.1322" customHeight="1">
+      <c r="A386" s="3" t="s">
+        <v>943</v>
+      </c>
+      <c r="B386" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C386" s="4">
+        <v>43944</v>
+      </c>
+      <c r="D386" s="26" t="s">
+        <v>944</v>
+      </c>
+      <c r="E386" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F386" s="6">
+        <v>2320</v>
+      </c>
+      <c r="G386" s="3" t="s">
+        <v>945</v>
+      </c>
+      <c r="H386" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I386" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J386" s="7">
+        <v>0</v>
+      </c>
+      <c r="K386" s="5"/>
+      <c r="L386" s="7"/>
+      <c r="M386" s="5"/>
+      <c r="N386" s="8"/>
+      <c r="O386" s="8"/>
+      <c r="P386" s="9"/>
+      <c r="Q386" s="8"/>
+      <c r="R386" s="5" t="s">
+        <v>953</v>
+      </c>
+      <c r="S386" s="5" t="s">
+        <v>954</v>
+      </c>
+      <c r="T386" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U386" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="V386" s="7">
+        <v>1.260731e6</v>
+      </c>
+      <c r="W386" s="24" t="s">
+        <v>964</v>
+      </c>
+      <c r="X386" s="7">
+        <v>2321</v>
+      </c>
+      <c r="Y386" s="5" t="s">
+        <v>948</v>
+      </c>
+      <c r="Z386" s="5" t="s">
+        <v>531</v>
+      </c>
+      <c r="AA386" s="3" t="s">
+        <v>508</v>
+      </c>
+      <c r="AB386" s="10">
+        <v>60</v>
+      </c>
+      <c r="AC386" s="11">
+        <v>271.97</v>
+      </c>
+      <c r="AD386" s="11">
+        <v>271.97</v>
+      </c>
+      <c r="AE386" s="12">
+        <v>16318.2</v>
+      </c>
+      <c r="AF386" s="12">
+        <v>16318.2</v>
+      </c>
+    </row>
+    <row r="387" s="1" customFormat="1" ht="18.1322" customHeight="1">
+      <c r="A387" s="13" t="s">
+        <v>943</v>
+      </c>
+      <c r="B387" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C387" s="14">
+        <v>43944</v>
+      </c>
+      <c r="D387" s="25" t="s">
+        <v>944</v>
+      </c>
+      <c r="E387" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F387" s="16">
+        <v>2320</v>
+      </c>
+      <c r="G387" s="13" t="s">
+        <v>945</v>
+      </c>
+      <c r="H387" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I387" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="J387" s="17">
+        <v>0</v>
+      </c>
+      <c r="K387" s="15"/>
+      <c r="L387" s="17"/>
+      <c r="M387" s="15"/>
+      <c r="N387" s="18"/>
+      <c r="O387" s="18"/>
+      <c r="P387" s="19"/>
+      <c r="Q387" s="18"/>
+      <c r="R387" s="15" t="s">
+        <v>953</v>
+      </c>
+      <c r="S387" s="15" t="s">
+        <v>954</v>
+      </c>
+      <c r="T387" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="U387" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="V387" s="17">
+        <v>1.687115e6</v>
+      </c>
+      <c r="W387" s="15" t="s">
+        <v>965</v>
+      </c>
+      <c r="X387" s="17">
+        <v>2321</v>
+      </c>
+      <c r="Y387" s="15" t="s">
+        <v>948</v>
+      </c>
+      <c r="Z387" s="15" t="s">
+        <v>531</v>
+      </c>
+      <c r="AA387" s="13" t="s">
+        <v>508</v>
+      </c>
+      <c r="AB387" s="21">
+        <v>60</v>
+      </c>
+      <c r="AC387" s="22">
+        <v>16.65</v>
+      </c>
+      <c r="AD387" s="22">
+        <v>16.65</v>
+      </c>
+      <c r="AE387" s="23">
+        <v>999</v>
+      </c>
+      <c r="AF387" s="23">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="388" s="1" customFormat="1" ht="18.1322" customHeight="1">
+      <c r="A388" s="3" t="s">
+        <v>943</v>
+      </c>
+      <c r="B388" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C388" s="4">
+        <v>43944</v>
+      </c>
+      <c r="D388" s="26" t="s">
+        <v>944</v>
+      </c>
+      <c r="E388" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F388" s="6">
+        <v>2320</v>
+      </c>
+      <c r="G388" s="3" t="s">
+        <v>945</v>
+      </c>
+      <c r="H388" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I388" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J388" s="7">
+        <v>0</v>
+      </c>
+      <c r="K388" s="5"/>
+      <c r="L388" s="7"/>
+      <c r="M388" s="5"/>
+      <c r="N388" s="8"/>
+      <c r="O388" s="8"/>
+      <c r="P388" s="9"/>
+      <c r="Q388" s="8"/>
+      <c r="R388" s="5" t="s">
+        <v>966</v>
+      </c>
+      <c r="S388" s="5" t="s">
+        <v>967</v>
+      </c>
+      <c r="T388" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U388" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="V388" s="7">
+        <v>1.257463e6</v>
+      </c>
+      <c r="W388" s="5" t="s">
+        <v>968</v>
+      </c>
+      <c r="X388" s="7">
+        <v>2321</v>
+      </c>
+      <c r="Y388" s="5" t="s">
+        <v>948</v>
+      </c>
+      <c r="Z388" s="5" t="s">
+        <v>531</v>
+      </c>
+      <c r="AA388" s="3" t="s">
+        <v>508</v>
+      </c>
+      <c r="AB388" s="10">
+        <v>200</v>
+      </c>
+      <c r="AC388" s="11">
+        <v>34.2</v>
+      </c>
+      <c r="AD388" s="11">
+        <v>34.2</v>
+      </c>
+      <c r="AE388" s="12">
+        <v>6840</v>
+      </c>
+      <c r="AF388" s="12">
+        <v>6840</v>
+      </c>
+    </row>
+    <row r="389" s="1" customFormat="1" ht="18.1322" customHeight="1">
+      <c r="A389" s="13" t="s">
+        <v>969</v>
+      </c>
+      <c r="B389" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C389" s="14">
+        <v>44012</v>
+      </c>
+      <c r="D389" s="15" t="s">
+        <v>970</v>
+      </c>
+      <c r="E389" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F389" s="16">
+        <v>2320</v>
+      </c>
+      <c r="G389" s="13" t="s">
+        <v>945</v>
+      </c>
+      <c r="H389" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I389" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="J389" s="17">
+        <v>0</v>
+      </c>
+      <c r="K389" s="15"/>
+      <c r="L389" s="17"/>
+      <c r="M389" s="15"/>
+      <c r="N389" s="18"/>
+      <c r="O389" s="18"/>
+      <c r="P389" s="19"/>
+      <c r="Q389" s="18"/>
+      <c r="R389" s="15" t="s">
+        <v>491</v>
+      </c>
+      <c r="S389" s="15" t="s">
+        <v>492</v>
+      </c>
+      <c r="T389" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="U389" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="V389" s="17">
+        <v>1.408623e6</v>
+      </c>
+      <c r="W389" s="15" t="s">
+        <v>971</v>
+      </c>
+      <c r="X389" s="17">
+        <v>2321</v>
+      </c>
+      <c r="Y389" s="15" t="s">
+        <v>948</v>
+      </c>
+      <c r="Z389" s="15" t="s">
+        <v>373</v>
+      </c>
+      <c r="AA389" s="13" t="s">
+        <v>508</v>
+      </c>
+      <c r="AB389" s="21">
         <v>2000</v>
       </c>
-      <c r="AC385" s="22">
+      <c r="AC389" s="22">
         <v>18.69</v>
       </c>
-      <c r="AD385" s="22">
+      <c r="AD389" s="22">
         <v>14.95</v>
       </c>
-      <c r="AE385" s="23">
+      <c r="AE389" s="23">
         <v>37380</v>
       </c>
-      <c r="AF385" s="23">
+      <c r="AF389" s="23">
         <v>29900</v>
       </c>
     </row>
-    <row r="386" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
+    <row r="390" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
   </sheetData>
   <pageSetup paperSize="9" scale="100" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>

<commit_message>
atualiza a planilha de compras -processo Unimontes
</commit_message>
<xml_diff>
--- a/data-raw/compras-coronavirus.xlsx
+++ b/data-raw/compras-coronavirus.xlsx
@@ -8,7 +8,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6389" uniqueCount="1029">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6820" uniqueCount="1066">
   <si>
     <t>Número Processo -  Formatado</t>
   </si>
@@ -3004,6 +3004,118 @@
   </si>
   <si>
     <t>EMBALAGEM DESCARTAVEL PARA ESTERILIZACAO -  MATERIA-PRIMA: SMS 100% POLIPROPILENO 45 G/M2; MATERIA-PRIMA 2: .; DIMENSOES (L X C ): 75 CM X 75 CM; TIPO ESTERILIZACAO: COMPATIVEL COM A MATERIA-PRIMA; INDICADOR: NAO POSSUI; APRESENTACAO: FOLHA 75 CM;</t>
+  </si>
+  <si>
+    <t>2311076 000512/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEDICAMENTOS
+COVID-19</t>
+  </si>
+  <si>
+    <t>08.778.201/0001-26</t>
+  </si>
+  <si>
+    <t>DROGAFONTE LTDA</t>
+  </si>
+  <si>
+    <t>ANLODIPINO, BESILATO - PRINCIPIO ATIVO: ANLODIPINO, BESILATO; CONCENTRACAO/DOSAGEM: 5 MG; FORMA FARMACEUTICA: COMPRIMIDO; APRESENTACAO: .; COMPONENTE: .;</t>
+  </si>
+  <si>
+    <t>AZITROMICINA - PRINCIPIO ATIVO: AZITROMICINA; CONCENTRACAO/DOSAGEM: 500 MG; FORMA FARMACEUTICA: COMPRIMIDO; APRESENTACAO: .; COMPONENTE: .;</t>
+  </si>
+  <si>
+    <t>DOBUTAMINA, CLORIDRATO - PRINCIPIO ATIVO: DOBUTAMINA, CLORIDRATO; CONCENTRACAO/DOSAGEM: 12,5 MG/ML; FORMA FARMACEUTICA: SOLUCAO INJETAVEL; APRESENTACAO: AMPOLA 20 ML; COMPONENTE: .;</t>
+  </si>
+  <si>
+    <t>SALBUTAMOL, SULFATO - PRINCIPIO ATIVO: SALBUTAMOL, SULFATO; CONCENTRACAO/DOSAGEM: 100 MCG/DOSE; FORMA FARMACEUTICA: AEROSSOL; APRESENTACAO: FRASCO TUBO 200 DOSES; COMPONENTE: APLICADOR;</t>
+  </si>
+  <si>
+    <t>INSULINA - PRINCIPIO ATIVO: INSULINA HUMANA NPH RECOMBINANTE; CONCENTRACAO/DOSAGEM: 100 UI/ML; FORMA FARMACEUTICA: SUSPENSAO INJETAVEL; APRESENTACAO: FRASCO 10 ML; COMPONENTE: .;</t>
+  </si>
+  <si>
+    <t>ENOXAPARINA SODICA PRINCIPIO ATIVO: ENOXAPARINA SODICA; CONCENTRACAO/DOSAGEM: 40 MG; FORMA FARMACEUTICA: SOLUCAO INJETAVEL; APRESENTACAO: SERINGA PREENCHIDA 0,4 ML; COMPONENTE: .;</t>
+  </si>
+  <si>
+    <t>LIDOCAINA SEM VASOCONSTRITOR PRINCIPIO ATIVO: LIDOCAINA, CLORIDRATO; CONCENTRACAO/DOSAGEM: 2%; FORMA FARMACEUTICA: SOLUCAO INJETAVEL; APRESENTACAO: AMPOLA 5 ML; COMPONENTE: .;</t>
+  </si>
+  <si>
+    <t>DEXAMETASONA - PRINCIPIO ATIVO: DEXAMETASONA, FOSFATO DISSODICO; CONCENTRACAO/DOSAGEM: 4 MG/ML; FORMA FARMACEUTICA: SOLUCAO INJETAVEL; APRESENTACAO: FRASCO-AMPOLA 2,5 ML; COMPONENTE: .;</t>
+  </si>
+  <si>
+    <t>DEXAMETASONA - PRINCIPIO ATIVO: DEXAMETASONA, FOSFATO DISSODICO; CONCENTRACAO/DOSAGEM: 2 MG/ML; FORMA FARMACEUTICA: SOLUCAO INJETAVEL; APRESENTACAO: AMPOLA 1 ML; COMPONENTE: .;</t>
+  </si>
+  <si>
+    <t>INSULINA - PRINCIPIO ATIVO: INSULINA HUMANA REGULAR; CONCENTRACAO/DOSAGEM: 100 UI/ML; FORMA FARMACEUTICA: SOLUCAO INJETAVEL; APRESENTACAO: FRASCO-AMPOLA 10 ML; COMPONENTE: .;</t>
+  </si>
+  <si>
+    <t>49.324.221/0020-77</t>
+  </si>
+  <si>
+    <t>FRESENIUS KABI BRASIL LTDA.</t>
+  </si>
+  <si>
+    <t>SUCCINATO SODICO DE METILPREDNISOLONA - PRINCIPIO ATIVO: SUCCINATO SODICO DE METILPREDNISOLONA; CONCENTRACAO/DOSAGEM: 500 MG; FORMA FARMACEUTICA: PO LIOFILIZADO; APRESENTACAO: FRASCO-AMPOLA; COMPONENTE: .;</t>
+  </si>
+  <si>
+    <t>58.635.830/0001-75</t>
+  </si>
+  <si>
+    <t>FARMARIN INDUSTRIA E COMERCIO LTDA</t>
+  </si>
+  <si>
+    <t>SOLUCAO PARA HEMODIALISE - IDENTIFICACAO: FRACAO ACIDA; PRINCIPIO ATIVO: CLORETO DE SODIO+CLORETO DE POTASSIO+ASSOCIACAO; FORMA FARMACEUTICA: SOLUCAO PARA HEMODIALISE; APRESENTACAO: EMBALAGEM 5L;</t>
+  </si>
+  <si>
+    <t>SOLUCAO PARA HEMODIALISE - IDENTIFICACAO: FRACAO BASICA; PRINCIPIO ATIVO: BICARBONATO DE SODIO; FORMA FARMACEUTICA: SOLUCAO PARA HEMODIALISE; APRESENTACAO: EMBALAGEM 5L;</t>
+  </si>
+  <si>
+    <t>https://www1.compras.mg.gov.br/contrato/gestaocontratos/arquivosContrato.html?idContrato=164493</t>
+  </si>
+  <si>
+    <t>HEPARINA SODICA - PRINCIPIO ATIVO: HEPARINA SODICA; CONCENTRACAO/DOSAGEM: 5000 UI/ML; FORMA FARMACEUTICA: SOLUCAO INJETAVEL INTRAVENOSA; APRESENTACAO: FRASCO-AMPOLA 5ML; COMPONENTE: .;</t>
+  </si>
+  <si>
+    <t>BROMETO DE PANCURONIO - PRINCIPIO ATIVO: BROMETO DE PANCURONIO; CONCENTRACAO/DOSAGEM: 2 MG/ML; FORMA FARMACEUTICA: SOLUCAO INJETAVEL; APRESENTACAO: AMPOLA 2 ML; COMPONENTE: .;</t>
+  </si>
+  <si>
+    <t>BESILATO DE ATRACURIO - PRINCIPIO ATIVO: BESILATO DE ATRACURIO; CONCENTRACAO/DOSAGEM: 10 MG/ML; FORMA FARMACEUTICA: SOLUCAO INJETAVEL; APRESENTACAO: AMPOLA 2,5 ML; COMPONENTE: .;</t>
+  </si>
+  <si>
+    <t>https://www1.compras.mg.gov.br/contrato/gestaocontratos/arquivosContrato.html?idContrato=164495</t>
+  </si>
+  <si>
+    <t>EPINEFRINA - PRINCIPIO ATIVO: EPINEFRINA; CONCENTRACAO/DOSAGEM: 1 MG/ML; FORMA FARMACEUTICA: SOLUCAO INJETAVEL; APRESENTACAO: AMPOLA 1 ML; COMPONENTE: .;</t>
+  </si>
+  <si>
+    <t>https://www1.compras.mg.gov.br/contrato/gestaocontratos/arquivosContrato.html?idContrato=164497</t>
+  </si>
+  <si>
+    <t>05.439.635/0004-56</t>
+  </si>
+  <si>
+    <t>Antibióticos do Brasil Ltda</t>
+  </si>
+  <si>
+    <t>MEROPENEM - PRINCIPIO ATIVO: MEROPENEM, TRI-HIDRATADO; CONCENTRACAO/DOSAGEM: 500 MG; FORMA FARMACEUTICA: PO PARA SOLUCAO INJETAVEL; APRESENTACAO: FRASCO-AMPOLA; COMPONENTE: .;</t>
+  </si>
+  <si>
+    <t>CEFEPIMA - PRINCIPIO ATIVO: CEFEPIMA; CONCENTRACAO/DOSAGEM: 1 G; FORMA FARMACEUTICA: PO LIOFILIZADO PARA SOLUCAO INJETAVEL; APRESENTACAO: FRASCO-AMPOLA; COMPONENTE: .;</t>
+  </si>
+  <si>
+    <t>VANCOMICINA - PRINCIPIO ATIVO: VANCOMICINA, CLORIDRATO; CONCENTRACAO/DOSAGEM: 500 MG; FORMA FARMACEUTICA: PO PARA SOLUCAO INJETAVEL; APRESENTACAO: FRASCO-AMPOLA; COMPONENTE: .;</t>
+  </si>
+  <si>
+    <t>https://www1.compras.mg.gov.br/contrato/gestaocontratos/arquivosContrato.html?idContrato=164510</t>
+  </si>
+  <si>
+    <t>81.706.251/0001-98</t>
+  </si>
+  <si>
+    <t>Promefarma Representações Comercias LTDA</t>
+  </si>
+  <si>
+    <t>ARGIPRESSINA - PRINCIPIO ATIVO: ARGIPRESSINA; CONCENTRACAO/DOSAGEM: 20 U/ML; FORMA FARMACEUTICA: SOLUCAO INJETAVEL; APRESENTACAO: AMPOLA 1 ML; COMPONENTE: .;</t>
   </si>
   <si>
     <t>2320310 000127/2020</t>
@@ -3299,7 +3411,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AF406"/>
+  <dimension ref="A1:AF433"/>
   <cols>
     <col min="1" max="1" width="27.8093" customWidth="1"/>
     <col min="2" max="2" width="23.8165" customWidth="1"/>
@@ -38088,7 +38200,7 @@
         <v>33</v>
       </c>
       <c r="C389" s="14">
-        <v>43944</v>
+        <v>44063</v>
       </c>
       <c r="D389" s="25" t="s">
         <v>997</v>
@@ -38097,10 +38209,10 @@
         <v>33</v>
       </c>
       <c r="F389" s="16">
-        <v>2320</v>
+        <v>2310</v>
       </c>
       <c r="G389" s="13" t="s">
-        <v>998</v>
+        <v>969</v>
       </c>
       <c r="H389" s="13" t="s">
         <v>36</v>
@@ -38119,49 +38231,49 @@
       <c r="P389" s="19"/>
       <c r="Q389" s="18"/>
       <c r="R389" s="15" t="s">
+        <v>998</v>
+      </c>
+      <c r="S389" s="15" t="s">
         <v>999</v>
       </c>
-      <c r="S389" s="15" t="s">
+      <c r="T389" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="U389" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="V389" s="17">
+        <v>1.489186e6</v>
+      </c>
+      <c r="W389" s="15" t="s">
         <v>1000</v>
       </c>
-      <c r="T389" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="U389" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="V389" s="17">
-        <v>1.692143e6</v>
-      </c>
-      <c r="W389" s="15" t="s">
-        <v>559</v>
-      </c>
       <c r="X389" s="17">
-        <v>2321</v>
+        <v>2311</v>
       </c>
       <c r="Y389" s="15" t="s">
-        <v>1001</v>
+        <v>969</v>
       </c>
       <c r="Z389" s="15" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="AA389" s="13" t="s">
-        <v>557</v>
+        <v>972</v>
       </c>
       <c r="AB389" s="21">
-        <v>3000</v>
+        <v>1170</v>
       </c>
       <c r="AC389" s="22">
-        <v>8.2</v>
+        <v>73000e-6</v>
       </c>
       <c r="AD389" s="22">
-        <v>8.2</v>
+        <v>73000e-6</v>
       </c>
       <c r="AE389" s="23">
-        <v>24600</v>
+        <v>85.41</v>
       </c>
       <c r="AF389" s="23">
-        <v>24600</v>
+        <v>85.41</v>
       </c>
     </row>
     <row r="390" s="1" customFormat="1" ht="18.1322" customHeight="1">
@@ -38172,7 +38284,7 @@
         <v>33</v>
       </c>
       <c r="C390" s="4">
-        <v>43944</v>
+        <v>44063</v>
       </c>
       <c r="D390" s="26" t="s">
         <v>997</v>
@@ -38181,10 +38293,10 @@
         <v>33</v>
       </c>
       <c r="F390" s="6">
-        <v>2320</v>
+        <v>2310</v>
       </c>
       <c r="G390" s="3" t="s">
-        <v>998</v>
+        <v>969</v>
       </c>
       <c r="H390" s="3" t="s">
         <v>36</v>
@@ -38203,10 +38315,10 @@
       <c r="P390" s="9"/>
       <c r="Q390" s="8"/>
       <c r="R390" s="5" t="s">
-        <v>1002</v>
+        <v>998</v>
       </c>
       <c r="S390" s="5" t="s">
-        <v>1003</v>
+        <v>999</v>
       </c>
       <c r="T390" s="3" t="s">
         <v>33</v>
@@ -38215,37 +38327,37 @@
         <v>33</v>
       </c>
       <c r="V390" s="7">
-        <v>1.143883e6</v>
+        <v>1.489259e6</v>
       </c>
       <c r="W390" s="5" t="s">
-        <v>1004</v>
+        <v>1001</v>
       </c>
       <c r="X390" s="7">
-        <v>2321</v>
+        <v>2311</v>
       </c>
       <c r="Y390" s="5" t="s">
-        <v>1001</v>
+        <v>969</v>
       </c>
       <c r="Z390" s="5" t="s">
-        <v>580</v>
+        <v>339</v>
       </c>
       <c r="AA390" s="3" t="s">
-        <v>557</v>
+        <v>972</v>
       </c>
       <c r="AB390" s="10">
-        <v>200000</v>
+        <v>1500</v>
       </c>
       <c r="AC390" s="11">
-        <v>600000e-6</v>
+        <v>2</v>
       </c>
       <c r="AD390" s="11">
-        <v>600000e-6</v>
+        <v>2</v>
       </c>
       <c r="AE390" s="12">
-        <v>120000</v>
+        <v>3000</v>
       </c>
       <c r="AF390" s="12">
-        <v>120000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="391" s="1" customFormat="1" ht="18.1322" customHeight="1">
@@ -38256,7 +38368,7 @@
         <v>33</v>
       </c>
       <c r="C391" s="14">
-        <v>43944</v>
+        <v>44063</v>
       </c>
       <c r="D391" s="25" t="s">
         <v>997</v>
@@ -38265,10 +38377,10 @@
         <v>33</v>
       </c>
       <c r="F391" s="16">
-        <v>2320</v>
+        <v>2310</v>
       </c>
       <c r="G391" s="13" t="s">
-        <v>998</v>
+        <v>969</v>
       </c>
       <c r="H391" s="13" t="s">
         <v>36</v>
@@ -38287,10 +38399,10 @@
       <c r="P391" s="19"/>
       <c r="Q391" s="18"/>
       <c r="R391" s="15" t="s">
-        <v>915</v>
+        <v>998</v>
       </c>
       <c r="S391" s="15" t="s">
-        <v>916</v>
+        <v>999</v>
       </c>
       <c r="T391" s="13" t="s">
         <v>33</v>
@@ -38299,37 +38411,37 @@
         <v>33</v>
       </c>
       <c r="V391" s="17">
-        <v>1.244515e6</v>
+        <v>1.489755e6</v>
       </c>
       <c r="W391" s="15" t="s">
-        <v>1005</v>
+        <v>1002</v>
       </c>
       <c r="X391" s="17">
-        <v>2321</v>
+        <v>2311</v>
       </c>
       <c r="Y391" s="15" t="s">
-        <v>1001</v>
+        <v>969</v>
       </c>
       <c r="Z391" s="15" t="s">
-        <v>580</v>
+        <v>339</v>
       </c>
       <c r="AA391" s="13" t="s">
-        <v>557</v>
+        <v>972</v>
       </c>
       <c r="AB391" s="21">
-        <v>50</v>
+        <v>1500</v>
       </c>
       <c r="AC391" s="22">
-        <v>20.1</v>
+        <v>9.43</v>
       </c>
       <c r="AD391" s="22">
-        <v>20.1</v>
+        <v>9.43</v>
       </c>
       <c r="AE391" s="23">
-        <v>1005</v>
+        <v>14145</v>
       </c>
       <c r="AF391" s="23">
-        <v>1005</v>
+        <v>14145</v>
       </c>
     </row>
     <row r="392" s="1" customFormat="1" ht="18.1322" customHeight="1">
@@ -38340,7 +38452,7 @@
         <v>33</v>
       </c>
       <c r="C392" s="4">
-        <v>43944</v>
+        <v>44063</v>
       </c>
       <c r="D392" s="26" t="s">
         <v>997</v>
@@ -38349,10 +38461,10 @@
         <v>33</v>
       </c>
       <c r="F392" s="6">
-        <v>2320</v>
+        <v>2310</v>
       </c>
       <c r="G392" s="3" t="s">
-        <v>998</v>
+        <v>969</v>
       </c>
       <c r="H392" s="3" t="s">
         <v>36</v>
@@ -38371,10 +38483,10 @@
       <c r="P392" s="9"/>
       <c r="Q392" s="8"/>
       <c r="R392" s="5" t="s">
-        <v>1006</v>
+        <v>998</v>
       </c>
       <c r="S392" s="5" t="s">
-        <v>1007</v>
+        <v>999</v>
       </c>
       <c r="T392" s="3" t="s">
         <v>33</v>
@@ -38383,37 +38495,37 @@
         <v>33</v>
       </c>
       <c r="V392" s="7">
-        <v>1.244108e6</v>
+        <v>1.490869e6</v>
       </c>
       <c r="W392" s="5" t="s">
-        <v>1008</v>
+        <v>1003</v>
       </c>
       <c r="X392" s="7">
-        <v>2321</v>
+        <v>2311</v>
       </c>
       <c r="Y392" s="5" t="s">
-        <v>1001</v>
+        <v>969</v>
       </c>
       <c r="Z392" s="5" t="s">
-        <v>580</v>
+        <v>339</v>
       </c>
       <c r="AA392" s="3" t="s">
-        <v>557</v>
+        <v>972</v>
       </c>
       <c r="AB392" s="10">
-        <v>90</v>
+        <v>2000</v>
       </c>
       <c r="AC392" s="11">
-        <v>358.24</v>
+        <v>7.9</v>
       </c>
       <c r="AD392" s="11">
-        <v>358.24</v>
+        <v>7.9</v>
       </c>
       <c r="AE392" s="12">
-        <v>32241.6</v>
+        <v>15800</v>
       </c>
       <c r="AF392" s="12">
-        <v>32241.6</v>
+        <v>15800</v>
       </c>
     </row>
     <row r="393" s="1" customFormat="1" ht="18.1322" customHeight="1">
@@ -38424,7 +38536,7 @@
         <v>33</v>
       </c>
       <c r="C393" s="14">
-        <v>43944</v>
+        <v>44063</v>
       </c>
       <c r="D393" s="25" t="s">
         <v>997</v>
@@ -38433,10 +38545,10 @@
         <v>33</v>
       </c>
       <c r="F393" s="16">
-        <v>2320</v>
+        <v>2310</v>
       </c>
       <c r="G393" s="13" t="s">
-        <v>998</v>
+        <v>969</v>
       </c>
       <c r="H393" s="13" t="s">
         <v>36</v>
@@ -38455,10 +38567,10 @@
       <c r="P393" s="19"/>
       <c r="Q393" s="18"/>
       <c r="R393" s="15" t="s">
-        <v>1006</v>
+        <v>998</v>
       </c>
       <c r="S393" s="15" t="s">
-        <v>1007</v>
+        <v>999</v>
       </c>
       <c r="T393" s="13" t="s">
         <v>33</v>
@@ -38467,37 +38579,37 @@
         <v>33</v>
       </c>
       <c r="V393" s="17">
-        <v>1.244507e6</v>
+        <v>1.512552e6</v>
       </c>
       <c r="W393" s="15" t="s">
-        <v>1009</v>
+        <v>468</v>
       </c>
       <c r="X393" s="17">
-        <v>2321</v>
+        <v>2311</v>
       </c>
       <c r="Y393" s="15" t="s">
-        <v>1001</v>
+        <v>969</v>
       </c>
       <c r="Z393" s="15" t="s">
-        <v>580</v>
+        <v>339</v>
       </c>
       <c r="AA393" s="13" t="s">
-        <v>557</v>
+        <v>972</v>
       </c>
       <c r="AB393" s="21">
-        <v>50</v>
+        <v>12650</v>
       </c>
       <c r="AC393" s="22">
-        <v>34.9</v>
+        <v>10.3</v>
       </c>
       <c r="AD393" s="22">
-        <v>34.9</v>
+        <v>10.3</v>
       </c>
       <c r="AE393" s="23">
-        <v>1745</v>
+        <v>130295</v>
       </c>
       <c r="AF393" s="23">
-        <v>1745</v>
+        <v>130295</v>
       </c>
     </row>
     <row r="394" s="1" customFormat="1" ht="18.1322" customHeight="1">
@@ -38508,7 +38620,7 @@
         <v>33</v>
       </c>
       <c r="C394" s="4">
-        <v>43944</v>
+        <v>44063</v>
       </c>
       <c r="D394" s="26" t="s">
         <v>997</v>
@@ -38517,10 +38629,10 @@
         <v>33</v>
       </c>
       <c r="F394" s="6">
-        <v>2320</v>
+        <v>2310</v>
       </c>
       <c r="G394" s="3" t="s">
-        <v>998</v>
+        <v>969</v>
       </c>
       <c r="H394" s="3" t="s">
         <v>36</v>
@@ -38539,10 +38651,10 @@
       <c r="P394" s="9"/>
       <c r="Q394" s="8"/>
       <c r="R394" s="5" t="s">
-        <v>1006</v>
+        <v>998</v>
       </c>
       <c r="S394" s="5" t="s">
-        <v>1007</v>
+        <v>999</v>
       </c>
       <c r="T394" s="3" t="s">
         <v>33</v>
@@ -38551,37 +38663,37 @@
         <v>33</v>
       </c>
       <c r="V394" s="7">
-        <v>1.257587e6</v>
+        <v>1.514385e6</v>
       </c>
       <c r="W394" s="5" t="s">
-        <v>1010</v>
+        <v>1004</v>
       </c>
       <c r="X394" s="7">
-        <v>2321</v>
+        <v>2311</v>
       </c>
       <c r="Y394" s="5" t="s">
-        <v>1001</v>
+        <v>969</v>
       </c>
       <c r="Z394" s="5" t="s">
-        <v>580</v>
+        <v>339</v>
       </c>
       <c r="AA394" s="3" t="s">
-        <v>557</v>
+        <v>972</v>
       </c>
       <c r="AB394" s="10">
-        <v>80000</v>
+        <v>120</v>
       </c>
       <c r="AC394" s="11">
-        <v>390000e-6</v>
+        <v>17.4</v>
       </c>
       <c r="AD394" s="11">
-        <v>390000e-6</v>
+        <v>17.4</v>
       </c>
       <c r="AE394" s="12">
-        <v>31200</v>
+        <v>2088</v>
       </c>
       <c r="AF394" s="12">
-        <v>31200</v>
+        <v>2088</v>
       </c>
     </row>
     <row r="395" s="1" customFormat="1" ht="18.1322" customHeight="1">
@@ -38592,7 +38704,7 @@
         <v>33</v>
       </c>
       <c r="C395" s="14">
-        <v>43944</v>
+        <v>44063</v>
       </c>
       <c r="D395" s="25" t="s">
         <v>997</v>
@@ -38601,10 +38713,10 @@
         <v>33</v>
       </c>
       <c r="F395" s="16">
-        <v>2320</v>
+        <v>2310</v>
       </c>
       <c r="G395" s="13" t="s">
-        <v>998</v>
+        <v>969</v>
       </c>
       <c r="H395" s="13" t="s">
         <v>36</v>
@@ -38623,10 +38735,10 @@
       <c r="P395" s="19"/>
       <c r="Q395" s="18"/>
       <c r="R395" s="15" t="s">
-        <v>1006</v>
+        <v>998</v>
       </c>
       <c r="S395" s="15" t="s">
-        <v>1007</v>
+        <v>999</v>
       </c>
       <c r="T395" s="13" t="s">
         <v>33</v>
@@ -38635,37 +38747,37 @@
         <v>33</v>
       </c>
       <c r="V395" s="17">
-        <v>1.257625e6</v>
+        <v>1.517287e6</v>
       </c>
       <c r="W395" s="15" t="s">
-        <v>1011</v>
+        <v>1005</v>
       </c>
       <c r="X395" s="17">
-        <v>2321</v>
+        <v>2311</v>
       </c>
       <c r="Y395" s="15" t="s">
-        <v>1001</v>
+        <v>969</v>
       </c>
       <c r="Z395" s="15" t="s">
-        <v>428</v>
+        <v>339</v>
       </c>
       <c r="AA395" s="13" t="s">
-        <v>557</v>
+        <v>972</v>
       </c>
       <c r="AB395" s="21">
-        <v>90</v>
+        <v>1130</v>
       </c>
       <c r="AC395" s="22">
-        <v>351</v>
+        <v>21.3</v>
       </c>
       <c r="AD395" s="22">
-        <v>351</v>
+        <v>21.3</v>
       </c>
       <c r="AE395" s="23">
-        <v>31590</v>
+        <v>24069</v>
       </c>
       <c r="AF395" s="23">
-        <v>31590</v>
+        <v>24069</v>
       </c>
     </row>
     <row r="396" s="1" customFormat="1" ht="18.1322" customHeight="1">
@@ -38676,7 +38788,7 @@
         <v>33</v>
       </c>
       <c r="C396" s="4">
-        <v>43944</v>
+        <v>44063</v>
       </c>
       <c r="D396" s="26" t="s">
         <v>997</v>
@@ -38685,10 +38797,10 @@
         <v>33</v>
       </c>
       <c r="F396" s="6">
-        <v>2320</v>
+        <v>2310</v>
       </c>
       <c r="G396" s="3" t="s">
-        <v>998</v>
+        <v>969</v>
       </c>
       <c r="H396" s="3" t="s">
         <v>36</v>
@@ -38707,49 +38819,49 @@
       <c r="P396" s="9"/>
       <c r="Q396" s="8"/>
       <c r="R396" s="5" t="s">
+        <v>998</v>
+      </c>
+      <c r="S396" s="5" t="s">
+        <v>999</v>
+      </c>
+      <c r="T396" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U396" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="V396" s="7">
+        <v>1.527703e6</v>
+      </c>
+      <c r="W396" s="5" t="s">
         <v>1006</v>
       </c>
-      <c r="S396" s="5" t="s">
-        <v>1007</v>
-      </c>
-      <c r="T396" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="U396" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="V396" s="7">
-        <v>1.258699e6</v>
-      </c>
-      <c r="W396" s="5" t="s">
-        <v>1012</v>
-      </c>
       <c r="X396" s="7">
-        <v>2321</v>
+        <v>2311</v>
       </c>
       <c r="Y396" s="5" t="s">
-        <v>1001</v>
+        <v>969</v>
       </c>
       <c r="Z396" s="5" t="s">
-        <v>580</v>
+        <v>339</v>
       </c>
       <c r="AA396" s="3" t="s">
-        <v>557</v>
+        <v>972</v>
       </c>
       <c r="AB396" s="10">
-        <v>2000</v>
+        <v>3400</v>
       </c>
       <c r="AC396" s="11">
-        <v>1.39</v>
+        <v>850000e-6</v>
       </c>
       <c r="AD396" s="11">
-        <v>1.39</v>
+        <v>850000e-6</v>
       </c>
       <c r="AE396" s="12">
-        <v>2780</v>
+        <v>2890</v>
       </c>
       <c r="AF396" s="12">
-        <v>2780</v>
+        <v>2890</v>
       </c>
     </row>
     <row r="397" s="1" customFormat="1" ht="18.1322" customHeight="1">
@@ -38760,7 +38872,7 @@
         <v>33</v>
       </c>
       <c r="C397" s="14">
-        <v>43944</v>
+        <v>44063</v>
       </c>
       <c r="D397" s="25" t="s">
         <v>997</v>
@@ -38769,10 +38881,10 @@
         <v>33</v>
       </c>
       <c r="F397" s="16">
-        <v>2320</v>
+        <v>2310</v>
       </c>
       <c r="G397" s="13" t="s">
-        <v>998</v>
+        <v>969</v>
       </c>
       <c r="H397" s="13" t="s">
         <v>36</v>
@@ -38791,49 +38903,49 @@
       <c r="P397" s="19"/>
       <c r="Q397" s="18"/>
       <c r="R397" s="15" t="s">
-        <v>1006</v>
+        <v>998</v>
       </c>
       <c r="S397" s="15" t="s">
+        <v>999</v>
+      </c>
+      <c r="T397" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="U397" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="V397" s="17">
+        <v>1.568515e6</v>
+      </c>
+      <c r="W397" s="15" t="s">
         <v>1007</v>
       </c>
-      <c r="T397" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="U397" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="V397" s="17">
-        <v>1.259784e6</v>
-      </c>
-      <c r="W397" s="15" t="s">
-        <v>1013</v>
-      </c>
       <c r="X397" s="17">
-        <v>2321</v>
+        <v>2311</v>
       </c>
       <c r="Y397" s="15" t="s">
-        <v>1001</v>
+        <v>969</v>
       </c>
       <c r="Z397" s="15" t="s">
-        <v>580</v>
+        <v>339</v>
       </c>
       <c r="AA397" s="13" t="s">
-        <v>557</v>
+        <v>972</v>
       </c>
       <c r="AB397" s="21">
-        <v>3000</v>
+        <v>9000</v>
       </c>
       <c r="AC397" s="22">
-        <v>600000e-6</v>
+        <v>880000e-6</v>
       </c>
       <c r="AD397" s="22">
-        <v>600000e-6</v>
+        <v>880000e-6</v>
       </c>
       <c r="AE397" s="23">
-        <v>1800</v>
+        <v>7920</v>
       </c>
       <c r="AF397" s="23">
-        <v>1800</v>
+        <v>7920</v>
       </c>
     </row>
     <row r="398" s="1" customFormat="1" ht="18.1322" customHeight="1">
@@ -38844,7 +38956,7 @@
         <v>33</v>
       </c>
       <c r="C398" s="4">
-        <v>43944</v>
+        <v>44063</v>
       </c>
       <c r="D398" s="26" t="s">
         <v>997</v>
@@ -38853,10 +38965,10 @@
         <v>33</v>
       </c>
       <c r="F398" s="6">
-        <v>2320</v>
+        <v>2310</v>
       </c>
       <c r="G398" s="3" t="s">
-        <v>998</v>
+        <v>969</v>
       </c>
       <c r="H398" s="3" t="s">
         <v>36</v>
@@ -38875,10 +38987,10 @@
       <c r="P398" s="9"/>
       <c r="Q398" s="8"/>
       <c r="R398" s="5" t="s">
-        <v>1006</v>
+        <v>998</v>
       </c>
       <c r="S398" s="5" t="s">
-        <v>1007</v>
+        <v>999</v>
       </c>
       <c r="T398" s="3" t="s">
         <v>33</v>
@@ -38887,37 +38999,37 @@
         <v>33</v>
       </c>
       <c r="V398" s="7">
-        <v>1.259792e6</v>
+        <v>1.573985e6</v>
       </c>
       <c r="W398" s="5" t="s">
-        <v>1014</v>
+        <v>1008</v>
       </c>
       <c r="X398" s="7">
-        <v>2321</v>
+        <v>2311</v>
       </c>
       <c r="Y398" s="5" t="s">
-        <v>1001</v>
+        <v>969</v>
       </c>
       <c r="Z398" s="5" t="s">
-        <v>580</v>
+        <v>339</v>
       </c>
       <c r="AA398" s="3" t="s">
-        <v>557</v>
+        <v>972</v>
       </c>
       <c r="AB398" s="10">
-        <v>80</v>
+        <v>4500</v>
       </c>
       <c r="AC398" s="11">
-        <v>15.35</v>
+        <v>1.25</v>
       </c>
       <c r="AD398" s="11">
-        <v>15.35</v>
+        <v>1.25</v>
       </c>
       <c r="AE398" s="12">
-        <v>1228</v>
+        <v>5625</v>
       </c>
       <c r="AF398" s="12">
-        <v>1228</v>
+        <v>5625</v>
       </c>
     </row>
     <row r="399" s="1" customFormat="1" ht="18.1322" customHeight="1">
@@ -38928,7 +39040,7 @@
         <v>33</v>
       </c>
       <c r="C399" s="14">
-        <v>43944</v>
+        <v>44063</v>
       </c>
       <c r="D399" s="25" t="s">
         <v>997</v>
@@ -38937,10 +39049,10 @@
         <v>33</v>
       </c>
       <c r="F399" s="16">
-        <v>2320</v>
+        <v>2310</v>
       </c>
       <c r="G399" s="13" t="s">
-        <v>998</v>
+        <v>969</v>
       </c>
       <c r="H399" s="13" t="s">
         <v>36</v>
@@ -38959,10 +39071,10 @@
       <c r="P399" s="19"/>
       <c r="Q399" s="18"/>
       <c r="R399" s="15" t="s">
-        <v>1006</v>
+        <v>998</v>
       </c>
       <c r="S399" s="15" t="s">
-        <v>1007</v>
+        <v>999</v>
       </c>
       <c r="T399" s="13" t="s">
         <v>33</v>
@@ -38971,37 +39083,37 @@
         <v>33</v>
       </c>
       <c r="V399" s="17">
-        <v>1.260669e6</v>
+        <v>1.582194e6</v>
       </c>
       <c r="W399" s="15" t="s">
-        <v>1015</v>
+        <v>1009</v>
       </c>
       <c r="X399" s="17">
-        <v>2321</v>
+        <v>2311</v>
       </c>
       <c r="Y399" s="15" t="s">
-        <v>1001</v>
+        <v>969</v>
       </c>
       <c r="Z399" s="15" t="s">
-        <v>580</v>
+        <v>339</v>
       </c>
       <c r="AA399" s="13" t="s">
-        <v>557</v>
+        <v>972</v>
       </c>
       <c r="AB399" s="21">
-        <v>1000</v>
+        <v>48</v>
       </c>
       <c r="AC399" s="22">
-        <v>1.49</v>
+        <v>17.4</v>
       </c>
       <c r="AD399" s="22">
-        <v>1.49</v>
+        <v>17.4</v>
       </c>
       <c r="AE399" s="23">
-        <v>1490</v>
+        <v>835.2</v>
       </c>
       <c r="AF399" s="23">
-        <v>1490</v>
+        <v>835.2</v>
       </c>
     </row>
     <row r="400" s="1" customFormat="1" ht="18.1322" customHeight="1">
@@ -39012,7 +39124,7 @@
         <v>33</v>
       </c>
       <c r="C400" s="4">
-        <v>43944</v>
+        <v>44063</v>
       </c>
       <c r="D400" s="26" t="s">
         <v>997</v>
@@ -39021,10 +39133,10 @@
         <v>33</v>
       </c>
       <c r="F400" s="6">
-        <v>2320</v>
+        <v>2310</v>
       </c>
       <c r="G400" s="3" t="s">
-        <v>998</v>
+        <v>969</v>
       </c>
       <c r="H400" s="3" t="s">
         <v>36</v>
@@ -39043,10 +39155,10 @@
       <c r="P400" s="9"/>
       <c r="Q400" s="8"/>
       <c r="R400" s="5" t="s">
-        <v>1006</v>
+        <v>1010</v>
       </c>
       <c r="S400" s="5" t="s">
-        <v>1007</v>
+        <v>1011</v>
       </c>
       <c r="T400" s="3" t="s">
         <v>33</v>
@@ -39055,37 +39167,37 @@
         <v>33</v>
       </c>
       <c r="V400" s="7">
-        <v>1.260677e6</v>
+        <v>1.527525e6</v>
       </c>
       <c r="W400" s="5" t="s">
-        <v>1016</v>
+        <v>1012</v>
       </c>
       <c r="X400" s="7">
-        <v>2321</v>
+        <v>2311</v>
       </c>
       <c r="Y400" s="5" t="s">
-        <v>1001</v>
+        <v>969</v>
       </c>
       <c r="Z400" s="5" t="s">
-        <v>580</v>
+        <v>339</v>
       </c>
       <c r="AA400" s="3" t="s">
-        <v>557</v>
+        <v>972</v>
       </c>
       <c r="AB400" s="10">
-        <v>3000</v>
+        <v>1000</v>
       </c>
       <c r="AC400" s="11">
-        <v>1.59</v>
+        <v>14.3</v>
       </c>
       <c r="AD400" s="11">
-        <v>1.59</v>
+        <v>14.3</v>
       </c>
       <c r="AE400" s="12">
-        <v>4770</v>
+        <v>14300</v>
       </c>
       <c r="AF400" s="12">
-        <v>4770</v>
+        <v>14300</v>
       </c>
     </row>
     <row r="401" s="1" customFormat="1" ht="18.1322" customHeight="1">
@@ -39096,7 +39208,7 @@
         <v>33</v>
       </c>
       <c r="C401" s="14">
-        <v>43944</v>
+        <v>44063</v>
       </c>
       <c r="D401" s="25" t="s">
         <v>997</v>
@@ -39105,10 +39217,10 @@
         <v>33</v>
       </c>
       <c r="F401" s="16">
-        <v>2320</v>
+        <v>2310</v>
       </c>
       <c r="G401" s="13" t="s">
-        <v>998</v>
+        <v>969</v>
       </c>
       <c r="H401" s="13" t="s">
         <v>36</v>
@@ -39127,10 +39239,10 @@
       <c r="P401" s="19"/>
       <c r="Q401" s="18"/>
       <c r="R401" s="15" t="s">
-        <v>1006</v>
+        <v>1013</v>
       </c>
       <c r="S401" s="15" t="s">
-        <v>1007</v>
+        <v>1014</v>
       </c>
       <c r="T401" s="13" t="s">
         <v>33</v>
@@ -39139,37 +39251,37 @@
         <v>33</v>
       </c>
       <c r="V401" s="17">
-        <v>1.260731e6</v>
-      </c>
-      <c r="W401" s="20" t="s">
-        <v>1017</v>
+        <v>1.513559e6</v>
+      </c>
+      <c r="W401" s="15" t="s">
+        <v>1015</v>
       </c>
       <c r="X401" s="17">
-        <v>2321</v>
+        <v>2311</v>
       </c>
       <c r="Y401" s="15" t="s">
-        <v>1001</v>
+        <v>969</v>
       </c>
       <c r="Z401" s="15" t="s">
-        <v>580</v>
+        <v>339</v>
       </c>
       <c r="AA401" s="13" t="s">
-        <v>557</v>
+        <v>972</v>
       </c>
       <c r="AB401" s="21">
-        <v>60</v>
+        <v>502</v>
       </c>
       <c r="AC401" s="22">
-        <v>271.97</v>
+        <v>13.9</v>
       </c>
       <c r="AD401" s="22">
-        <v>271.97</v>
+        <v>13.9</v>
       </c>
       <c r="AE401" s="23">
-        <v>16318.2</v>
+        <v>6977.8</v>
       </c>
       <c r="AF401" s="23">
-        <v>16318.2</v>
+        <v>6977.8</v>
       </c>
     </row>
     <row r="402" s="1" customFormat="1" ht="18.1322" customHeight="1">
@@ -39180,7 +39292,7 @@
         <v>33</v>
       </c>
       <c r="C402" s="4">
-        <v>43944</v>
+        <v>44063</v>
       </c>
       <c r="D402" s="26" t="s">
         <v>997</v>
@@ -39189,10 +39301,10 @@
         <v>33</v>
       </c>
       <c r="F402" s="6">
-        <v>2320</v>
+        <v>2310</v>
       </c>
       <c r="G402" s="3" t="s">
-        <v>998</v>
+        <v>969</v>
       </c>
       <c r="H402" s="3" t="s">
         <v>36</v>
@@ -39211,10 +39323,10 @@
       <c r="P402" s="9"/>
       <c r="Q402" s="8"/>
       <c r="R402" s="5" t="s">
-        <v>1006</v>
+        <v>1013</v>
       </c>
       <c r="S402" s="5" t="s">
-        <v>1007</v>
+        <v>1014</v>
       </c>
       <c r="T402" s="3" t="s">
         <v>33</v>
@@ -39223,37 +39335,37 @@
         <v>33</v>
       </c>
       <c r="V402" s="7">
-        <v>1.687115e6</v>
+        <v>1.51421e6</v>
       </c>
       <c r="W402" s="5" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="X402" s="7">
-        <v>2321</v>
+        <v>2311</v>
       </c>
       <c r="Y402" s="5" t="s">
-        <v>1001</v>
+        <v>969</v>
       </c>
       <c r="Z402" s="5" t="s">
-        <v>580</v>
+        <v>339</v>
       </c>
       <c r="AA402" s="3" t="s">
-        <v>557</v>
+        <v>972</v>
       </c>
       <c r="AB402" s="10">
-        <v>60</v>
+        <v>502</v>
       </c>
       <c r="AC402" s="11">
-        <v>16.65</v>
+        <v>8.55</v>
       </c>
       <c r="AD402" s="11">
-        <v>16.65</v>
+        <v>8.55</v>
       </c>
       <c r="AE402" s="12">
-        <v>999</v>
+        <v>4292.1</v>
       </c>
       <c r="AF402" s="12">
-        <v>999</v>
+        <v>4292.1</v>
       </c>
     </row>
     <row r="403" s="1" customFormat="1" ht="18.1322" customHeight="1">
@@ -39264,7 +39376,7 @@
         <v>33</v>
       </c>
       <c r="C403" s="14">
-        <v>43944</v>
+        <v>44063</v>
       </c>
       <c r="D403" s="25" t="s">
         <v>997</v>
@@ -39273,10 +39385,10 @@
         <v>33</v>
       </c>
       <c r="F403" s="16">
-        <v>2320</v>
+        <v>2310</v>
       </c>
       <c r="G403" s="13" t="s">
-        <v>998</v>
+        <v>969</v>
       </c>
       <c r="H403" s="13" t="s">
         <v>36</v>
@@ -39285,20 +39397,34 @@
         <v>37</v>
       </c>
       <c r="J403" s="17">
-        <v>0</v>
-      </c>
-      <c r="K403" s="15"/>
-      <c r="L403" s="17"/>
-      <c r="M403" s="15"/>
-      <c r="N403" s="18"/>
-      <c r="O403" s="18"/>
-      <c r="P403" s="19"/>
-      <c r="Q403" s="18"/>
+        <v>9.261504e6</v>
+      </c>
+      <c r="K403" s="15" t="s">
+        <v>1017</v>
+      </c>
+      <c r="L403" s="17">
+        <v>2310</v>
+      </c>
+      <c r="M403" s="15" t="s">
+        <v>969</v>
+      </c>
+      <c r="N403" s="18">
+        <v>44084</v>
+      </c>
+      <c r="O403" s="18">
+        <v>44084</v>
+      </c>
+      <c r="P403" s="19">
+        <v>44449</v>
+      </c>
+      <c r="Q403" s="18">
+        <v>44264</v>
+      </c>
       <c r="R403" s="15" t="s">
-        <v>1019</v>
+        <v>496</v>
       </c>
       <c r="S403" s="15" t="s">
-        <v>1020</v>
+        <v>497</v>
       </c>
       <c r="T403" s="13" t="s">
         <v>33</v>
@@ -39307,60 +39433,60 @@
         <v>33</v>
       </c>
       <c r="V403" s="17">
-        <v>1.257463e6</v>
+        <v>1.487779e6</v>
       </c>
       <c r="W403" s="15" t="s">
-        <v>1021</v>
+        <v>1018</v>
       </c>
       <c r="X403" s="17">
-        <v>2321</v>
+        <v>2311</v>
       </c>
       <c r="Y403" s="15" t="s">
-        <v>1001</v>
+        <v>969</v>
       </c>
       <c r="Z403" s="15" t="s">
-        <v>580</v>
+        <v>339</v>
       </c>
       <c r="AA403" s="13" t="s">
-        <v>557</v>
+        <v>972</v>
       </c>
       <c r="AB403" s="21">
-        <v>200</v>
+        <v>1130</v>
       </c>
       <c r="AC403" s="22">
-        <v>34.2</v>
+        <v>22.27</v>
       </c>
       <c r="AD403" s="22">
-        <v>34.2</v>
+        <v>22.27</v>
       </c>
       <c r="AE403" s="23">
-        <v>6840</v>
+        <v>25165.1</v>
       </c>
       <c r="AF403" s="23">
-        <v>6840</v>
+        <v>25165.1</v>
       </c>
     </row>
     <row r="404" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A404" s="3" t="s">
-        <v>1022</v>
+        <v>996</v>
       </c>
       <c r="B404" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C404" s="4">
-        <v>44012</v>
-      </c>
-      <c r="D404" s="5" t="s">
-        <v>1023</v>
+        <v>44063</v>
+      </c>
+      <c r="D404" s="26" t="s">
+        <v>997</v>
       </c>
       <c r="E404" s="5" t="s">
         <v>33</v>
       </c>
       <c r="F404" s="6">
-        <v>2320</v>
+        <v>2310</v>
       </c>
       <c r="G404" s="3" t="s">
-        <v>998</v>
+        <v>969</v>
       </c>
       <c r="H404" s="3" t="s">
         <v>36</v>
@@ -39369,20 +39495,34 @@
         <v>37</v>
       </c>
       <c r="J404" s="7">
-        <v>0</v>
-      </c>
-      <c r="K404" s="5"/>
-      <c r="L404" s="7"/>
-      <c r="M404" s="5"/>
-      <c r="N404" s="8"/>
-      <c r="O404" s="8"/>
-      <c r="P404" s="9"/>
-      <c r="Q404" s="8"/>
+        <v>9.261504e6</v>
+      </c>
+      <c r="K404" s="5" t="s">
+        <v>1017</v>
+      </c>
+      <c r="L404" s="7">
+        <v>2310</v>
+      </c>
+      <c r="M404" s="5" t="s">
+        <v>969</v>
+      </c>
+      <c r="N404" s="8">
+        <v>44084</v>
+      </c>
+      <c r="O404" s="8">
+        <v>44084</v>
+      </c>
+      <c r="P404" s="9">
+        <v>44449</v>
+      </c>
+      <c r="Q404" s="8">
+        <v>44264</v>
+      </c>
       <c r="R404" s="5" t="s">
-        <v>540</v>
+        <v>496</v>
       </c>
       <c r="S404" s="5" t="s">
-        <v>541</v>
+        <v>497</v>
       </c>
       <c r="T404" s="3" t="s">
         <v>33</v>
@@ -39391,138 +39531,2560 @@
         <v>33</v>
       </c>
       <c r="V404" s="7">
-        <v>1.408623e6</v>
+        <v>1.512285e6</v>
       </c>
       <c r="W404" s="5" t="s">
-        <v>1024</v>
+        <v>499</v>
       </c>
       <c r="X404" s="7">
-        <v>2321</v>
+        <v>2311</v>
       </c>
       <c r="Y404" s="5" t="s">
-        <v>1001</v>
+        <v>969</v>
       </c>
       <c r="Z404" s="5" t="s">
-        <v>422</v>
+        <v>339</v>
       </c>
       <c r="AA404" s="3" t="s">
-        <v>557</v>
+        <v>972</v>
       </c>
       <c r="AB404" s="10">
-        <v>2000</v>
+        <v>250</v>
       </c>
       <c r="AC404" s="11">
-        <v>18.69</v>
+        <v>69.9</v>
       </c>
       <c r="AD404" s="11">
-        <v>14.95</v>
+        <v>69.9</v>
       </c>
       <c r="AE404" s="12">
-        <v>37380</v>
+        <v>17475</v>
       </c>
       <c r="AF404" s="12">
-        <v>29900</v>
+        <v>17475</v>
       </c>
     </row>
     <row r="405" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A405" s="13" t="s">
+        <v>996</v>
+      </c>
+      <c r="B405" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C405" s="14">
+        <v>44063</v>
+      </c>
+      <c r="D405" s="25" t="s">
+        <v>997</v>
+      </c>
+      <c r="E405" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F405" s="16">
+        <v>2310</v>
+      </c>
+      <c r="G405" s="13" t="s">
+        <v>969</v>
+      </c>
+      <c r="H405" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I405" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="J405" s="17">
+        <v>9.261504e6</v>
+      </c>
+      <c r="K405" s="15" t="s">
+        <v>1017</v>
+      </c>
+      <c r="L405" s="17">
+        <v>2310</v>
+      </c>
+      <c r="M405" s="15" t="s">
+        <v>969</v>
+      </c>
+      <c r="N405" s="18">
+        <v>44084</v>
+      </c>
+      <c r="O405" s="18">
+        <v>44084</v>
+      </c>
+      <c r="P405" s="19">
+        <v>44449</v>
+      </c>
+      <c r="Q405" s="18">
+        <v>44264</v>
+      </c>
+      <c r="R405" s="15" t="s">
+        <v>496</v>
+      </c>
+      <c r="S405" s="15" t="s">
+        <v>497</v>
+      </c>
+      <c r="T405" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="U405" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="V405" s="17">
+        <v>1.512293e6</v>
+      </c>
+      <c r="W405" s="15" t="s">
+        <v>500</v>
+      </c>
+      <c r="X405" s="17">
+        <v>2311</v>
+      </c>
+      <c r="Y405" s="15" t="s">
+        <v>969</v>
+      </c>
+      <c r="Z405" s="15" t="s">
+        <v>339</v>
+      </c>
+      <c r="AA405" s="13" t="s">
+        <v>972</v>
+      </c>
+      <c r="AB405" s="21">
+        <v>900</v>
+      </c>
+      <c r="AC405" s="22">
+        <v>13.76</v>
+      </c>
+      <c r="AD405" s="22">
+        <v>13.76</v>
+      </c>
+      <c r="AE405" s="23">
+        <v>12384</v>
+      </c>
+      <c r="AF405" s="23">
+        <v>12384</v>
+      </c>
+    </row>
+    <row r="406" s="1" customFormat="1" ht="18.1322" customHeight="1">
+      <c r="A406" s="3" t="s">
+        <v>996</v>
+      </c>
+      <c r="B406" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C406" s="4">
+        <v>44063</v>
+      </c>
+      <c r="D406" s="26" t="s">
+        <v>997</v>
+      </c>
+      <c r="E406" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F406" s="6">
+        <v>2310</v>
+      </c>
+      <c r="G406" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="H406" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I406" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J406" s="7">
+        <v>9.261504e6</v>
+      </c>
+      <c r="K406" s="5" t="s">
+        <v>1017</v>
+      </c>
+      <c r="L406" s="7">
+        <v>2310</v>
+      </c>
+      <c r="M406" s="5" t="s">
+        <v>969</v>
+      </c>
+      <c r="N406" s="8">
+        <v>44084</v>
+      </c>
+      <c r="O406" s="8">
+        <v>44084</v>
+      </c>
+      <c r="P406" s="9">
+        <v>44449</v>
+      </c>
+      <c r="Q406" s="8">
+        <v>44264</v>
+      </c>
+      <c r="R406" s="5" t="s">
+        <v>496</v>
+      </c>
+      <c r="S406" s="5" t="s">
+        <v>497</v>
+      </c>
+      <c r="T406" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U406" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="V406" s="7">
+        <v>1.512552e6</v>
+      </c>
+      <c r="W406" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="X406" s="7">
+        <v>2311</v>
+      </c>
+      <c r="Y406" s="5" t="s">
+        <v>969</v>
+      </c>
+      <c r="Z406" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="AA406" s="3" t="s">
+        <v>972</v>
+      </c>
+      <c r="AB406" s="10">
+        <v>4000</v>
+      </c>
+      <c r="AC406" s="11">
+        <v>6.9</v>
+      </c>
+      <c r="AD406" s="11">
+        <v>6.9</v>
+      </c>
+      <c r="AE406" s="12">
+        <v>27600</v>
+      </c>
+      <c r="AF406" s="12">
+        <v>27600</v>
+      </c>
+    </row>
+    <row r="407" s="1" customFormat="1" ht="18.1322" customHeight="1">
+      <c r="A407" s="13" t="s">
+        <v>996</v>
+      </c>
+      <c r="B407" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C407" s="14">
+        <v>44063</v>
+      </c>
+      <c r="D407" s="25" t="s">
+        <v>997</v>
+      </c>
+      <c r="E407" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F407" s="16">
+        <v>2310</v>
+      </c>
+      <c r="G407" s="13" t="s">
+        <v>969</v>
+      </c>
+      <c r="H407" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I407" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="J407" s="17">
+        <v>9.261504e6</v>
+      </c>
+      <c r="K407" s="15" t="s">
+        <v>1017</v>
+      </c>
+      <c r="L407" s="17">
+        <v>2310</v>
+      </c>
+      <c r="M407" s="15" t="s">
+        <v>969</v>
+      </c>
+      <c r="N407" s="18">
+        <v>44084</v>
+      </c>
+      <c r="O407" s="18">
+        <v>44084</v>
+      </c>
+      <c r="P407" s="19">
+        <v>44449</v>
+      </c>
+      <c r="Q407" s="18">
+        <v>44264</v>
+      </c>
+      <c r="R407" s="15" t="s">
+        <v>496</v>
+      </c>
+      <c r="S407" s="15" t="s">
+        <v>497</v>
+      </c>
+      <c r="T407" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="U407" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="V407" s="17">
+        <v>1.512897e6</v>
+      </c>
+      <c r="W407" s="15" t="s">
+        <v>507</v>
+      </c>
+      <c r="X407" s="17">
+        <v>2311</v>
+      </c>
+      <c r="Y407" s="15" t="s">
+        <v>969</v>
+      </c>
+      <c r="Z407" s="15" t="s">
+        <v>339</v>
+      </c>
+      <c r="AA407" s="13" t="s">
+        <v>972</v>
+      </c>
+      <c r="AB407" s="21">
+        <v>2000</v>
+      </c>
+      <c r="AC407" s="22">
+        <v>13.54</v>
+      </c>
+      <c r="AD407" s="22">
+        <v>13.54</v>
+      </c>
+      <c r="AE407" s="23">
+        <v>27080</v>
+      </c>
+      <c r="AF407" s="23">
+        <v>27080</v>
+      </c>
+    </row>
+    <row r="408" s="1" customFormat="1" ht="18.1322" customHeight="1">
+      <c r="A408" s="3" t="s">
+        <v>996</v>
+      </c>
+      <c r="B408" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C408" s="4">
+        <v>44063</v>
+      </c>
+      <c r="D408" s="26" t="s">
+        <v>997</v>
+      </c>
+      <c r="E408" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F408" s="6">
+        <v>2310</v>
+      </c>
+      <c r="G408" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="H408" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I408" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J408" s="7">
+        <v>9.261504e6</v>
+      </c>
+      <c r="K408" s="5" t="s">
+        <v>1017</v>
+      </c>
+      <c r="L408" s="7">
+        <v>2310</v>
+      </c>
+      <c r="M408" s="5" t="s">
+        <v>969</v>
+      </c>
+      <c r="N408" s="8">
+        <v>44084</v>
+      </c>
+      <c r="O408" s="8">
+        <v>44084</v>
+      </c>
+      <c r="P408" s="9">
+        <v>44449</v>
+      </c>
+      <c r="Q408" s="8">
+        <v>44264</v>
+      </c>
+      <c r="R408" s="5" t="s">
+        <v>496</v>
+      </c>
+      <c r="S408" s="5" t="s">
+        <v>497</v>
+      </c>
+      <c r="T408" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U408" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="V408" s="7">
+        <v>1.525662e6</v>
+      </c>
+      <c r="W408" s="5" t="s">
+        <v>495</v>
+      </c>
+      <c r="X408" s="7">
+        <v>2311</v>
+      </c>
+      <c r="Y408" s="5" t="s">
+        <v>969</v>
+      </c>
+      <c r="Z408" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="AA408" s="3" t="s">
+        <v>972</v>
+      </c>
+      <c r="AB408" s="10">
+        <v>250</v>
+      </c>
+      <c r="AC408" s="11">
+        <v>20.5</v>
+      </c>
+      <c r="AD408" s="11">
+        <v>20.5</v>
+      </c>
+      <c r="AE408" s="12">
+        <v>5125</v>
+      </c>
+      <c r="AF408" s="12">
+        <v>5125</v>
+      </c>
+    </row>
+    <row r="409" s="1" customFormat="1" ht="18.1322" customHeight="1">
+      <c r="A409" s="13" t="s">
+        <v>996</v>
+      </c>
+      <c r="B409" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C409" s="14">
+        <v>44063</v>
+      </c>
+      <c r="D409" s="25" t="s">
+        <v>997</v>
+      </c>
+      <c r="E409" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F409" s="16">
+        <v>2310</v>
+      </c>
+      <c r="G409" s="13" t="s">
+        <v>969</v>
+      </c>
+      <c r="H409" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I409" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="J409" s="17">
+        <v>9.261504e6</v>
+      </c>
+      <c r="K409" s="15" t="s">
+        <v>1017</v>
+      </c>
+      <c r="L409" s="17">
+        <v>2310</v>
+      </c>
+      <c r="M409" s="15" t="s">
+        <v>969</v>
+      </c>
+      <c r="N409" s="18">
+        <v>44084</v>
+      </c>
+      <c r="O409" s="18">
+        <v>44084</v>
+      </c>
+      <c r="P409" s="19">
+        <v>44449</v>
+      </c>
+      <c r="Q409" s="18">
+        <v>44264</v>
+      </c>
+      <c r="R409" s="15" t="s">
+        <v>496</v>
+      </c>
+      <c r="S409" s="15" t="s">
+        <v>497</v>
+      </c>
+      <c r="T409" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="U409" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="V409" s="17">
+        <v>1.525689e6</v>
+      </c>
+      <c r="W409" s="15" t="s">
+        <v>1019</v>
+      </c>
+      <c r="X409" s="17">
+        <v>2311</v>
+      </c>
+      <c r="Y409" s="15" t="s">
+        <v>969</v>
+      </c>
+      <c r="Z409" s="15" t="s">
+        <v>339</v>
+      </c>
+      <c r="AA409" s="13" t="s">
+        <v>972</v>
+      </c>
+      <c r="AB409" s="21">
+        <v>1300</v>
+      </c>
+      <c r="AC409" s="22">
+        <v>7.5</v>
+      </c>
+      <c r="AD409" s="22">
+        <v>7.5</v>
+      </c>
+      <c r="AE409" s="23">
+        <v>9750</v>
+      </c>
+      <c r="AF409" s="23">
+        <v>9750</v>
+      </c>
+    </row>
+    <row r="410" s="1" customFormat="1" ht="18.1322" customHeight="1">
+      <c r="A410" s="3" t="s">
+        <v>996</v>
+      </c>
+      <c r="B410" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C410" s="4">
+        <v>44063</v>
+      </c>
+      <c r="D410" s="26" t="s">
+        <v>997</v>
+      </c>
+      <c r="E410" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F410" s="6">
+        <v>2310</v>
+      </c>
+      <c r="G410" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="H410" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I410" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J410" s="7">
+        <v>9.261504e6</v>
+      </c>
+      <c r="K410" s="5" t="s">
+        <v>1017</v>
+      </c>
+      <c r="L410" s="7">
+        <v>2310</v>
+      </c>
+      <c r="M410" s="5" t="s">
+        <v>969</v>
+      </c>
+      <c r="N410" s="8">
+        <v>44084</v>
+      </c>
+      <c r="O410" s="8">
+        <v>44084</v>
+      </c>
+      <c r="P410" s="9">
+        <v>44449</v>
+      </c>
+      <c r="Q410" s="8">
+        <v>44264</v>
+      </c>
+      <c r="R410" s="5" t="s">
+        <v>496</v>
+      </c>
+      <c r="S410" s="5" t="s">
+        <v>497</v>
+      </c>
+      <c r="T410" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U410" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="V410" s="7">
+        <v>1.525727e6</v>
+      </c>
+      <c r="W410" s="5" t="s">
+        <v>1020</v>
+      </c>
+      <c r="X410" s="7">
+        <v>2311</v>
+      </c>
+      <c r="Y410" s="5" t="s">
+        <v>969</v>
+      </c>
+      <c r="Z410" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="AA410" s="3" t="s">
+        <v>972</v>
+      </c>
+      <c r="AB410" s="10">
+        <v>3700</v>
+      </c>
+      <c r="AC410" s="11">
+        <v>14.1</v>
+      </c>
+      <c r="AD410" s="11">
+        <v>14.1</v>
+      </c>
+      <c r="AE410" s="12">
+        <v>52170</v>
+      </c>
+      <c r="AF410" s="12">
+        <v>52170</v>
+      </c>
+    </row>
+    <row r="411" s="1" customFormat="1" ht="18.1322" customHeight="1">
+      <c r="A411" s="13" t="s">
+        <v>996</v>
+      </c>
+      <c r="B411" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C411" s="14">
+        <v>44063</v>
+      </c>
+      <c r="D411" s="25" t="s">
+        <v>997</v>
+      </c>
+      <c r="E411" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F411" s="16">
+        <v>2310</v>
+      </c>
+      <c r="G411" s="13" t="s">
+        <v>969</v>
+      </c>
+      <c r="H411" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I411" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="J411" s="17">
+        <v>9.261506e6</v>
+      </c>
+      <c r="K411" s="15" t="s">
+        <v>1021</v>
+      </c>
+      <c r="L411" s="17">
+        <v>2310</v>
+      </c>
+      <c r="M411" s="15" t="s">
+        <v>969</v>
+      </c>
+      <c r="N411" s="18">
+        <v>44085</v>
+      </c>
+      <c r="O411" s="18">
+        <v>44085</v>
+      </c>
+      <c r="P411" s="19">
+        <v>44449</v>
+      </c>
+      <c r="Q411" s="18">
+        <v>44265</v>
+      </c>
+      <c r="R411" s="15" t="s">
+        <v>466</v>
+      </c>
+      <c r="S411" s="15" t="s">
+        <v>467</v>
+      </c>
+      <c r="T411" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="U411" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="V411" s="17">
+        <v>1.487264e6</v>
+      </c>
+      <c r="W411" s="15" t="s">
+        <v>1022</v>
+      </c>
+      <c r="X411" s="17">
+        <v>2311</v>
+      </c>
+      <c r="Y411" s="15" t="s">
+        <v>969</v>
+      </c>
+      <c r="Z411" s="15" t="s">
+        <v>339</v>
+      </c>
+      <c r="AA411" s="13" t="s">
+        <v>972</v>
+      </c>
+      <c r="AB411" s="21">
+        <v>5600</v>
+      </c>
+      <c r="AC411" s="22">
+        <v>1.899</v>
+      </c>
+      <c r="AD411" s="22">
+        <v>1.899</v>
+      </c>
+      <c r="AE411" s="23">
+        <v>10634.4</v>
+      </c>
+      <c r="AF411" s="23">
+        <v>10634.4</v>
+      </c>
+    </row>
+    <row r="412" s="1" customFormat="1" ht="18.1322" customHeight="1">
+      <c r="A412" s="3" t="s">
+        <v>996</v>
+      </c>
+      <c r="B412" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C412" s="4">
+        <v>44063</v>
+      </c>
+      <c r="D412" s="26" t="s">
+        <v>997</v>
+      </c>
+      <c r="E412" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F412" s="6">
+        <v>2310</v>
+      </c>
+      <c r="G412" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="H412" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I412" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J412" s="7">
+        <v>9.261509e6</v>
+      </c>
+      <c r="K412" s="5" t="s">
+        <v>1023</v>
+      </c>
+      <c r="L412" s="7">
+        <v>2310</v>
+      </c>
+      <c r="M412" s="5" t="s">
+        <v>969</v>
+      </c>
+      <c r="N412" s="8">
+        <v>44085</v>
+      </c>
+      <c r="O412" s="8">
+        <v>44084</v>
+      </c>
+      <c r="P412" s="9">
+        <v>44449</v>
+      </c>
+      <c r="Q412" s="8">
+        <v>44264</v>
+      </c>
+      <c r="R412" s="5" t="s">
+        <v>1024</v>
+      </c>
+      <c r="S412" s="5" t="s">
         <v>1025</v>
       </c>
-      <c r="B405" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C405" s="14">
+      <c r="T412" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U412" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="V412" s="7">
+        <v>1.523619e6</v>
+      </c>
+      <c r="W412" s="5" t="s">
+        <v>1026</v>
+      </c>
+      <c r="X412" s="7">
+        <v>2311</v>
+      </c>
+      <c r="Y412" s="5" t="s">
+        <v>969</v>
+      </c>
+      <c r="Z412" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="AA412" s="3" t="s">
+        <v>972</v>
+      </c>
+      <c r="AB412" s="10">
+        <v>4300</v>
+      </c>
+      <c r="AC412" s="11">
+        <v>12.7</v>
+      </c>
+      <c r="AD412" s="11">
+        <v>12.7</v>
+      </c>
+      <c r="AE412" s="12">
+        <v>54610</v>
+      </c>
+      <c r="AF412" s="12">
+        <v>54610</v>
+      </c>
+    </row>
+    <row r="413" s="1" customFormat="1" ht="18.1322" customHeight="1">
+      <c r="A413" s="13" t="s">
+        <v>996</v>
+      </c>
+      <c r="B413" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C413" s="14">
+        <v>44063</v>
+      </c>
+      <c r="D413" s="25" t="s">
+        <v>997</v>
+      </c>
+      <c r="E413" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F413" s="16">
+        <v>2310</v>
+      </c>
+      <c r="G413" s="13" t="s">
+        <v>969</v>
+      </c>
+      <c r="H413" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I413" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="J413" s="17">
+        <v>9.261509e6</v>
+      </c>
+      <c r="K413" s="15" t="s">
+        <v>1023</v>
+      </c>
+      <c r="L413" s="17">
+        <v>2310</v>
+      </c>
+      <c r="M413" s="15" t="s">
+        <v>969</v>
+      </c>
+      <c r="N413" s="18">
+        <v>44085</v>
+      </c>
+      <c r="O413" s="18">
+        <v>44084</v>
+      </c>
+      <c r="P413" s="19">
+        <v>44449</v>
+      </c>
+      <c r="Q413" s="18">
+        <v>44264</v>
+      </c>
+      <c r="R413" s="15" t="s">
+        <v>1024</v>
+      </c>
+      <c r="S413" s="15" t="s">
+        <v>1025</v>
+      </c>
+      <c r="T413" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="U413" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="V413" s="17">
+        <v>1.523775e6</v>
+      </c>
+      <c r="W413" s="15" t="s">
+        <v>1027</v>
+      </c>
+      <c r="X413" s="17">
+        <v>2311</v>
+      </c>
+      <c r="Y413" s="15" t="s">
+        <v>969</v>
+      </c>
+      <c r="Z413" s="15" t="s">
+        <v>339</v>
+      </c>
+      <c r="AA413" s="13" t="s">
+        <v>972</v>
+      </c>
+      <c r="AB413" s="21">
+        <v>1900</v>
+      </c>
+      <c r="AC413" s="22">
+        <v>35</v>
+      </c>
+      <c r="AD413" s="22">
+        <v>35</v>
+      </c>
+      <c r="AE413" s="23">
+        <v>66500</v>
+      </c>
+      <c r="AF413" s="23">
+        <v>66500</v>
+      </c>
+    </row>
+    <row r="414" s="1" customFormat="1" ht="18.1322" customHeight="1">
+      <c r="A414" s="3" t="s">
+        <v>996</v>
+      </c>
+      <c r="B414" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C414" s="4">
+        <v>44063</v>
+      </c>
+      <c r="D414" s="26" t="s">
+        <v>997</v>
+      </c>
+      <c r="E414" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F414" s="6">
+        <v>2310</v>
+      </c>
+      <c r="G414" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="H414" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I414" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J414" s="7">
+        <v>9.261509e6</v>
+      </c>
+      <c r="K414" s="5" t="s">
+        <v>1023</v>
+      </c>
+      <c r="L414" s="7">
+        <v>2310</v>
+      </c>
+      <c r="M414" s="5" t="s">
+        <v>969</v>
+      </c>
+      <c r="N414" s="8">
+        <v>44085</v>
+      </c>
+      <c r="O414" s="8">
+        <v>44084</v>
+      </c>
+      <c r="P414" s="9">
+        <v>44449</v>
+      </c>
+      <c r="Q414" s="8">
+        <v>44264</v>
+      </c>
+      <c r="R414" s="5" t="s">
+        <v>1024</v>
+      </c>
+      <c r="S414" s="5" t="s">
+        <v>1025</v>
+      </c>
+      <c r="T414" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U414" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="V414" s="7">
+        <v>1.5245e6</v>
+      </c>
+      <c r="W414" s="5" t="s">
+        <v>1028</v>
+      </c>
+      <c r="X414" s="7">
+        <v>2311</v>
+      </c>
+      <c r="Y414" s="5" t="s">
+        <v>969</v>
+      </c>
+      <c r="Z414" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="AA414" s="3" t="s">
+        <v>972</v>
+      </c>
+      <c r="AB414" s="10">
+        <v>2400</v>
+      </c>
+      <c r="AC414" s="11">
+        <v>4.5</v>
+      </c>
+      <c r="AD414" s="11">
+        <v>4.5</v>
+      </c>
+      <c r="AE414" s="12">
+        <v>10800</v>
+      </c>
+      <c r="AF414" s="12">
+        <v>10800</v>
+      </c>
+    </row>
+    <row r="415" s="1" customFormat="1" ht="18.1322" customHeight="1">
+      <c r="A415" s="13" t="s">
+        <v>996</v>
+      </c>
+      <c r="B415" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C415" s="14">
+        <v>44063</v>
+      </c>
+      <c r="D415" s="25" t="s">
+        <v>997</v>
+      </c>
+      <c r="E415" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F415" s="16">
+        <v>2310</v>
+      </c>
+      <c r="G415" s="13" t="s">
+        <v>969</v>
+      </c>
+      <c r="H415" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I415" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="J415" s="17">
+        <v>9.261535e6</v>
+      </c>
+      <c r="K415" s="15" t="s">
+        <v>1029</v>
+      </c>
+      <c r="L415" s="17">
+        <v>2310</v>
+      </c>
+      <c r="M415" s="15" t="s">
+        <v>969</v>
+      </c>
+      <c r="N415" s="18">
+        <v>44088</v>
+      </c>
+      <c r="O415" s="18">
+        <v>44088</v>
+      </c>
+      <c r="P415" s="19">
+        <v>44450</v>
+      </c>
+      <c r="Q415" s="18">
+        <v>44268</v>
+      </c>
+      <c r="R415" s="15" t="s">
+        <v>1030</v>
+      </c>
+      <c r="S415" s="15" t="s">
+        <v>1031</v>
+      </c>
+      <c r="T415" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="U415" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="V415" s="17">
+        <v>1.527878e6</v>
+      </c>
+      <c r="W415" s="15" t="s">
+        <v>1032</v>
+      </c>
+      <c r="X415" s="17">
+        <v>2311</v>
+      </c>
+      <c r="Y415" s="15" t="s">
+        <v>969</v>
+      </c>
+      <c r="Z415" s="15" t="s">
+        <v>339</v>
+      </c>
+      <c r="AA415" s="13" t="s">
+        <v>972</v>
+      </c>
+      <c r="AB415" s="21">
+        <v>500</v>
+      </c>
+      <c r="AC415" s="22">
+        <v>22.95</v>
+      </c>
+      <c r="AD415" s="22">
+        <v>22.95</v>
+      </c>
+      <c r="AE415" s="23">
+        <v>11475</v>
+      </c>
+      <c r="AF415" s="23">
+        <v>11475</v>
+      </c>
+    </row>
+    <row r="416" s="1" customFormat="1" ht="18.1322" customHeight="1">
+      <c r="A416" s="3" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B416" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C416" s="4">
+        <v>43944</v>
+      </c>
+      <c r="D416" s="26" t="s">
+        <v>1034</v>
+      </c>
+      <c r="E416" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F416" s="6">
+        <v>2320</v>
+      </c>
+      <c r="G416" s="3" t="s">
+        <v>1035</v>
+      </c>
+      <c r="H416" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I416" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J416" s="7">
+        <v>0</v>
+      </c>
+      <c r="K416" s="5"/>
+      <c r="L416" s="7"/>
+      <c r="M416" s="5"/>
+      <c r="N416" s="8"/>
+      <c r="O416" s="8"/>
+      <c r="P416" s="9"/>
+      <c r="Q416" s="8"/>
+      <c r="R416" s="5" t="s">
+        <v>1036</v>
+      </c>
+      <c r="S416" s="5" t="s">
+        <v>1037</v>
+      </c>
+      <c r="T416" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U416" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="V416" s="7">
+        <v>1.692143e6</v>
+      </c>
+      <c r="W416" s="5" t="s">
+        <v>559</v>
+      </c>
+      <c r="X416" s="7">
+        <v>2321</v>
+      </c>
+      <c r="Y416" s="5" t="s">
+        <v>1038</v>
+      </c>
+      <c r="Z416" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="AA416" s="3" t="s">
+        <v>557</v>
+      </c>
+      <c r="AB416" s="10">
+        <v>3000</v>
+      </c>
+      <c r="AC416" s="11">
+        <v>8.2</v>
+      </c>
+      <c r="AD416" s="11">
+        <v>8.2</v>
+      </c>
+      <c r="AE416" s="12">
+        <v>24600</v>
+      </c>
+      <c r="AF416" s="12">
+        <v>24600</v>
+      </c>
+    </row>
+    <row r="417" s="1" customFormat="1" ht="18.1322" customHeight="1">
+      <c r="A417" s="13" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B417" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C417" s="14">
+        <v>43944</v>
+      </c>
+      <c r="D417" s="25" t="s">
+        <v>1034</v>
+      </c>
+      <c r="E417" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F417" s="16">
+        <v>2320</v>
+      </c>
+      <c r="G417" s="13" t="s">
+        <v>1035</v>
+      </c>
+      <c r="H417" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I417" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="J417" s="17">
+        <v>0</v>
+      </c>
+      <c r="K417" s="15"/>
+      <c r="L417" s="17"/>
+      <c r="M417" s="15"/>
+      <c r="N417" s="18"/>
+      <c r="O417" s="18"/>
+      <c r="P417" s="19"/>
+      <c r="Q417" s="18"/>
+      <c r="R417" s="15" t="s">
+        <v>1039</v>
+      </c>
+      <c r="S417" s="15" t="s">
+        <v>1040</v>
+      </c>
+      <c r="T417" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="U417" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="V417" s="17">
+        <v>1.143883e6</v>
+      </c>
+      <c r="W417" s="15" t="s">
+        <v>1041</v>
+      </c>
+      <c r="X417" s="17">
+        <v>2321</v>
+      </c>
+      <c r="Y417" s="15" t="s">
+        <v>1038</v>
+      </c>
+      <c r="Z417" s="15" t="s">
+        <v>580</v>
+      </c>
+      <c r="AA417" s="13" t="s">
+        <v>557</v>
+      </c>
+      <c r="AB417" s="21">
+        <v>200000</v>
+      </c>
+      <c r="AC417" s="22">
+        <v>600000e-6</v>
+      </c>
+      <c r="AD417" s="22">
+        <v>600000e-6</v>
+      </c>
+      <c r="AE417" s="23">
+        <v>120000</v>
+      </c>
+      <c r="AF417" s="23">
+        <v>120000</v>
+      </c>
+    </row>
+    <row r="418" s="1" customFormat="1" ht="18.1322" customHeight="1">
+      <c r="A418" s="3" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B418" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C418" s="4">
+        <v>43944</v>
+      </c>
+      <c r="D418" s="26" t="s">
+        <v>1034</v>
+      </c>
+      <c r="E418" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F418" s="6">
+        <v>2320</v>
+      </c>
+      <c r="G418" s="3" t="s">
+        <v>1035</v>
+      </c>
+      <c r="H418" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I418" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J418" s="7">
+        <v>0</v>
+      </c>
+      <c r="K418" s="5"/>
+      <c r="L418" s="7"/>
+      <c r="M418" s="5"/>
+      <c r="N418" s="8"/>
+      <c r="O418" s="8"/>
+      <c r="P418" s="9"/>
+      <c r="Q418" s="8"/>
+      <c r="R418" s="5" t="s">
+        <v>915</v>
+      </c>
+      <c r="S418" s="5" t="s">
+        <v>916</v>
+      </c>
+      <c r="T418" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U418" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="V418" s="7">
+        <v>1.244515e6</v>
+      </c>
+      <c r="W418" s="5" t="s">
+        <v>1042</v>
+      </c>
+      <c r="X418" s="7">
+        <v>2321</v>
+      </c>
+      <c r="Y418" s="5" t="s">
+        <v>1038</v>
+      </c>
+      <c r="Z418" s="5" t="s">
+        <v>580</v>
+      </c>
+      <c r="AA418" s="3" t="s">
+        <v>557</v>
+      </c>
+      <c r="AB418" s="10">
+        <v>50</v>
+      </c>
+      <c r="AC418" s="11">
+        <v>20.1</v>
+      </c>
+      <c r="AD418" s="11">
+        <v>20.1</v>
+      </c>
+      <c r="AE418" s="12">
+        <v>1005</v>
+      </c>
+      <c r="AF418" s="12">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="419" s="1" customFormat="1" ht="18.1322" customHeight="1">
+      <c r="A419" s="13" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B419" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C419" s="14">
+        <v>43944</v>
+      </c>
+      <c r="D419" s="25" t="s">
+        <v>1034</v>
+      </c>
+      <c r="E419" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F419" s="16">
+        <v>2320</v>
+      </c>
+      <c r="G419" s="13" t="s">
+        <v>1035</v>
+      </c>
+      <c r="H419" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I419" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="J419" s="17">
+        <v>0</v>
+      </c>
+      <c r="K419" s="15"/>
+      <c r="L419" s="17"/>
+      <c r="M419" s="15"/>
+      <c r="N419" s="18"/>
+      <c r="O419" s="18"/>
+      <c r="P419" s="19"/>
+      <c r="Q419" s="18"/>
+      <c r="R419" s="15" t="s">
+        <v>1043</v>
+      </c>
+      <c r="S419" s="15" t="s">
+        <v>1044</v>
+      </c>
+      <c r="T419" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="U419" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="V419" s="17">
+        <v>1.244108e6</v>
+      </c>
+      <c r="W419" s="15" t="s">
+        <v>1045</v>
+      </c>
+      <c r="X419" s="17">
+        <v>2321</v>
+      </c>
+      <c r="Y419" s="15" t="s">
+        <v>1038</v>
+      </c>
+      <c r="Z419" s="15" t="s">
+        <v>580</v>
+      </c>
+      <c r="AA419" s="13" t="s">
+        <v>557</v>
+      </c>
+      <c r="AB419" s="21">
+        <v>90</v>
+      </c>
+      <c r="AC419" s="22">
+        <v>358.24</v>
+      </c>
+      <c r="AD419" s="22">
+        <v>358.24</v>
+      </c>
+      <c r="AE419" s="23">
+        <v>32241.6</v>
+      </c>
+      <c r="AF419" s="23">
+        <v>32241.6</v>
+      </c>
+    </row>
+    <row r="420" s="1" customFormat="1" ht="18.1322" customHeight="1">
+      <c r="A420" s="3" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B420" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C420" s="4">
+        <v>43944</v>
+      </c>
+      <c r="D420" s="26" t="s">
+        <v>1034</v>
+      </c>
+      <c r="E420" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F420" s="6">
+        <v>2320</v>
+      </c>
+      <c r="G420" s="3" t="s">
+        <v>1035</v>
+      </c>
+      <c r="H420" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I420" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J420" s="7">
+        <v>0</v>
+      </c>
+      <c r="K420" s="5"/>
+      <c r="L420" s="7"/>
+      <c r="M420" s="5"/>
+      <c r="N420" s="8"/>
+      <c r="O420" s="8"/>
+      <c r="P420" s="9"/>
+      <c r="Q420" s="8"/>
+      <c r="R420" s="5" t="s">
+        <v>1043</v>
+      </c>
+      <c r="S420" s="5" t="s">
+        <v>1044</v>
+      </c>
+      <c r="T420" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U420" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="V420" s="7">
+        <v>1.244507e6</v>
+      </c>
+      <c r="W420" s="5" t="s">
+        <v>1046</v>
+      </c>
+      <c r="X420" s="7">
+        <v>2321</v>
+      </c>
+      <c r="Y420" s="5" t="s">
+        <v>1038</v>
+      </c>
+      <c r="Z420" s="5" t="s">
+        <v>580</v>
+      </c>
+      <c r="AA420" s="3" t="s">
+        <v>557</v>
+      </c>
+      <c r="AB420" s="10">
+        <v>50</v>
+      </c>
+      <c r="AC420" s="11">
+        <v>34.9</v>
+      </c>
+      <c r="AD420" s="11">
+        <v>34.9</v>
+      </c>
+      <c r="AE420" s="12">
+        <v>1745</v>
+      </c>
+      <c r="AF420" s="12">
+        <v>1745</v>
+      </c>
+    </row>
+    <row r="421" s="1" customFormat="1" ht="18.1322" customHeight="1">
+      <c r="A421" s="13" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B421" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C421" s="14">
+        <v>43944</v>
+      </c>
+      <c r="D421" s="25" t="s">
+        <v>1034</v>
+      </c>
+      <c r="E421" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F421" s="16">
+        <v>2320</v>
+      </c>
+      <c r="G421" s="13" t="s">
+        <v>1035</v>
+      </c>
+      <c r="H421" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I421" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="J421" s="17">
+        <v>0</v>
+      </c>
+      <c r="K421" s="15"/>
+      <c r="L421" s="17"/>
+      <c r="M421" s="15"/>
+      <c r="N421" s="18"/>
+      <c r="O421" s="18"/>
+      <c r="P421" s="19"/>
+      <c r="Q421" s="18"/>
+      <c r="R421" s="15" t="s">
+        <v>1043</v>
+      </c>
+      <c r="S421" s="15" t="s">
+        <v>1044</v>
+      </c>
+      <c r="T421" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="U421" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="V421" s="17">
+        <v>1.257587e6</v>
+      </c>
+      <c r="W421" s="15" t="s">
+        <v>1047</v>
+      </c>
+      <c r="X421" s="17">
+        <v>2321</v>
+      </c>
+      <c r="Y421" s="15" t="s">
+        <v>1038</v>
+      </c>
+      <c r="Z421" s="15" t="s">
+        <v>580</v>
+      </c>
+      <c r="AA421" s="13" t="s">
+        <v>557</v>
+      </c>
+      <c r="AB421" s="21">
+        <v>80000</v>
+      </c>
+      <c r="AC421" s="22">
+        <v>390000e-6</v>
+      </c>
+      <c r="AD421" s="22">
+        <v>390000e-6</v>
+      </c>
+      <c r="AE421" s="23">
+        <v>31200</v>
+      </c>
+      <c r="AF421" s="23">
+        <v>31200</v>
+      </c>
+    </row>
+    <row r="422" s="1" customFormat="1" ht="18.1322" customHeight="1">
+      <c r="A422" s="3" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B422" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C422" s="4">
+        <v>43944</v>
+      </c>
+      <c r="D422" s="26" t="s">
+        <v>1034</v>
+      </c>
+      <c r="E422" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F422" s="6">
+        <v>2320</v>
+      </c>
+      <c r="G422" s="3" t="s">
+        <v>1035</v>
+      </c>
+      <c r="H422" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I422" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J422" s="7">
+        <v>0</v>
+      </c>
+      <c r="K422" s="5"/>
+      <c r="L422" s="7"/>
+      <c r="M422" s="5"/>
+      <c r="N422" s="8"/>
+      <c r="O422" s="8"/>
+      <c r="P422" s="9"/>
+      <c r="Q422" s="8"/>
+      <c r="R422" s="5" t="s">
+        <v>1043</v>
+      </c>
+      <c r="S422" s="5" t="s">
+        <v>1044</v>
+      </c>
+      <c r="T422" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U422" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="V422" s="7">
+        <v>1.257625e6</v>
+      </c>
+      <c r="W422" s="5" t="s">
+        <v>1048</v>
+      </c>
+      <c r="X422" s="7">
+        <v>2321</v>
+      </c>
+      <c r="Y422" s="5" t="s">
+        <v>1038</v>
+      </c>
+      <c r="Z422" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="AA422" s="3" t="s">
+        <v>557</v>
+      </c>
+      <c r="AB422" s="10">
+        <v>90</v>
+      </c>
+      <c r="AC422" s="11">
+        <v>351</v>
+      </c>
+      <c r="AD422" s="11">
+        <v>351</v>
+      </c>
+      <c r="AE422" s="12">
+        <v>31590</v>
+      </c>
+      <c r="AF422" s="12">
+        <v>31590</v>
+      </c>
+    </row>
+    <row r="423" s="1" customFormat="1" ht="18.1322" customHeight="1">
+      <c r="A423" s="13" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B423" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C423" s="14">
+        <v>43944</v>
+      </c>
+      <c r="D423" s="25" t="s">
+        <v>1034</v>
+      </c>
+      <c r="E423" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F423" s="16">
+        <v>2320</v>
+      </c>
+      <c r="G423" s="13" t="s">
+        <v>1035</v>
+      </c>
+      <c r="H423" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I423" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="J423" s="17">
+        <v>0</v>
+      </c>
+      <c r="K423" s="15"/>
+      <c r="L423" s="17"/>
+      <c r="M423" s="15"/>
+      <c r="N423" s="18"/>
+      <c r="O423" s="18"/>
+      <c r="P423" s="19"/>
+      <c r="Q423" s="18"/>
+      <c r="R423" s="15" t="s">
+        <v>1043</v>
+      </c>
+      <c r="S423" s="15" t="s">
+        <v>1044</v>
+      </c>
+      <c r="T423" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="U423" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="V423" s="17">
+        <v>1.258699e6</v>
+      </c>
+      <c r="W423" s="15" t="s">
+        <v>1049</v>
+      </c>
+      <c r="X423" s="17">
+        <v>2321</v>
+      </c>
+      <c r="Y423" s="15" t="s">
+        <v>1038</v>
+      </c>
+      <c r="Z423" s="15" t="s">
+        <v>580</v>
+      </c>
+      <c r="AA423" s="13" t="s">
+        <v>557</v>
+      </c>
+      <c r="AB423" s="21">
+        <v>2000</v>
+      </c>
+      <c r="AC423" s="22">
+        <v>1.39</v>
+      </c>
+      <c r="AD423" s="22">
+        <v>1.39</v>
+      </c>
+      <c r="AE423" s="23">
+        <v>2780</v>
+      </c>
+      <c r="AF423" s="23">
+        <v>2780</v>
+      </c>
+    </row>
+    <row r="424" s="1" customFormat="1" ht="18.1322" customHeight="1">
+      <c r="A424" s="3" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B424" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C424" s="4">
+        <v>43944</v>
+      </c>
+      <c r="D424" s="26" t="s">
+        <v>1034</v>
+      </c>
+      <c r="E424" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F424" s="6">
+        <v>2320</v>
+      </c>
+      <c r="G424" s="3" t="s">
+        <v>1035</v>
+      </c>
+      <c r="H424" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I424" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J424" s="7">
+        <v>0</v>
+      </c>
+      <c r="K424" s="5"/>
+      <c r="L424" s="7"/>
+      <c r="M424" s="5"/>
+      <c r="N424" s="8"/>
+      <c r="O424" s="8"/>
+      <c r="P424" s="9"/>
+      <c r="Q424" s="8"/>
+      <c r="R424" s="5" t="s">
+        <v>1043</v>
+      </c>
+      <c r="S424" s="5" t="s">
+        <v>1044</v>
+      </c>
+      <c r="T424" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U424" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="V424" s="7">
+        <v>1.259784e6</v>
+      </c>
+      <c r="W424" s="5" t="s">
+        <v>1050</v>
+      </c>
+      <c r="X424" s="7">
+        <v>2321</v>
+      </c>
+      <c r="Y424" s="5" t="s">
+        <v>1038</v>
+      </c>
+      <c r="Z424" s="5" t="s">
+        <v>580</v>
+      </c>
+      <c r="AA424" s="3" t="s">
+        <v>557</v>
+      </c>
+      <c r="AB424" s="10">
+        <v>3000</v>
+      </c>
+      <c r="AC424" s="11">
+        <v>600000e-6</v>
+      </c>
+      <c r="AD424" s="11">
+        <v>600000e-6</v>
+      </c>
+      <c r="AE424" s="12">
+        <v>1800</v>
+      </c>
+      <c r="AF424" s="12">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="425" s="1" customFormat="1" ht="18.1322" customHeight="1">
+      <c r="A425" s="13" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B425" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C425" s="14">
+        <v>43944</v>
+      </c>
+      <c r="D425" s="25" t="s">
+        <v>1034</v>
+      </c>
+      <c r="E425" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F425" s="16">
+        <v>2320</v>
+      </c>
+      <c r="G425" s="13" t="s">
+        <v>1035</v>
+      </c>
+      <c r="H425" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I425" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="J425" s="17">
+        <v>0</v>
+      </c>
+      <c r="K425" s="15"/>
+      <c r="L425" s="17"/>
+      <c r="M425" s="15"/>
+      <c r="N425" s="18"/>
+      <c r="O425" s="18"/>
+      <c r="P425" s="19"/>
+      <c r="Q425" s="18"/>
+      <c r="R425" s="15" t="s">
+        <v>1043</v>
+      </c>
+      <c r="S425" s="15" t="s">
+        <v>1044</v>
+      </c>
+      <c r="T425" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="U425" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="V425" s="17">
+        <v>1.259792e6</v>
+      </c>
+      <c r="W425" s="15" t="s">
+        <v>1051</v>
+      </c>
+      <c r="X425" s="17">
+        <v>2321</v>
+      </c>
+      <c r="Y425" s="15" t="s">
+        <v>1038</v>
+      </c>
+      <c r="Z425" s="15" t="s">
+        <v>580</v>
+      </c>
+      <c r="AA425" s="13" t="s">
+        <v>557</v>
+      </c>
+      <c r="AB425" s="21">
+        <v>80</v>
+      </c>
+      <c r="AC425" s="22">
+        <v>15.35</v>
+      </c>
+      <c r="AD425" s="22">
+        <v>15.35</v>
+      </c>
+      <c r="AE425" s="23">
+        <v>1228</v>
+      </c>
+      <c r="AF425" s="23">
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="426" s="1" customFormat="1" ht="18.1322" customHeight="1">
+      <c r="A426" s="3" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B426" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C426" s="4">
+        <v>43944</v>
+      </c>
+      <c r="D426" s="26" t="s">
+        <v>1034</v>
+      </c>
+      <c r="E426" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F426" s="6">
+        <v>2320</v>
+      </c>
+      <c r="G426" s="3" t="s">
+        <v>1035</v>
+      </c>
+      <c r="H426" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I426" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J426" s="7">
+        <v>0</v>
+      </c>
+      <c r="K426" s="5"/>
+      <c r="L426" s="7"/>
+      <c r="M426" s="5"/>
+      <c r="N426" s="8"/>
+      <c r="O426" s="8"/>
+      <c r="P426" s="9"/>
+      <c r="Q426" s="8"/>
+      <c r="R426" s="5" t="s">
+        <v>1043</v>
+      </c>
+      <c r="S426" s="5" t="s">
+        <v>1044</v>
+      </c>
+      <c r="T426" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U426" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="V426" s="7">
+        <v>1.260669e6</v>
+      </c>
+      <c r="W426" s="5" t="s">
+        <v>1052</v>
+      </c>
+      <c r="X426" s="7">
+        <v>2321</v>
+      </c>
+      <c r="Y426" s="5" t="s">
+        <v>1038</v>
+      </c>
+      <c r="Z426" s="5" t="s">
+        <v>580</v>
+      </c>
+      <c r="AA426" s="3" t="s">
+        <v>557</v>
+      </c>
+      <c r="AB426" s="10">
+        <v>1000</v>
+      </c>
+      <c r="AC426" s="11">
+        <v>1.49</v>
+      </c>
+      <c r="AD426" s="11">
+        <v>1.49</v>
+      </c>
+      <c r="AE426" s="12">
+        <v>1490</v>
+      </c>
+      <c r="AF426" s="12">
+        <v>1490</v>
+      </c>
+    </row>
+    <row r="427" s="1" customFormat="1" ht="18.1322" customHeight="1">
+      <c r="A427" s="13" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B427" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C427" s="14">
+        <v>43944</v>
+      </c>
+      <c r="D427" s="25" t="s">
+        <v>1034</v>
+      </c>
+      <c r="E427" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F427" s="16">
+        <v>2320</v>
+      </c>
+      <c r="G427" s="13" t="s">
+        <v>1035</v>
+      </c>
+      <c r="H427" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I427" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="J427" s="17">
+        <v>0</v>
+      </c>
+      <c r="K427" s="15"/>
+      <c r="L427" s="17"/>
+      <c r="M427" s="15"/>
+      <c r="N427" s="18"/>
+      <c r="O427" s="18"/>
+      <c r="P427" s="19"/>
+      <c r="Q427" s="18"/>
+      <c r="R427" s="15" t="s">
+        <v>1043</v>
+      </c>
+      <c r="S427" s="15" t="s">
+        <v>1044</v>
+      </c>
+      <c r="T427" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="U427" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="V427" s="17">
+        <v>1.260677e6</v>
+      </c>
+      <c r="W427" s="15" t="s">
+        <v>1053</v>
+      </c>
+      <c r="X427" s="17">
+        <v>2321</v>
+      </c>
+      <c r="Y427" s="15" t="s">
+        <v>1038</v>
+      </c>
+      <c r="Z427" s="15" t="s">
+        <v>580</v>
+      </c>
+      <c r="AA427" s="13" t="s">
+        <v>557</v>
+      </c>
+      <c r="AB427" s="21">
+        <v>3000</v>
+      </c>
+      <c r="AC427" s="22">
+        <v>1.59</v>
+      </c>
+      <c r="AD427" s="22">
+        <v>1.59</v>
+      </c>
+      <c r="AE427" s="23">
+        <v>4770</v>
+      </c>
+      <c r="AF427" s="23">
+        <v>4770</v>
+      </c>
+    </row>
+    <row r="428" s="1" customFormat="1" ht="18.1322" customHeight="1">
+      <c r="A428" s="3" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B428" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C428" s="4">
+        <v>43944</v>
+      </c>
+      <c r="D428" s="26" t="s">
+        <v>1034</v>
+      </c>
+      <c r="E428" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F428" s="6">
+        <v>2320</v>
+      </c>
+      <c r="G428" s="3" t="s">
+        <v>1035</v>
+      </c>
+      <c r="H428" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I428" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J428" s="7">
+        <v>0</v>
+      </c>
+      <c r="K428" s="5"/>
+      <c r="L428" s="7"/>
+      <c r="M428" s="5"/>
+      <c r="N428" s="8"/>
+      <c r="O428" s="8"/>
+      <c r="P428" s="9"/>
+      <c r="Q428" s="8"/>
+      <c r="R428" s="5" t="s">
+        <v>1043</v>
+      </c>
+      <c r="S428" s="5" t="s">
+        <v>1044</v>
+      </c>
+      <c r="T428" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U428" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="V428" s="7">
+        <v>1.260731e6</v>
+      </c>
+      <c r="W428" s="24" t="s">
+        <v>1054</v>
+      </c>
+      <c r="X428" s="7">
+        <v>2321</v>
+      </c>
+      <c r="Y428" s="5" t="s">
+        <v>1038</v>
+      </c>
+      <c r="Z428" s="5" t="s">
+        <v>580</v>
+      </c>
+      <c r="AA428" s="3" t="s">
+        <v>557</v>
+      </c>
+      <c r="AB428" s="10">
+        <v>60</v>
+      </c>
+      <c r="AC428" s="11">
+        <v>271.97</v>
+      </c>
+      <c r="AD428" s="11">
+        <v>271.97</v>
+      </c>
+      <c r="AE428" s="12">
+        <v>16318.2</v>
+      </c>
+      <c r="AF428" s="12">
+        <v>16318.2</v>
+      </c>
+    </row>
+    <row r="429" s="1" customFormat="1" ht="18.1322" customHeight="1">
+      <c r="A429" s="13" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B429" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C429" s="14">
+        <v>43944</v>
+      </c>
+      <c r="D429" s="25" t="s">
+        <v>1034</v>
+      </c>
+      <c r="E429" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F429" s="16">
+        <v>2320</v>
+      </c>
+      <c r="G429" s="13" t="s">
+        <v>1035</v>
+      </c>
+      <c r="H429" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I429" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="J429" s="17">
+        <v>0</v>
+      </c>
+      <c r="K429" s="15"/>
+      <c r="L429" s="17"/>
+      <c r="M429" s="15"/>
+      <c r="N429" s="18"/>
+      <c r="O429" s="18"/>
+      <c r="P429" s="19"/>
+      <c r="Q429" s="18"/>
+      <c r="R429" s="15" t="s">
+        <v>1043</v>
+      </c>
+      <c r="S429" s="15" t="s">
+        <v>1044</v>
+      </c>
+      <c r="T429" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="U429" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="V429" s="17">
+        <v>1.687115e6</v>
+      </c>
+      <c r="W429" s="15" t="s">
+        <v>1055</v>
+      </c>
+      <c r="X429" s="17">
+        <v>2321</v>
+      </c>
+      <c r="Y429" s="15" t="s">
+        <v>1038</v>
+      </c>
+      <c r="Z429" s="15" t="s">
+        <v>580</v>
+      </c>
+      <c r="AA429" s="13" t="s">
+        <v>557</v>
+      </c>
+      <c r="AB429" s="21">
+        <v>60</v>
+      </c>
+      <c r="AC429" s="22">
+        <v>16.65</v>
+      </c>
+      <c r="AD429" s="22">
+        <v>16.65</v>
+      </c>
+      <c r="AE429" s="23">
+        <v>999</v>
+      </c>
+      <c r="AF429" s="23">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="430" s="1" customFormat="1" ht="18.1322" customHeight="1">
+      <c r="A430" s="3" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B430" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C430" s="4">
+        <v>43944</v>
+      </c>
+      <c r="D430" s="26" t="s">
+        <v>1034</v>
+      </c>
+      <c r="E430" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F430" s="6">
+        <v>2320</v>
+      </c>
+      <c r="G430" s="3" t="s">
+        <v>1035</v>
+      </c>
+      <c r="H430" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I430" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J430" s="7">
+        <v>0</v>
+      </c>
+      <c r="K430" s="5"/>
+      <c r="L430" s="7"/>
+      <c r="M430" s="5"/>
+      <c r="N430" s="8"/>
+      <c r="O430" s="8"/>
+      <c r="P430" s="9"/>
+      <c r="Q430" s="8"/>
+      <c r="R430" s="5" t="s">
+        <v>1056</v>
+      </c>
+      <c r="S430" s="5" t="s">
+        <v>1057</v>
+      </c>
+      <c r="T430" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U430" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="V430" s="7">
+        <v>1.257463e6</v>
+      </c>
+      <c r="W430" s="5" t="s">
+        <v>1058</v>
+      </c>
+      <c r="X430" s="7">
+        <v>2321</v>
+      </c>
+      <c r="Y430" s="5" t="s">
+        <v>1038</v>
+      </c>
+      <c r="Z430" s="5" t="s">
+        <v>580</v>
+      </c>
+      <c r="AA430" s="3" t="s">
+        <v>557</v>
+      </c>
+      <c r="AB430" s="10">
+        <v>200</v>
+      </c>
+      <c r="AC430" s="11">
+        <v>34.2</v>
+      </c>
+      <c r="AD430" s="11">
+        <v>34.2</v>
+      </c>
+      <c r="AE430" s="12">
+        <v>6840</v>
+      </c>
+      <c r="AF430" s="12">
+        <v>6840</v>
+      </c>
+    </row>
+    <row r="431" s="1" customFormat="1" ht="18.1322" customHeight="1">
+      <c r="A431" s="13" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B431" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C431" s="14">
+        <v>44012</v>
+      </c>
+      <c r="D431" s="15" t="s">
+        <v>1060</v>
+      </c>
+      <c r="E431" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F431" s="16">
+        <v>2320</v>
+      </c>
+      <c r="G431" s="13" t="s">
+        <v>1035</v>
+      </c>
+      <c r="H431" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I431" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="J431" s="17">
+        <v>0</v>
+      </c>
+      <c r="K431" s="15"/>
+      <c r="L431" s="17"/>
+      <c r="M431" s="15"/>
+      <c r="N431" s="18"/>
+      <c r="O431" s="18"/>
+      <c r="P431" s="19"/>
+      <c r="Q431" s="18"/>
+      <c r="R431" s="15" t="s">
+        <v>540</v>
+      </c>
+      <c r="S431" s="15" t="s">
+        <v>541</v>
+      </c>
+      <c r="T431" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="U431" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="V431" s="17">
+        <v>1.408623e6</v>
+      </c>
+      <c r="W431" s="15" t="s">
+        <v>1061</v>
+      </c>
+      <c r="X431" s="17">
+        <v>2321</v>
+      </c>
+      <c r="Y431" s="15" t="s">
+        <v>1038</v>
+      </c>
+      <c r="Z431" s="15" t="s">
+        <v>422</v>
+      </c>
+      <c r="AA431" s="13" t="s">
+        <v>557</v>
+      </c>
+      <c r="AB431" s="21">
+        <v>2000</v>
+      </c>
+      <c r="AC431" s="22">
+        <v>18.69</v>
+      </c>
+      <c r="AD431" s="22">
+        <v>14.95</v>
+      </c>
+      <c r="AE431" s="23">
+        <v>37380</v>
+      </c>
+      <c r="AF431" s="23">
+        <v>29900</v>
+      </c>
+    </row>
+    <row r="432" s="1" customFormat="1" ht="18.1322" customHeight="1">
+      <c r="A432" s="3" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B432" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C432" s="4">
         <v>44034</v>
       </c>
-      <c r="D405" s="25" t="s">
-        <v>1026</v>
-      </c>
-      <c r="E405" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="F405" s="16">
+      <c r="D432" s="26" t="s">
+        <v>1063</v>
+      </c>
+      <c r="E432" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F432" s="6">
         <v>2320</v>
       </c>
-      <c r="G405" s="13" t="s">
-        <v>998</v>
-      </c>
-      <c r="H405" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="I405" s="13" t="s">
-        <v>1027</v>
-      </c>
-      <c r="J405" s="17">
+      <c r="G432" s="3" t="s">
+        <v>1035</v>
+      </c>
+      <c r="H432" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I432" s="3" t="s">
+        <v>1064</v>
+      </c>
+      <c r="J432" s="7">
         <v>9.260962e6</v>
       </c>
-      <c r="K405" s="15" t="s">
-        <v>1028</v>
-      </c>
-      <c r="L405" s="17">
+      <c r="K432" s="5" t="s">
+        <v>1065</v>
+      </c>
+      <c r="L432" s="7">
         <v>2320</v>
       </c>
-      <c r="M405" s="15" t="s">
-        <v>998</v>
-      </c>
-      <c r="N405" s="18">
+      <c r="M432" s="5" t="s">
+        <v>1035</v>
+      </c>
+      <c r="N432" s="8">
         <v>44056</v>
       </c>
-      <c r="O405" s="18">
+      <c r="O432" s="8">
         <v>44056</v>
       </c>
-      <c r="P405" s="19">
+      <c r="P432" s="9">
         <v>44240</v>
       </c>
-      <c r="Q405" s="18">
+      <c r="Q432" s="8">
         <v>44240</v>
       </c>
-      <c r="R405" s="15" t="s">
+      <c r="R432" s="5" t="s">
         <v>841</v>
       </c>
-      <c r="S405" s="15" t="s">
+      <c r="S432" s="5" t="s">
         <v>842</v>
       </c>
-      <c r="T405" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="U405" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="V405" s="17">
+      <c r="T432" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U432" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="V432" s="7">
         <v>1.758276e6</v>
       </c>
-      <c r="W405" s="15" t="s">
+      <c r="W432" s="5" t="s">
         <v>843</v>
       </c>
-      <c r="X405" s="17">
+      <c r="X432" s="7">
         <v>2321</v>
       </c>
-      <c r="Y405" s="15" t="s">
-        <v>1001</v>
-      </c>
-      <c r="Z405" s="15" t="s">
+      <c r="Y432" s="5" t="s">
+        <v>1038</v>
+      </c>
+      <c r="Z432" s="5" t="s">
         <v>428</v>
       </c>
-      <c r="AA405" s="13" t="s">
+      <c r="AA432" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="AB405" s="21">
+      <c r="AB432" s="10">
         <v>7000</v>
       </c>
-      <c r="AC405" s="22">
+      <c r="AC432" s="11">
         <v>34.54</v>
       </c>
-      <c r="AD405" s="22">
+      <c r="AD432" s="11">
         <v>34.536</v>
       </c>
-      <c r="AE405" s="23">
+      <c r="AE432" s="12">
         <v>241780</v>
       </c>
-      <c r="AF405" s="23">
+      <c r="AF432" s="12">
         <v>241752</v>
       </c>
     </row>
-    <row r="406" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
+    <row r="433" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
   </sheetData>
   <pageSetup paperSize="9" scale="100" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>

<commit_message>
atualiza processo da UNIMONTES
</commit_message>
<xml_diff>
--- a/data-raw/compras-coronavirus.xlsx
+++ b/data-raw/compras-coronavirus.xlsx
@@ -8,7 +8,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7083" uniqueCount="1120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7134" uniqueCount="1132">
   <si>
     <t>Número Processo -  Formatado</t>
   </si>
@@ -1993,7 +1993,7 @@
     <t>VASSOURA -  TIPO DAS CERDAS: PIACAVA NATURAL; LARGURA BASE: NUMERO 5, MINIMO 13 CM DE BASE; MATERIAL BASE: MADEIRA; MATERIAL CABO: MADEIRA REVESTIDO PLASTICO; COMPRIMENTO CABO: 1,50 M;</t>
   </si>
   <si>
-    <t>DESINFETANTE DE USO GERAL -  TIPO: CONCENTRADO; ACAO PRINCIPAL: BACTERICIDA E GERMICIDA; PRINCIPIO ATIVO: QUATERNARIO DE AMONIO; COMPOSICAO BASICA: TENSOATIVOS CATIONICOS, DILUICAO 1/300; FRAGRANCIA: CONFORME SOLICITADO PELO ORGAO/ENTIDADE; APRESENTACAO: FRASCO 5 L;</t>
+    <t>DESINFETANTE  -  TIPO: CONCENTRADO; ACAO PRINCIPAL: BACTERICIDA E GERMICIDA; PRINCIPIO ATIVO: QUATERNARIO DE AMONIO; COMPOSICAO BASICA: TENSOATIVOS CATIONICOS; DILUICAO: 1:300; FRAGRANCIA: CONFORME SOLICITADO PELO ORGAO/ENTIDADE; APRESENTACAO: FRASCO 5 L;</t>
   </si>
   <si>
     <t>1401269 000049/2020</t>
@@ -3278,6 +3278,42 @@
   </si>
   <si>
     <t>ARGIPRESSINA - PRINCIPIO ATIVO: ARGIPRESSINA; CONCENTRACAO/DOSAGEM: 20 U/ML; FORMA FARMACEUTICA: SOLUCAO INJETAVEL; APRESENTACAO: AMPOLA 1 ML; COMPONENTE: .;</t>
+  </si>
+  <si>
+    <t>2311076 000663/2020</t>
+  </si>
+  <si>
+    <t>EQUIPAMENTOS PARA HEMODIALISE</t>
+  </si>
+  <si>
+    <t>https://www1.compras.mg.gov.br/contrato/gestaocontratos/arquivosContrato.html?idContrato=165468</t>
+  </si>
+  <si>
+    <t>01.440.590/0001-36</t>
+  </si>
+  <si>
+    <t>FRESENIUS MEDICAL CARE LTDA</t>
+  </si>
+  <si>
+    <t>UNIDADE PARA HEMODIALISE - CONTROLE: TOTALMENTE MICROPROCESSADO; PAINEL DE COMANDO: TELA DE CRISTAL LIQUIDO C/INFORMACOES EM PORTUGUES; FLUXO: VARIACAO DO FLUXO DE DIALISATO:300 A 800 ML/MINUTO; MONITORACAO:  PRESSAO DAS LINHAS ARTERIAL E VENOSA DO SISTEMA E; INTERFACE: --; TENSAO/FREQUENCIA: EM REDE 60 HZ, 127 OU 220 VOLTS;</t>
+  </si>
+  <si>
+    <t>https://www1.compras.mg.gov.br/contrato/gestaocontratos/arquivosContrato.html?idContrato=165457</t>
+  </si>
+  <si>
+    <t>36.078.798/0001-31</t>
+  </si>
+  <si>
+    <t>IPABRAS INDUSTRIA E COMERCIO LTDA</t>
+  </si>
+  <si>
+    <t>SISTEMA DE OSMOSE REVERSA - APLICACAO: TRATAR AGUAS PROBLEMATICAS COM ALTA CONDUTIVIDADE; CAPACIDADE DE VAZAO: 60 LITROS/HORA; COMPONENTE (1): CONDUTIVIMETRO DIGITAL COM DISPLAY LCD; COMPONENTE (2): HORIMETRO TOTAL; ALIMENTACAO: BIVOLT AUTOMATICO, 127V-240V;</t>
+  </si>
+  <si>
+    <t>EQUIPAMENTOS E ARTIGOS  PARA PURIFICACAO E TRATAMENTO  DE AGUA E TRATAMENTO DE ESGOTO</t>
+  </si>
+  <si>
+    <t>FILTRO ABRANDADOR - MATERIA-PRIMA: ACO INOX E TERMOPLASTICO; VAZAO: 200 LITROS/HORA; CICLO: 200 LITROS/HORA; TEMPERATURA: NOMINAL FORNECIDA; VOLUME: 200 LITROS/HORA; DIMENSOES: APROXIMADAMENTE 120CM(ALT)X 50CM(LARG)X 30CM(PROF);</t>
   </si>
   <si>
     <t>2320310 000127/2020</t>
@@ -3573,7 +3609,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AF448"/>
+  <dimension ref="A1:AF451"/>
   <cols>
     <col min="1" max="1" width="27.8093" customWidth="1"/>
     <col min="2" max="2" width="23.8165" customWidth="1"/>
@@ -25697,7 +25733,7 @@
       <c r="V248" s="7">
         <v>1.698915e6</v>
       </c>
-      <c r="W248" s="24" t="s">
+      <c r="W248" s="5" t="s">
         <v>659</v>
       </c>
       <c r="X248" s="7">
@@ -42334,19 +42370,19 @@
         <v>33</v>
       </c>
       <c r="C431" s="14">
-        <v>43944</v>
-      </c>
-      <c r="D431" s="26" t="s">
+        <v>44125</v>
+      </c>
+      <c r="D431" s="15" t="s">
         <v>1088</v>
       </c>
       <c r="E431" s="15" t="s">
         <v>33</v>
       </c>
       <c r="F431" s="16">
-        <v>2320</v>
+        <v>2310</v>
       </c>
       <c r="G431" s="13" t="s">
-        <v>1089</v>
+        <v>1019</v>
       </c>
       <c r="H431" s="13" t="s">
         <v>36</v>
@@ -42355,15 +42391,29 @@
         <v>37</v>
       </c>
       <c r="J431" s="17">
-        <v>0</v>
-      </c>
-      <c r="K431" s="15"/>
-      <c r="L431" s="17"/>
-      <c r="M431" s="15"/>
-      <c r="N431" s="18"/>
-      <c r="O431" s="18"/>
-      <c r="P431" s="19"/>
-      <c r="Q431" s="18"/>
+        <v>9.263559e6</v>
+      </c>
+      <c r="K431" s="15" t="s">
+        <v>1089</v>
+      </c>
+      <c r="L431" s="17">
+        <v>2310</v>
+      </c>
+      <c r="M431" s="15" t="s">
+        <v>1019</v>
+      </c>
+      <c r="N431" s="18">
+        <v>44161</v>
+      </c>
+      <c r="O431" s="18">
+        <v>44161</v>
+      </c>
+      <c r="P431" s="19">
+        <v>44891</v>
+      </c>
+      <c r="Q431" s="18">
+        <v>44341</v>
+      </c>
       <c r="R431" s="15" t="s">
         <v>1090</v>
       </c>
@@ -42377,37 +42427,37 @@
         <v>33</v>
       </c>
       <c r="V431" s="17">
-        <v>1.692143e6</v>
-      </c>
-      <c r="W431" s="15" t="s">
-        <v>583</v>
+        <v>1.427423e6</v>
+      </c>
+      <c r="W431" s="20" t="s">
+        <v>1092</v>
       </c>
       <c r="X431" s="17">
-        <v>2321</v>
+        <v>2311</v>
       </c>
       <c r="Y431" s="15" t="s">
-        <v>1092</v>
+        <v>1019</v>
       </c>
       <c r="Z431" s="15" t="s">
-        <v>347</v>
+        <v>142</v>
       </c>
       <c r="AA431" s="13" t="s">
-        <v>581</v>
+        <v>1022</v>
       </c>
       <c r="AB431" s="21">
-        <v>3000</v>
+        <v>2</v>
       </c>
       <c r="AC431" s="22">
-        <v>8.2</v>
+        <v>57990</v>
       </c>
       <c r="AD431" s="22">
-        <v>8.2</v>
+        <v>57990</v>
       </c>
       <c r="AE431" s="23">
-        <v>24600</v>
+        <v>115980</v>
       </c>
       <c r="AF431" s="23">
-        <v>24600</v>
+        <v>115980</v>
       </c>
     </row>
     <row r="432" s="1" customFormat="1" ht="18.1322" customHeight="1">
@@ -42418,19 +42468,19 @@
         <v>33</v>
       </c>
       <c r="C432" s="4">
-        <v>43944</v>
-      </c>
-      <c r="D432" s="25" t="s">
+        <v>44125</v>
+      </c>
+      <c r="D432" s="5" t="s">
         <v>1088</v>
       </c>
       <c r="E432" s="5" t="s">
         <v>33</v>
       </c>
       <c r="F432" s="6">
-        <v>2320</v>
+        <v>2310</v>
       </c>
       <c r="G432" s="3" t="s">
-        <v>1089</v>
+        <v>1019</v>
       </c>
       <c r="H432" s="3" t="s">
         <v>36</v>
@@ -42439,20 +42489,34 @@
         <v>37</v>
       </c>
       <c r="J432" s="7">
-        <v>0</v>
-      </c>
-      <c r="K432" s="5"/>
-      <c r="L432" s="7"/>
-      <c r="M432" s="5"/>
-      <c r="N432" s="8"/>
-      <c r="O432" s="8"/>
-      <c r="P432" s="9"/>
-      <c r="Q432" s="8"/>
+        <v>9.263561e6</v>
+      </c>
+      <c r="K432" s="5" t="s">
+        <v>1093</v>
+      </c>
+      <c r="L432" s="7">
+        <v>2310</v>
+      </c>
+      <c r="M432" s="5" t="s">
+        <v>1019</v>
+      </c>
+      <c r="N432" s="8">
+        <v>44162</v>
+      </c>
+      <c r="O432" s="8">
+        <v>44161</v>
+      </c>
+      <c r="P432" s="9">
+        <v>44891</v>
+      </c>
+      <c r="Q432" s="8">
+        <v>44341</v>
+      </c>
       <c r="R432" s="5" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="S432" s="5" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="T432" s="3" t="s">
         <v>33</v>
@@ -42461,37 +42525,37 @@
         <v>33</v>
       </c>
       <c r="V432" s="7">
-        <v>1.143883e6</v>
-      </c>
-      <c r="W432" s="5" t="s">
-        <v>1095</v>
+        <v>1.398113e6</v>
+      </c>
+      <c r="W432" s="24" t="s">
+        <v>1096</v>
       </c>
       <c r="X432" s="7">
-        <v>2321</v>
+        <v>2311</v>
       </c>
       <c r="Y432" s="5" t="s">
-        <v>1092</v>
+        <v>1019</v>
       </c>
       <c r="Z432" s="5" t="s">
-        <v>604</v>
+        <v>1097</v>
       </c>
       <c r="AA432" s="3" t="s">
-        <v>581</v>
+        <v>1022</v>
       </c>
       <c r="AB432" s="10">
-        <v>200000</v>
+        <v>2</v>
       </c>
       <c r="AC432" s="11">
-        <v>600000e-6</v>
+        <v>37809.01</v>
       </c>
       <c r="AD432" s="11">
-        <v>600000e-6</v>
+        <v>37809.01</v>
       </c>
       <c r="AE432" s="12">
-        <v>120000</v>
+        <v>75618.02</v>
       </c>
       <c r="AF432" s="12">
-        <v>120000</v>
+        <v>75618.02</v>
       </c>
     </row>
     <row r="433" s="1" customFormat="1" ht="18.1322" customHeight="1">
@@ -42502,19 +42566,19 @@
         <v>33</v>
       </c>
       <c r="C433" s="14">
-        <v>43944</v>
-      </c>
-      <c r="D433" s="26" t="s">
+        <v>44125</v>
+      </c>
+      <c r="D433" s="15" t="s">
         <v>1088</v>
       </c>
       <c r="E433" s="15" t="s">
         <v>33</v>
       </c>
       <c r="F433" s="16">
-        <v>2320</v>
+        <v>2310</v>
       </c>
       <c r="G433" s="13" t="s">
-        <v>1089</v>
+        <v>1019</v>
       </c>
       <c r="H433" s="13" t="s">
         <v>36</v>
@@ -42523,20 +42587,34 @@
         <v>37</v>
       </c>
       <c r="J433" s="17">
-        <v>0</v>
-      </c>
-      <c r="K433" s="15"/>
-      <c r="L433" s="17"/>
-      <c r="M433" s="15"/>
-      <c r="N433" s="18"/>
-      <c r="O433" s="18"/>
-      <c r="P433" s="19"/>
-      <c r="Q433" s="18"/>
+        <v>9.263561e6</v>
+      </c>
+      <c r="K433" s="15" t="s">
+        <v>1093</v>
+      </c>
+      <c r="L433" s="17">
+        <v>2310</v>
+      </c>
+      <c r="M433" s="15" t="s">
+        <v>1019</v>
+      </c>
+      <c r="N433" s="18">
+        <v>44162</v>
+      </c>
+      <c r="O433" s="18">
+        <v>44161</v>
+      </c>
+      <c r="P433" s="19">
+        <v>44891</v>
+      </c>
+      <c r="Q433" s="18">
+        <v>44341</v>
+      </c>
       <c r="R433" s="15" t="s">
-        <v>950</v>
+        <v>1094</v>
       </c>
       <c r="S433" s="15" t="s">
-        <v>951</v>
+        <v>1095</v>
       </c>
       <c r="T433" s="13" t="s">
         <v>33</v>
@@ -42545,42 +42623,42 @@
         <v>33</v>
       </c>
       <c r="V433" s="17">
-        <v>1.244515e6</v>
+        <v>1.398709e6</v>
       </c>
       <c r="W433" s="15" t="s">
-        <v>1096</v>
+        <v>1098</v>
       </c>
       <c r="X433" s="17">
-        <v>2321</v>
+        <v>2311</v>
       </c>
       <c r="Y433" s="15" t="s">
-        <v>1092</v>
+        <v>1019</v>
       </c>
       <c r="Z433" s="15" t="s">
-        <v>604</v>
+        <v>1097</v>
       </c>
       <c r="AA433" s="13" t="s">
-        <v>581</v>
+        <v>1022</v>
       </c>
       <c r="AB433" s="21">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="AC433" s="22">
-        <v>20.1</v>
+        <v>5071.2</v>
       </c>
       <c r="AD433" s="22">
-        <v>20.1</v>
+        <v>5071.2</v>
       </c>
       <c r="AE433" s="23">
-        <v>1005</v>
+        <v>10142.4</v>
       </c>
       <c r="AF433" s="23">
-        <v>1005</v>
+        <v>10142.4</v>
       </c>
     </row>
     <row r="434" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A434" s="3" t="s">
-        <v>1087</v>
+        <v>1099</v>
       </c>
       <c r="B434" s="3" t="s">
         <v>33</v>
@@ -42589,7 +42667,7 @@
         <v>43944</v>
       </c>
       <c r="D434" s="25" t="s">
-        <v>1088</v>
+        <v>1100</v>
       </c>
       <c r="E434" s="5" t="s">
         <v>33</v>
@@ -42598,7 +42676,7 @@
         <v>2320</v>
       </c>
       <c r="G434" s="3" t="s">
-        <v>1089</v>
+        <v>1101</v>
       </c>
       <c r="H434" s="3" t="s">
         <v>36</v>
@@ -42617,10 +42695,10 @@
       <c r="P434" s="9"/>
       <c r="Q434" s="8"/>
       <c r="R434" s="5" t="s">
-        <v>1097</v>
+        <v>1102</v>
       </c>
       <c r="S434" s="5" t="s">
-        <v>1098</v>
+        <v>1103</v>
       </c>
       <c r="T434" s="3" t="s">
         <v>33</v>
@@ -42629,42 +42707,42 @@
         <v>33</v>
       </c>
       <c r="V434" s="7">
-        <v>1.244108e6</v>
+        <v>1.692143e6</v>
       </c>
       <c r="W434" s="5" t="s">
-        <v>1099</v>
+        <v>583</v>
       </c>
       <c r="X434" s="7">
         <v>2321</v>
       </c>
       <c r="Y434" s="5" t="s">
-        <v>1092</v>
+        <v>1104</v>
       </c>
       <c r="Z434" s="5" t="s">
-        <v>604</v>
+        <v>347</v>
       </c>
       <c r="AA434" s="3" t="s">
         <v>581</v>
       </c>
       <c r="AB434" s="10">
-        <v>90</v>
+        <v>3000</v>
       </c>
       <c r="AC434" s="11">
-        <v>358.24</v>
+        <v>8.2</v>
       </c>
       <c r="AD434" s="11">
-        <v>358.24</v>
+        <v>8.2</v>
       </c>
       <c r="AE434" s="12">
-        <v>32241.6</v>
+        <v>24600</v>
       </c>
       <c r="AF434" s="12">
-        <v>32241.6</v>
+        <v>24600</v>
       </c>
     </row>
     <row r="435" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A435" s="13" t="s">
-        <v>1087</v>
+        <v>1099</v>
       </c>
       <c r="B435" s="13" t="s">
         <v>33</v>
@@ -42673,7 +42751,7 @@
         <v>43944</v>
       </c>
       <c r="D435" s="26" t="s">
-        <v>1088</v>
+        <v>1100</v>
       </c>
       <c r="E435" s="15" t="s">
         <v>33</v>
@@ -42682,7 +42760,7 @@
         <v>2320</v>
       </c>
       <c r="G435" s="13" t="s">
-        <v>1089</v>
+        <v>1101</v>
       </c>
       <c r="H435" s="13" t="s">
         <v>36</v>
@@ -42701,10 +42779,10 @@
       <c r="P435" s="19"/>
       <c r="Q435" s="18"/>
       <c r="R435" s="15" t="s">
-        <v>1097</v>
+        <v>1105</v>
       </c>
       <c r="S435" s="15" t="s">
-        <v>1098</v>
+        <v>1106</v>
       </c>
       <c r="T435" s="13" t="s">
         <v>33</v>
@@ -42713,16 +42791,16 @@
         <v>33</v>
       </c>
       <c r="V435" s="17">
-        <v>1.244507e6</v>
+        <v>1.143883e6</v>
       </c>
       <c r="W435" s="15" t="s">
-        <v>1100</v>
+        <v>1107</v>
       </c>
       <c r="X435" s="17">
         <v>2321</v>
       </c>
       <c r="Y435" s="15" t="s">
-        <v>1092</v>
+        <v>1104</v>
       </c>
       <c r="Z435" s="15" t="s">
         <v>604</v>
@@ -42731,24 +42809,24 @@
         <v>581</v>
       </c>
       <c r="AB435" s="21">
-        <v>50</v>
+        <v>200000</v>
       </c>
       <c r="AC435" s="22">
-        <v>34.9</v>
+        <v>600000e-6</v>
       </c>
       <c r="AD435" s="22">
-        <v>34.9</v>
+        <v>600000e-6</v>
       </c>
       <c r="AE435" s="23">
-        <v>1745</v>
+        <v>120000</v>
       </c>
       <c r="AF435" s="23">
-        <v>1745</v>
+        <v>120000</v>
       </c>
     </row>
     <row r="436" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A436" s="3" t="s">
-        <v>1087</v>
+        <v>1099</v>
       </c>
       <c r="B436" s="3" t="s">
         <v>33</v>
@@ -42757,7 +42835,7 @@
         <v>43944</v>
       </c>
       <c r="D436" s="25" t="s">
-        <v>1088</v>
+        <v>1100</v>
       </c>
       <c r="E436" s="5" t="s">
         <v>33</v>
@@ -42766,7 +42844,7 @@
         <v>2320</v>
       </c>
       <c r="G436" s="3" t="s">
-        <v>1089</v>
+        <v>1101</v>
       </c>
       <c r="H436" s="3" t="s">
         <v>36</v>
@@ -42785,10 +42863,10 @@
       <c r="P436" s="9"/>
       <c r="Q436" s="8"/>
       <c r="R436" s="5" t="s">
-        <v>1097</v>
+        <v>950</v>
       </c>
       <c r="S436" s="5" t="s">
-        <v>1098</v>
+        <v>951</v>
       </c>
       <c r="T436" s="3" t="s">
         <v>33</v>
@@ -42797,16 +42875,16 @@
         <v>33</v>
       </c>
       <c r="V436" s="7">
-        <v>1.257587e6</v>
+        <v>1.244515e6</v>
       </c>
       <c r="W436" s="5" t="s">
-        <v>1101</v>
+        <v>1108</v>
       </c>
       <c r="X436" s="7">
         <v>2321</v>
       </c>
       <c r="Y436" s="5" t="s">
-        <v>1092</v>
+        <v>1104</v>
       </c>
       <c r="Z436" s="5" t="s">
         <v>604</v>
@@ -42815,24 +42893,24 @@
         <v>581</v>
       </c>
       <c r="AB436" s="10">
-        <v>80000</v>
+        <v>50</v>
       </c>
       <c r="AC436" s="11">
-        <v>390000e-6</v>
+        <v>20.1</v>
       </c>
       <c r="AD436" s="11">
-        <v>390000e-6</v>
+        <v>20.1</v>
       </c>
       <c r="AE436" s="12">
-        <v>31200</v>
+        <v>1005</v>
       </c>
       <c r="AF436" s="12">
-        <v>31200</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="437" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A437" s="13" t="s">
-        <v>1087</v>
+        <v>1099</v>
       </c>
       <c r="B437" s="13" t="s">
         <v>33</v>
@@ -42841,7 +42919,7 @@
         <v>43944</v>
       </c>
       <c r="D437" s="26" t="s">
-        <v>1088</v>
+        <v>1100</v>
       </c>
       <c r="E437" s="15" t="s">
         <v>33</v>
@@ -42850,7 +42928,7 @@
         <v>2320</v>
       </c>
       <c r="G437" s="13" t="s">
-        <v>1089</v>
+        <v>1101</v>
       </c>
       <c r="H437" s="13" t="s">
         <v>36</v>
@@ -42869,10 +42947,10 @@
       <c r="P437" s="19"/>
       <c r="Q437" s="18"/>
       <c r="R437" s="15" t="s">
-        <v>1097</v>
+        <v>1109</v>
       </c>
       <c r="S437" s="15" t="s">
-        <v>1098</v>
+        <v>1110</v>
       </c>
       <c r="T437" s="13" t="s">
         <v>33</v>
@@ -42881,19 +42959,19 @@
         <v>33</v>
       </c>
       <c r="V437" s="17">
-        <v>1.257625e6</v>
+        <v>1.244108e6</v>
       </c>
       <c r="W437" s="15" t="s">
-        <v>1102</v>
+        <v>1111</v>
       </c>
       <c r="X437" s="17">
         <v>2321</v>
       </c>
       <c r="Y437" s="15" t="s">
-        <v>1092</v>
+        <v>1104</v>
       </c>
       <c r="Z437" s="15" t="s">
-        <v>429</v>
+        <v>604</v>
       </c>
       <c r="AA437" s="13" t="s">
         <v>581</v>
@@ -42902,21 +42980,21 @@
         <v>90</v>
       </c>
       <c r="AC437" s="22">
-        <v>351</v>
+        <v>358.24</v>
       </c>
       <c r="AD437" s="22">
-        <v>351</v>
+        <v>358.24</v>
       </c>
       <c r="AE437" s="23">
-        <v>31590</v>
+        <v>32241.6</v>
       </c>
       <c r="AF437" s="23">
-        <v>31590</v>
+        <v>32241.6</v>
       </c>
     </row>
     <row r="438" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A438" s="3" t="s">
-        <v>1087</v>
+        <v>1099</v>
       </c>
       <c r="B438" s="3" t="s">
         <v>33</v>
@@ -42925,7 +43003,7 @@
         <v>43944</v>
       </c>
       <c r="D438" s="25" t="s">
-        <v>1088</v>
+        <v>1100</v>
       </c>
       <c r="E438" s="5" t="s">
         <v>33</v>
@@ -42934,7 +43012,7 @@
         <v>2320</v>
       </c>
       <c r="G438" s="3" t="s">
-        <v>1089</v>
+        <v>1101</v>
       </c>
       <c r="H438" s="3" t="s">
         <v>36</v>
@@ -42953,10 +43031,10 @@
       <c r="P438" s="9"/>
       <c r="Q438" s="8"/>
       <c r="R438" s="5" t="s">
-        <v>1097</v>
+        <v>1109</v>
       </c>
       <c r="S438" s="5" t="s">
-        <v>1098</v>
+        <v>1110</v>
       </c>
       <c r="T438" s="3" t="s">
         <v>33</v>
@@ -42965,16 +43043,16 @@
         <v>33</v>
       </c>
       <c r="V438" s="7">
-        <v>1.258699e6</v>
+        <v>1.244507e6</v>
       </c>
       <c r="W438" s="5" t="s">
-        <v>1103</v>
+        <v>1112</v>
       </c>
       <c r="X438" s="7">
         <v>2321</v>
       </c>
       <c r="Y438" s="5" t="s">
-        <v>1092</v>
+        <v>1104</v>
       </c>
       <c r="Z438" s="5" t="s">
         <v>604</v>
@@ -42983,24 +43061,24 @@
         <v>581</v>
       </c>
       <c r="AB438" s="10">
-        <v>2000</v>
+        <v>50</v>
       </c>
       <c r="AC438" s="11">
-        <v>1.39</v>
+        <v>34.9</v>
       </c>
       <c r="AD438" s="11">
-        <v>1.39</v>
+        <v>34.9</v>
       </c>
       <c r="AE438" s="12">
-        <v>2780</v>
+        <v>1745</v>
       </c>
       <c r="AF438" s="12">
-        <v>2780</v>
+        <v>1745</v>
       </c>
     </row>
     <row r="439" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A439" s="13" t="s">
-        <v>1087</v>
+        <v>1099</v>
       </c>
       <c r="B439" s="13" t="s">
         <v>33</v>
@@ -43009,7 +43087,7 @@
         <v>43944</v>
       </c>
       <c r="D439" s="26" t="s">
-        <v>1088</v>
+        <v>1100</v>
       </c>
       <c r="E439" s="15" t="s">
         <v>33</v>
@@ -43018,7 +43096,7 @@
         <v>2320</v>
       </c>
       <c r="G439" s="13" t="s">
-        <v>1089</v>
+        <v>1101</v>
       </c>
       <c r="H439" s="13" t="s">
         <v>36</v>
@@ -43037,10 +43115,10 @@
       <c r="P439" s="19"/>
       <c r="Q439" s="18"/>
       <c r="R439" s="15" t="s">
-        <v>1097</v>
+        <v>1109</v>
       </c>
       <c r="S439" s="15" t="s">
-        <v>1098</v>
+        <v>1110</v>
       </c>
       <c r="T439" s="13" t="s">
         <v>33</v>
@@ -43049,16 +43127,16 @@
         <v>33</v>
       </c>
       <c r="V439" s="17">
-        <v>1.259784e6</v>
+        <v>1.257587e6</v>
       </c>
       <c r="W439" s="15" t="s">
-        <v>1104</v>
+        <v>1113</v>
       </c>
       <c r="X439" s="17">
         <v>2321</v>
       </c>
       <c r="Y439" s="15" t="s">
-        <v>1092</v>
+        <v>1104</v>
       </c>
       <c r="Z439" s="15" t="s">
         <v>604</v>
@@ -43067,24 +43145,24 @@
         <v>581</v>
       </c>
       <c r="AB439" s="21">
-        <v>3000</v>
+        <v>80000</v>
       </c>
       <c r="AC439" s="22">
-        <v>600000e-6</v>
+        <v>390000e-6</v>
       </c>
       <c r="AD439" s="22">
-        <v>600000e-6</v>
+        <v>390000e-6</v>
       </c>
       <c r="AE439" s="23">
-        <v>1800</v>
+        <v>31200</v>
       </c>
       <c r="AF439" s="23">
-        <v>1800</v>
+        <v>31200</v>
       </c>
     </row>
     <row r="440" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A440" s="3" t="s">
-        <v>1087</v>
+        <v>1099</v>
       </c>
       <c r="B440" s="3" t="s">
         <v>33</v>
@@ -43093,7 +43171,7 @@
         <v>43944</v>
       </c>
       <c r="D440" s="25" t="s">
-        <v>1088</v>
+        <v>1100</v>
       </c>
       <c r="E440" s="5" t="s">
         <v>33</v>
@@ -43102,7 +43180,7 @@
         <v>2320</v>
       </c>
       <c r="G440" s="3" t="s">
-        <v>1089</v>
+        <v>1101</v>
       </c>
       <c r="H440" s="3" t="s">
         <v>36</v>
@@ -43121,10 +43199,10 @@
       <c r="P440" s="9"/>
       <c r="Q440" s="8"/>
       <c r="R440" s="5" t="s">
-        <v>1097</v>
+        <v>1109</v>
       </c>
       <c r="S440" s="5" t="s">
-        <v>1098</v>
+        <v>1110</v>
       </c>
       <c r="T440" s="3" t="s">
         <v>33</v>
@@ -43133,42 +43211,42 @@
         <v>33</v>
       </c>
       <c r="V440" s="7">
-        <v>1.259792e6</v>
+        <v>1.257625e6</v>
       </c>
       <c r="W440" s="5" t="s">
-        <v>1105</v>
+        <v>1114</v>
       </c>
       <c r="X440" s="7">
         <v>2321</v>
       </c>
       <c r="Y440" s="5" t="s">
-        <v>1092</v>
+        <v>1104</v>
       </c>
       <c r="Z440" s="5" t="s">
-        <v>604</v>
+        <v>429</v>
       </c>
       <c r="AA440" s="3" t="s">
         <v>581</v>
       </c>
       <c r="AB440" s="10">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="AC440" s="11">
-        <v>15.35</v>
+        <v>351</v>
       </c>
       <c r="AD440" s="11">
-        <v>15.35</v>
+        <v>351</v>
       </c>
       <c r="AE440" s="12">
-        <v>1228</v>
+        <v>31590</v>
       </c>
       <c r="AF440" s="12">
-        <v>1228</v>
+        <v>31590</v>
       </c>
     </row>
     <row r="441" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A441" s="13" t="s">
-        <v>1087</v>
+        <v>1099</v>
       </c>
       <c r="B441" s="13" t="s">
         <v>33</v>
@@ -43177,7 +43255,7 @@
         <v>43944</v>
       </c>
       <c r="D441" s="26" t="s">
-        <v>1088</v>
+        <v>1100</v>
       </c>
       <c r="E441" s="15" t="s">
         <v>33</v>
@@ -43186,7 +43264,7 @@
         <v>2320</v>
       </c>
       <c r="G441" s="13" t="s">
-        <v>1089</v>
+        <v>1101</v>
       </c>
       <c r="H441" s="13" t="s">
         <v>36</v>
@@ -43205,10 +43283,10 @@
       <c r="P441" s="19"/>
       <c r="Q441" s="18"/>
       <c r="R441" s="15" t="s">
-        <v>1097</v>
+        <v>1109</v>
       </c>
       <c r="S441" s="15" t="s">
-        <v>1098</v>
+        <v>1110</v>
       </c>
       <c r="T441" s="13" t="s">
         <v>33</v>
@@ -43217,16 +43295,16 @@
         <v>33</v>
       </c>
       <c r="V441" s="17">
-        <v>1.260669e6</v>
+        <v>1.258699e6</v>
       </c>
       <c r="W441" s="15" t="s">
-        <v>1106</v>
+        <v>1115</v>
       </c>
       <c r="X441" s="17">
         <v>2321</v>
       </c>
       <c r="Y441" s="15" t="s">
-        <v>1092</v>
+        <v>1104</v>
       </c>
       <c r="Z441" s="15" t="s">
         <v>604</v>
@@ -43235,24 +43313,24 @@
         <v>581</v>
       </c>
       <c r="AB441" s="21">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="AC441" s="22">
-        <v>1.49</v>
+        <v>1.39</v>
       </c>
       <c r="AD441" s="22">
-        <v>1.49</v>
+        <v>1.39</v>
       </c>
       <c r="AE441" s="23">
-        <v>1490</v>
+        <v>2780</v>
       </c>
       <c r="AF441" s="23">
-        <v>1490</v>
+        <v>2780</v>
       </c>
     </row>
     <row r="442" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A442" s="3" t="s">
-        <v>1087</v>
+        <v>1099</v>
       </c>
       <c r="B442" s="3" t="s">
         <v>33</v>
@@ -43261,7 +43339,7 @@
         <v>43944</v>
       </c>
       <c r="D442" s="25" t="s">
-        <v>1088</v>
+        <v>1100</v>
       </c>
       <c r="E442" s="5" t="s">
         <v>33</v>
@@ -43270,7 +43348,7 @@
         <v>2320</v>
       </c>
       <c r="G442" s="3" t="s">
-        <v>1089</v>
+        <v>1101</v>
       </c>
       <c r="H442" s="3" t="s">
         <v>36</v>
@@ -43289,10 +43367,10 @@
       <c r="P442" s="9"/>
       <c r="Q442" s="8"/>
       <c r="R442" s="5" t="s">
-        <v>1097</v>
+        <v>1109</v>
       </c>
       <c r="S442" s="5" t="s">
-        <v>1098</v>
+        <v>1110</v>
       </c>
       <c r="T442" s="3" t="s">
         <v>33</v>
@@ -43301,16 +43379,16 @@
         <v>33</v>
       </c>
       <c r="V442" s="7">
-        <v>1.260677e6</v>
+        <v>1.259784e6</v>
       </c>
       <c r="W442" s="5" t="s">
-        <v>1107</v>
+        <v>1116</v>
       </c>
       <c r="X442" s="7">
         <v>2321</v>
       </c>
       <c r="Y442" s="5" t="s">
-        <v>1092</v>
+        <v>1104</v>
       </c>
       <c r="Z442" s="5" t="s">
         <v>604</v>
@@ -43322,21 +43400,21 @@
         <v>3000</v>
       </c>
       <c r="AC442" s="11">
-        <v>1.59</v>
+        <v>600000e-6</v>
       </c>
       <c r="AD442" s="11">
-        <v>1.59</v>
+        <v>600000e-6</v>
       </c>
       <c r="AE442" s="12">
-        <v>4770</v>
+        <v>1800</v>
       </c>
       <c r="AF442" s="12">
-        <v>4770</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="443" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A443" s="13" t="s">
-        <v>1087</v>
+        <v>1099</v>
       </c>
       <c r="B443" s="13" t="s">
         <v>33</v>
@@ -43345,7 +43423,7 @@
         <v>43944</v>
       </c>
       <c r="D443" s="26" t="s">
-        <v>1088</v>
+        <v>1100</v>
       </c>
       <c r="E443" s="15" t="s">
         <v>33</v>
@@ -43354,7 +43432,7 @@
         <v>2320</v>
       </c>
       <c r="G443" s="13" t="s">
-        <v>1089</v>
+        <v>1101</v>
       </c>
       <c r="H443" s="13" t="s">
         <v>36</v>
@@ -43373,10 +43451,10 @@
       <c r="P443" s="19"/>
       <c r="Q443" s="18"/>
       <c r="R443" s="15" t="s">
-        <v>1097</v>
+        <v>1109</v>
       </c>
       <c r="S443" s="15" t="s">
-        <v>1098</v>
+        <v>1110</v>
       </c>
       <c r="T443" s="13" t="s">
         <v>33</v>
@@ -43385,16 +43463,16 @@
         <v>33</v>
       </c>
       <c r="V443" s="17">
-        <v>1.260731e6</v>
-      </c>
-      <c r="W443" s="20" t="s">
-        <v>1108</v>
+        <v>1.259792e6</v>
+      </c>
+      <c r="W443" s="15" t="s">
+        <v>1117</v>
       </c>
       <c r="X443" s="17">
         <v>2321</v>
       </c>
       <c r="Y443" s="15" t="s">
-        <v>1092</v>
+        <v>1104</v>
       </c>
       <c r="Z443" s="15" t="s">
         <v>604</v>
@@ -43403,24 +43481,24 @@
         <v>581</v>
       </c>
       <c r="AB443" s="21">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="AC443" s="22">
-        <v>271.97</v>
+        <v>15.35</v>
       </c>
       <c r="AD443" s="22">
-        <v>271.97</v>
+        <v>15.35</v>
       </c>
       <c r="AE443" s="23">
-        <v>16318.2</v>
+        <v>1228</v>
       </c>
       <c r="AF443" s="23">
-        <v>16318.2</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="444" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A444" s="3" t="s">
-        <v>1087</v>
+        <v>1099</v>
       </c>
       <c r="B444" s="3" t="s">
         <v>33</v>
@@ -43429,7 +43507,7 @@
         <v>43944</v>
       </c>
       <c r="D444" s="25" t="s">
-        <v>1088</v>
+        <v>1100</v>
       </c>
       <c r="E444" s="5" t="s">
         <v>33</v>
@@ -43438,7 +43516,7 @@
         <v>2320</v>
       </c>
       <c r="G444" s="3" t="s">
-        <v>1089</v>
+        <v>1101</v>
       </c>
       <c r="H444" s="3" t="s">
         <v>36</v>
@@ -43457,10 +43535,10 @@
       <c r="P444" s="9"/>
       <c r="Q444" s="8"/>
       <c r="R444" s="5" t="s">
-        <v>1097</v>
+        <v>1109</v>
       </c>
       <c r="S444" s="5" t="s">
-        <v>1098</v>
+        <v>1110</v>
       </c>
       <c r="T444" s="3" t="s">
         <v>33</v>
@@ -43469,16 +43547,16 @@
         <v>33</v>
       </c>
       <c r="V444" s="7">
-        <v>1.687115e6</v>
+        <v>1.260669e6</v>
       </c>
       <c r="W444" s="5" t="s">
-        <v>1109</v>
+        <v>1118</v>
       </c>
       <c r="X444" s="7">
         <v>2321</v>
       </c>
       <c r="Y444" s="5" t="s">
-        <v>1092</v>
+        <v>1104</v>
       </c>
       <c r="Z444" s="5" t="s">
         <v>604</v>
@@ -43487,24 +43565,24 @@
         <v>581</v>
       </c>
       <c r="AB444" s="10">
-        <v>60</v>
+        <v>1000</v>
       </c>
       <c r="AC444" s="11">
-        <v>16.65</v>
+        <v>1.49</v>
       </c>
       <c r="AD444" s="11">
-        <v>16.65</v>
+        <v>1.49</v>
       </c>
       <c r="AE444" s="12">
-        <v>999</v>
+        <v>1490</v>
       </c>
       <c r="AF444" s="12">
-        <v>999</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="445" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A445" s="13" t="s">
-        <v>1087</v>
+        <v>1099</v>
       </c>
       <c r="B445" s="13" t="s">
         <v>33</v>
@@ -43513,7 +43591,7 @@
         <v>43944</v>
       </c>
       <c r="D445" s="26" t="s">
-        <v>1088</v>
+        <v>1100</v>
       </c>
       <c r="E445" s="15" t="s">
         <v>33</v>
@@ -43522,7 +43600,7 @@
         <v>2320</v>
       </c>
       <c r="G445" s="13" t="s">
-        <v>1089</v>
+        <v>1101</v>
       </c>
       <c r="H445" s="13" t="s">
         <v>36</v>
@@ -43541,11 +43619,11 @@
       <c r="P445" s="19"/>
       <c r="Q445" s="18"/>
       <c r="R445" s="15" t="s">
+        <v>1109</v>
+      </c>
+      <c r="S445" s="15" t="s">
         <v>1110</v>
       </c>
-      <c r="S445" s="15" t="s">
-        <v>1111</v>
-      </c>
       <c r="T445" s="13" t="s">
         <v>33</v>
       </c>
@@ -43553,16 +43631,16 @@
         <v>33</v>
       </c>
       <c r="V445" s="17">
-        <v>1.257463e6</v>
+        <v>1.260677e6</v>
       </c>
       <c r="W445" s="15" t="s">
-        <v>1112</v>
+        <v>1119</v>
       </c>
       <c r="X445" s="17">
         <v>2321</v>
       </c>
       <c r="Y445" s="15" t="s">
-        <v>1092</v>
+        <v>1104</v>
       </c>
       <c r="Z445" s="15" t="s">
         <v>604</v>
@@ -43571,33 +43649,33 @@
         <v>581</v>
       </c>
       <c r="AB445" s="21">
-        <v>200</v>
+        <v>3000</v>
       </c>
       <c r="AC445" s="22">
-        <v>34.2</v>
+        <v>1.59</v>
       </c>
       <c r="AD445" s="22">
-        <v>34.2</v>
+        <v>1.59</v>
       </c>
       <c r="AE445" s="23">
-        <v>6840</v>
+        <v>4770</v>
       </c>
       <c r="AF445" s="23">
-        <v>6840</v>
+        <v>4770</v>
       </c>
     </row>
     <row r="446" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A446" s="3" t="s">
-        <v>1113</v>
+        <v>1099</v>
       </c>
       <c r="B446" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C446" s="4">
-        <v>44012</v>
-      </c>
-      <c r="D446" s="5" t="s">
-        <v>1114</v>
+        <v>43944</v>
+      </c>
+      <c r="D446" s="25" t="s">
+        <v>1100</v>
       </c>
       <c r="E446" s="5" t="s">
         <v>33</v>
@@ -43606,7 +43684,7 @@
         <v>2320</v>
       </c>
       <c r="G446" s="3" t="s">
-        <v>1089</v>
+        <v>1101</v>
       </c>
       <c r="H446" s="3" t="s">
         <v>36</v>
@@ -43625,10 +43703,10 @@
       <c r="P446" s="9"/>
       <c r="Q446" s="8"/>
       <c r="R446" s="5" t="s">
-        <v>564</v>
+        <v>1109</v>
       </c>
       <c r="S446" s="5" t="s">
-        <v>565</v>
+        <v>1110</v>
       </c>
       <c r="T446" s="3" t="s">
         <v>33</v>
@@ -43637,51 +43715,51 @@
         <v>33</v>
       </c>
       <c r="V446" s="7">
-        <v>1.408623e6</v>
-      </c>
-      <c r="W446" s="5" t="s">
-        <v>1115</v>
+        <v>1.260731e6</v>
+      </c>
+      <c r="W446" s="24" t="s">
+        <v>1120</v>
       </c>
       <c r="X446" s="7">
         <v>2321</v>
       </c>
       <c r="Y446" s="5" t="s">
-        <v>1092</v>
+        <v>1104</v>
       </c>
       <c r="Z446" s="5" t="s">
-        <v>436</v>
+        <v>604</v>
       </c>
       <c r="AA446" s="3" t="s">
         <v>581</v>
       </c>
       <c r="AB446" s="10">
-        <v>2000</v>
+        <v>60</v>
       </c>
       <c r="AC446" s="11">
-        <v>18.69</v>
+        <v>271.97</v>
       </c>
       <c r="AD446" s="11">
-        <v>14.95</v>
+        <v>271.97</v>
       </c>
       <c r="AE446" s="12">
-        <v>37380</v>
+        <v>16318.2</v>
       </c>
       <c r="AF446" s="12">
-        <v>29900</v>
+        <v>16318.2</v>
       </c>
     </row>
     <row r="447" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A447" s="13" t="s">
-        <v>1116</v>
+        <v>1099</v>
       </c>
       <c r="B447" s="13" t="s">
         <v>33</v>
       </c>
       <c r="C447" s="14">
-        <v>44034</v>
+        <v>43944</v>
       </c>
       <c r="D447" s="26" t="s">
-        <v>1117</v>
+        <v>1100</v>
       </c>
       <c r="E447" s="15" t="s">
         <v>33</v>
@@ -43690,43 +43768,29 @@
         <v>2320</v>
       </c>
       <c r="G447" s="13" t="s">
-        <v>1089</v>
+        <v>1101</v>
       </c>
       <c r="H447" s="13" t="s">
         <v>36</v>
       </c>
       <c r="I447" s="13" t="s">
-        <v>1118</v>
+        <v>37</v>
       </c>
       <c r="J447" s="17">
-        <v>9.260962e6</v>
-      </c>
-      <c r="K447" s="15" t="s">
-        <v>1119</v>
-      </c>
-      <c r="L447" s="17">
-        <v>2320</v>
-      </c>
-      <c r="M447" s="15" t="s">
-        <v>1089</v>
-      </c>
-      <c r="N447" s="18">
-        <v>44056</v>
-      </c>
-      <c r="O447" s="18">
-        <v>44056</v>
-      </c>
-      <c r="P447" s="19">
-        <v>44240</v>
-      </c>
-      <c r="Q447" s="18">
-        <v>44240</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K447" s="15"/>
+      <c r="L447" s="17"/>
+      <c r="M447" s="15"/>
+      <c r="N447" s="18"/>
+      <c r="O447" s="18"/>
+      <c r="P447" s="19"/>
+      <c r="Q447" s="18"/>
       <c r="R447" s="15" t="s">
-        <v>864</v>
+        <v>1109</v>
       </c>
       <c r="S447" s="15" t="s">
-        <v>865</v>
+        <v>1110</v>
       </c>
       <c r="T447" s="13" t="s">
         <v>33</v>
@@ -43735,40 +43799,306 @@
         <v>33</v>
       </c>
       <c r="V447" s="17">
-        <v>1.758276e6</v>
+        <v>1.687115e6</v>
       </c>
       <c r="W447" s="15" t="s">
-        <v>866</v>
+        <v>1121</v>
       </c>
       <c r="X447" s="17">
         <v>2321</v>
       </c>
       <c r="Y447" s="15" t="s">
-        <v>1092</v>
+        <v>1104</v>
       </c>
       <c r="Z447" s="15" t="s">
+        <v>604</v>
+      </c>
+      <c r="AA447" s="13" t="s">
+        <v>581</v>
+      </c>
+      <c r="AB447" s="21">
+        <v>60</v>
+      </c>
+      <c r="AC447" s="22">
+        <v>16.65</v>
+      </c>
+      <c r="AD447" s="22">
+        <v>16.65</v>
+      </c>
+      <c r="AE447" s="23">
+        <v>999</v>
+      </c>
+      <c r="AF447" s="23">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="448" s="1" customFormat="1" ht="18.1322" customHeight="1">
+      <c r="A448" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B448" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C448" s="4">
+        <v>43944</v>
+      </c>
+      <c r="D448" s="25" t="s">
+        <v>1100</v>
+      </c>
+      <c r="E448" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F448" s="6">
+        <v>2320</v>
+      </c>
+      <c r="G448" s="3" t="s">
+        <v>1101</v>
+      </c>
+      <c r="H448" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I448" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J448" s="7">
+        <v>0</v>
+      </c>
+      <c r="K448" s="5"/>
+      <c r="L448" s="7"/>
+      <c r="M448" s="5"/>
+      <c r="N448" s="8"/>
+      <c r="O448" s="8"/>
+      <c r="P448" s="9"/>
+      <c r="Q448" s="8"/>
+      <c r="R448" s="5" t="s">
+        <v>1122</v>
+      </c>
+      <c r="S448" s="5" t="s">
+        <v>1123</v>
+      </c>
+      <c r="T448" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U448" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="V448" s="7">
+        <v>1.257463e6</v>
+      </c>
+      <c r="W448" s="5" t="s">
+        <v>1124</v>
+      </c>
+      <c r="X448" s="7">
+        <v>2321</v>
+      </c>
+      <c r="Y448" s="5" t="s">
+        <v>1104</v>
+      </c>
+      <c r="Z448" s="5" t="s">
+        <v>604</v>
+      </c>
+      <c r="AA448" s="3" t="s">
+        <v>581</v>
+      </c>
+      <c r="AB448" s="10">
+        <v>200</v>
+      </c>
+      <c r="AC448" s="11">
+        <v>34.2</v>
+      </c>
+      <c r="AD448" s="11">
+        <v>34.2</v>
+      </c>
+      <c r="AE448" s="12">
+        <v>6840</v>
+      </c>
+      <c r="AF448" s="12">
+        <v>6840</v>
+      </c>
+    </row>
+    <row r="449" s="1" customFormat="1" ht="18.1322" customHeight="1">
+      <c r="A449" s="13" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B449" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C449" s="14">
+        <v>44012</v>
+      </c>
+      <c r="D449" s="15" t="s">
+        <v>1126</v>
+      </c>
+      <c r="E449" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F449" s="16">
+        <v>2320</v>
+      </c>
+      <c r="G449" s="13" t="s">
+        <v>1101</v>
+      </c>
+      <c r="H449" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I449" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="J449" s="17">
+        <v>0</v>
+      </c>
+      <c r="K449" s="15"/>
+      <c r="L449" s="17"/>
+      <c r="M449" s="15"/>
+      <c r="N449" s="18"/>
+      <c r="O449" s="18"/>
+      <c r="P449" s="19"/>
+      <c r="Q449" s="18"/>
+      <c r="R449" s="15" t="s">
+        <v>564</v>
+      </c>
+      <c r="S449" s="15" t="s">
+        <v>565</v>
+      </c>
+      <c r="T449" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="U449" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="V449" s="17">
+        <v>1.408623e6</v>
+      </c>
+      <c r="W449" s="15" t="s">
+        <v>1127</v>
+      </c>
+      <c r="X449" s="17">
+        <v>2321</v>
+      </c>
+      <c r="Y449" s="15" t="s">
+        <v>1104</v>
+      </c>
+      <c r="Z449" s="15" t="s">
+        <v>436</v>
+      </c>
+      <c r="AA449" s="13" t="s">
+        <v>581</v>
+      </c>
+      <c r="AB449" s="21">
+        <v>2000</v>
+      </c>
+      <c r="AC449" s="22">
+        <v>18.69</v>
+      </c>
+      <c r="AD449" s="22">
+        <v>14.95</v>
+      </c>
+      <c r="AE449" s="23">
+        <v>37380</v>
+      </c>
+      <c r="AF449" s="23">
+        <v>29900</v>
+      </c>
+    </row>
+    <row r="450" s="1" customFormat="1" ht="18.1322" customHeight="1">
+      <c r="A450" s="3" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B450" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C450" s="4">
+        <v>44034</v>
+      </c>
+      <c r="D450" s="25" t="s">
+        <v>1129</v>
+      </c>
+      <c r="E450" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F450" s="6">
+        <v>2320</v>
+      </c>
+      <c r="G450" s="3" t="s">
+        <v>1101</v>
+      </c>
+      <c r="H450" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I450" s="3" t="s">
+        <v>1130</v>
+      </c>
+      <c r="J450" s="7">
+        <v>9.260962e6</v>
+      </c>
+      <c r="K450" s="5" t="s">
+        <v>1131</v>
+      </c>
+      <c r="L450" s="7">
+        <v>2320</v>
+      </c>
+      <c r="M450" s="5" t="s">
+        <v>1101</v>
+      </c>
+      <c r="N450" s="8">
+        <v>44056</v>
+      </c>
+      <c r="O450" s="8">
+        <v>44056</v>
+      </c>
+      <c r="P450" s="9">
+        <v>44240</v>
+      </c>
+      <c r="Q450" s="8">
+        <v>44240</v>
+      </c>
+      <c r="R450" s="5" t="s">
+        <v>864</v>
+      </c>
+      <c r="S450" s="5" t="s">
+        <v>865</v>
+      </c>
+      <c r="T450" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U450" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="V450" s="7">
+        <v>1.758276e6</v>
+      </c>
+      <c r="W450" s="5" t="s">
+        <v>866</v>
+      </c>
+      <c r="X450" s="7">
+        <v>2321</v>
+      </c>
+      <c r="Y450" s="5" t="s">
+        <v>1104</v>
+      </c>
+      <c r="Z450" s="5" t="s">
         <v>429</v>
       </c>
-      <c r="AA447" s="13" t="s">
+      <c r="AA450" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="AB447" s="21">
+      <c r="AB450" s="10">
         <v>7000</v>
       </c>
-      <c r="AC447" s="22">
+      <c r="AC450" s="11">
         <v>34.54</v>
       </c>
-      <c r="AD447" s="22">
+      <c r="AD450" s="11">
         <v>34.536</v>
       </c>
-      <c r="AE447" s="23">
+      <c r="AE450" s="12">
         <v>241780</v>
       </c>
-      <c r="AF447" s="23">
+      <c r="AF450" s="12">
         <v>241752</v>
       </c>
     </row>
-    <row r="448" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
+    <row r="451" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
   </sheetData>
   <pageSetup paperSize="9" scale="100" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>